<commit_message>
acwi hmm play and sddp merton play
</commit_message>
<xml_diff>
--- a/julia_msp/goal_data.xlsx
+++ b/julia_msp/goal_data.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matsz\programowanie\Optymalizacja portfela\julia_msp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{02B784AB-71A0-404B-9F25-1D48814DFBA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D125E526-1F36-4648-8480-172C1D1A898A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{E8CF1CA2-D953-46E5-99F4-DA96611E7E6D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E8CF1CA2-D953-46E5-99F4-DA96611E7E6D}"/>
   </bookViews>
   <sheets>
     <sheet name="goal_data" sheetId="1" r:id="rId1"/>
-    <sheet name="utilities" sheetId="2" r:id="rId2"/>
+    <sheet name="goal_data (2)" sheetId="3" r:id="rId2"/>
+    <sheet name="utilities" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="27">
   <si>
     <t>minimum_limit</t>
   </si>
@@ -116,6 +117,9 @@
   <si>
     <t>priority</t>
   </si>
+  <si>
+    <t>goal34</t>
+  </si>
 </sst>
 </file>
 
@@ -123,11 +127,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="6">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="168" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="169" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="171" formatCode="_-* #,##0.00\ _z_ł_-;\-* #,##0.00\ _z_ł_-;_-* &quot;-&quot;??\ _z_ł_-;_-@_-"/>
-    <numFmt numFmtId="174" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="175" formatCode="_-* #,##0.0000\ _z_ł_-;\-* #,##0.0000\ _z_ł_-;_-* &quot;-&quot;????\ _z_ł_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0.00\ _z_ł_-;\-* #,##0.00\ _z_ł_-;_-* &quot;-&quot;??\ _z_ł_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="168" formatCode="_-* #,##0.0000\ _z_ł_-;\-* #,##0.0000\ _z_ł_-;_-* &quot;-&quot;????\ _z_ł_-;_-@_-"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -183,7 +187,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -191,14 +195,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -536,19 +539,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FFE0B56-DF8B-44CF-9758-6EDE70A13051}">
-  <dimension ref="A1:I41"/>
+  <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22:E41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="16.77734375" customWidth="1"/>
-    <col min="9" max="9" width="8.88671875" style="10"/>
+    <col min="6" max="6" width="16.7109375" customWidth="1"/>
+    <col min="9" max="9" width="8.85546875" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -573,1446 +576,1482 @@
       <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I1" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
         <f>utilities!$B$8</f>
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C2">
         <f>utilities!$C$8</f>
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="D2">
         <f>utilities!$D$8</f>
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2" s="4">
         <f>utilities!$B$11</f>
-        <v>0.15625</v>
+        <v>0.69444444444444453</v>
       </c>
       <c r="G2" s="4">
         <f>utilities!$C$11</f>
-        <v>0.1</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="H2" s="4">
         <f>utilities!$D$11</f>
-        <v>0.05</v>
-      </c>
-      <c r="I2" s="10">
-        <f>utilities!$E$11</f>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="I2" s="9">
+        <f>utilities!$E$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
         <f>utilities!$B$8</f>
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C3">
         <f>utilities!$C$8</f>
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="D3">
         <f>utilities!$D$8</f>
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="E3">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="F3" s="4">
         <f>utilities!$B$11</f>
-        <v>0.15625</v>
+        <v>0.69444444444444453</v>
       </c>
       <c r="G3" s="4">
         <f>utilities!$C$11</f>
-        <v>0.1</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="H3" s="4">
         <f>utilities!$D$11</f>
-        <v>0.05</v>
-      </c>
-      <c r="I3" s="10">
-        <f>utilities!$E$11</f>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="I3" s="9">
+        <f>utilities!$E$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
         <f>utilities!$B$8</f>
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C4">
         <f>utilities!$C$8</f>
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="D4">
         <f>utilities!$D$8</f>
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="E4">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="F4" s="4">
         <f>utilities!$B$11</f>
-        <v>0.15625</v>
+        <v>0.69444444444444453</v>
       </c>
       <c r="G4" s="4">
         <f>utilities!$C$11</f>
-        <v>0.1</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="H4" s="4">
         <f>utilities!$D$11</f>
-        <v>0.05</v>
-      </c>
-      <c r="I4" s="10">
-        <f>utilities!$E$11</f>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="I4" s="9">
+        <f>utilities!$E$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
         <f>utilities!$B$8</f>
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C5">
         <f>utilities!$C$8</f>
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="D5">
         <f>utilities!$D$8</f>
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="E5">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="F5" s="4">
         <f>utilities!$B$11</f>
-        <v>0.15625</v>
+        <v>0.69444444444444453</v>
       </c>
       <c r="G5" s="4">
         <f>utilities!$C$11</f>
-        <v>0.1</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="H5" s="4">
         <f>utilities!$D$11</f>
-        <v>0.05</v>
-      </c>
-      <c r="I5" s="10">
-        <f>utilities!$E$11</f>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="I5" s="9">
+        <f>utilities!$E$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
         <f>utilities!$B$8</f>
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C6">
         <f>utilities!$C$8</f>
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="D6">
         <f>utilities!$D$8</f>
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="E6">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="F6" s="4">
         <f>utilities!$B$11</f>
-        <v>0.15625</v>
+        <v>0.69444444444444453</v>
       </c>
       <c r="G6" s="4">
         <f>utilities!$C$11</f>
-        <v>0.1</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="H6" s="4">
         <f>utilities!$D$11</f>
-        <v>0.05</v>
-      </c>
-      <c r="I6" s="10">
-        <f>utilities!$E$11</f>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="I6" s="9">
+        <f>utilities!$E$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7">
         <f>utilities!$B$8</f>
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C7">
         <f>utilities!$C$8</f>
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="D7">
         <f>utilities!$D$8</f>
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="E7">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="F7" s="4">
         <f>utilities!$B$11</f>
-        <v>0.15625</v>
+        <v>0.69444444444444453</v>
       </c>
       <c r="G7" s="4">
         <f>utilities!$C$11</f>
-        <v>0.1</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="H7" s="4">
         <f>utilities!$D$11</f>
-        <v>0.05</v>
-      </c>
-      <c r="I7" s="10">
-        <f>utilities!$E$11</f>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="I7" s="9">
+        <f>utilities!$E$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8">
-        <f>utilities!$B$8</f>
-        <v>16</v>
+        <f>utilities!$N$8</f>
+        <v>56</v>
       </c>
       <c r="C8">
-        <f>utilities!$C$8</f>
-        <v>21</v>
+        <f>utilities!$O$8</f>
+        <v>98</v>
       </c>
       <c r="D8">
-        <f>utilities!$D$8</f>
-        <v>23</v>
+        <f>utilities!$P$8</f>
+        <v>109</v>
       </c>
       <c r="E8">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="F8" s="4">
-        <f>utilities!$B$11</f>
-        <v>0.15625</v>
+        <f>utilities!N11</f>
+        <v>0.46875</v>
       </c>
       <c r="G8" s="4">
-        <f>utilities!$C$11</f>
-        <v>0.1</v>
+        <f>utilities!O11</f>
+        <v>0.125</v>
       </c>
       <c r="H8" s="4">
-        <f>utilities!$D$11</f>
-        <v>0.05</v>
-      </c>
-      <c r="I8" s="10">
-        <f>utilities!$E$11</f>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+        <f>utilities!P11</f>
+        <v>9.5454545454545459E-2</v>
+      </c>
+      <c r="I8" s="9">
+        <f>utilities!$E$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9">
         <f>utilities!$B$8</f>
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C9">
         <f>utilities!$C$8</f>
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="D9">
         <f>utilities!$D$8</f>
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="E9">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="F9" s="4">
         <f>utilities!$B$11</f>
-        <v>0.15625</v>
+        <v>0.69444444444444453</v>
       </c>
       <c r="G9" s="4">
         <f>utilities!$C$11</f>
-        <v>0.1</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="H9" s="4">
         <f>utilities!$D$11</f>
-        <v>0.05</v>
-      </c>
-      <c r="I9" s="10">
-        <f>utilities!$E$11</f>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="I9" s="9">
+        <f>utilities!$E$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10">
         <f>utilities!$B$8</f>
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C10">
         <f>utilities!$C$8</f>
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="D10">
         <f>utilities!$D$8</f>
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="E10">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="F10" s="4">
         <f>utilities!$B$11</f>
-        <v>0.15625</v>
+        <v>0.69444444444444453</v>
       </c>
       <c r="G10" s="4">
         <f>utilities!$C$11</f>
-        <v>0.1</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="H10" s="4">
         <f>utilities!$D$11</f>
-        <v>0.05</v>
-      </c>
-      <c r="I10" s="10">
-        <f>utilities!$E$11</f>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="I10" s="9">
+        <f>utilities!$E$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11">
         <f>utilities!$B$8</f>
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C11">
         <f>utilities!$C$8</f>
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="D11">
         <f>utilities!$D$8</f>
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="E11">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="F11" s="4">
         <f>utilities!$B$11</f>
-        <v>0.15625</v>
+        <v>0.69444444444444453</v>
       </c>
       <c r="G11" s="4">
         <f>utilities!$C$11</f>
-        <v>0.1</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="H11" s="4">
         <f>utilities!$D$11</f>
-        <v>0.05</v>
-      </c>
-      <c r="I11" s="10">
-        <f>utilities!$E$11</f>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="I11" s="9">
+        <f>utilities!$E$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12">
-        <f>utilities!N$8</f>
-        <v>66</v>
+        <f>utilities!$B$8</f>
+        <v>6</v>
       </c>
       <c r="C12">
-        <f>utilities!O$8</f>
-        <v>121</v>
+        <f>utilities!$C$8</f>
+        <v>8</v>
       </c>
       <c r="D12">
-        <f>utilities!P$8</f>
-        <v>148</v>
+        <f>utilities!$D$8</f>
+        <v>9</v>
       </c>
       <c r="E12">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="F12" s="4">
-        <f>utilities!N$11</f>
-        <v>0.39772727272727271</v>
+        <f>utilities!$B$11</f>
+        <v>0.69444444444444453</v>
       </c>
       <c r="G12" s="4">
-        <f>utilities!O$11</f>
-        <v>9.5454545454545459E-2</v>
+        <f>utilities!$C$11</f>
+        <v>0.41666666666666669</v>
       </c>
       <c r="H12" s="4">
-        <f>utilities!P$11</f>
-        <v>3.888888888888889E-2</v>
-      </c>
-      <c r="I12" s="10">
-        <f>utilities!Q$11</f>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+        <f>utilities!$D$11</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="I12" s="9">
+        <f>utilities!$E$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13">
         <f>utilities!$B$8</f>
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C13">
         <f>utilities!$C$8</f>
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="D13">
         <f>utilities!$D$8</f>
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="E13">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="F13" s="4">
         <f>utilities!$B$11</f>
-        <v>0.15625</v>
+        <v>0.69444444444444453</v>
       </c>
       <c r="G13" s="4">
         <f>utilities!$C$11</f>
-        <v>0.1</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="H13" s="4">
         <f>utilities!$D$11</f>
-        <v>0.05</v>
-      </c>
-      <c r="I13" s="10">
-        <f>utilities!$E$11</f>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="I13" s="9">
+        <f>utilities!$E$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14">
-        <f>utilities!$B$8</f>
-        <v>16</v>
+        <f>utilities!T8</f>
+        <v>81</v>
       </c>
       <c r="C14">
-        <f>utilities!$C$8</f>
-        <v>21</v>
+        <f>utilities!U8</f>
+        <v>143</v>
       </c>
       <c r="D14">
-        <f>utilities!$D$8</f>
-        <v>23</v>
+        <f>utilities!V8</f>
+        <v>159</v>
       </c>
       <c r="E14">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="F14" s="4">
-        <f>utilities!$B$11</f>
-        <v>0.15625</v>
+        <f>utilities!T11</f>
+        <v>0.32407407407407407</v>
       </c>
       <c r="G14" s="4">
-        <f>utilities!$C$11</f>
-        <v>0.1</v>
+        <f>utilities!U11</f>
+        <v>8.4677419354838704E-2</v>
       </c>
       <c r="H14" s="4">
-        <f>utilities!$D$11</f>
-        <v>0.05</v>
-      </c>
-      <c r="I14" s="10">
-        <f>utilities!$E$11</f>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+        <f>utilities!V11</f>
+        <v>6.5625000000000003E-2</v>
+      </c>
+      <c r="I14" s="9">
+        <f>utilities!$E$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <f>utilities!$B$8</f>
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C15">
         <f>utilities!$C$8</f>
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="D15">
         <f>utilities!$D$8</f>
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="E15">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="F15" s="4">
         <f>utilities!$B$11</f>
-        <v>0.15625</v>
+        <v>0.69444444444444453</v>
       </c>
       <c r="G15" s="4">
         <f>utilities!$C$11</f>
-        <v>0.1</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="H15" s="4">
         <f>utilities!$D$11</f>
-        <v>0.05</v>
-      </c>
-      <c r="I15" s="10">
-        <f>utilities!$E$11</f>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="I15" s="9">
+        <f>utilities!$E$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
         <f>utilities!$B$8</f>
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C16">
         <f>utilities!$C$8</f>
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="D16">
         <f>utilities!$D$8</f>
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="E16">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="F16" s="4">
         <f>utilities!$B$11</f>
-        <v>0.15625</v>
+        <v>0.69444444444444453</v>
       </c>
       <c r="G16" s="4">
         <f>utilities!$C$11</f>
-        <v>0.1</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="H16" s="4">
         <f>utilities!$D$11</f>
-        <v>0.05</v>
-      </c>
-      <c r="I16" s="10">
-        <f>utilities!$E$11</f>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="I16" s="9">
+        <f>utilities!$E$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <f>utilities!$B$8</f>
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C17">
         <f>utilities!$C$8</f>
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="D17">
         <f>utilities!$D$8</f>
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="E17">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="F17" s="4">
         <f>utilities!$B$11</f>
-        <v>0.15625</v>
+        <v>0.69444444444444453</v>
       </c>
       <c r="G17" s="4">
         <f>utilities!$C$11</f>
-        <v>0.1</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="H17" s="4">
         <f>utilities!$D$11</f>
-        <v>0.05</v>
-      </c>
-      <c r="I17" s="10">
-        <f>utilities!$E$11</f>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="I17" s="9">
+        <f>utilities!$E$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <f>utilities!$B$8</f>
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C18">
         <f>utilities!$C$8</f>
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="D18">
         <f>utilities!$D$8</f>
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="E18">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="F18" s="4">
         <f>utilities!$B$11</f>
-        <v>0.15625</v>
+        <v>0.69444444444444453</v>
       </c>
       <c r="G18" s="4">
         <f>utilities!$C$11</f>
-        <v>0.1</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="H18" s="4">
         <f>utilities!$D$11</f>
-        <v>0.05</v>
-      </c>
-      <c r="I18" s="10">
-        <f>utilities!$E$11</f>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="I18" s="9">
+        <f>utilities!$E$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
         <f>utilities!$B$8</f>
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C19">
         <f>utilities!$C$8</f>
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="D19">
         <f>utilities!$D$8</f>
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="E19">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="F19" s="4">
         <f>utilities!$B$11</f>
-        <v>0.15625</v>
+        <v>0.69444444444444453</v>
       </c>
       <c r="G19" s="4">
         <f>utilities!$C$11</f>
-        <v>0.1</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="H19" s="4">
         <f>utilities!$D$11</f>
-        <v>0.05</v>
-      </c>
-      <c r="I19" s="10">
-        <f>utilities!$E$11</f>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="I19" s="9">
+        <f>utilities!$E$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <f>utilities!$B$8</f>
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C20">
         <f>utilities!$C$8</f>
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="D20">
         <f>utilities!$D$8</f>
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="E20">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="F20" s="4">
         <f>utilities!$B$11</f>
-        <v>0.15625</v>
+        <v>0.69444444444444453</v>
       </c>
       <c r="G20" s="4">
         <f>utilities!$C$11</f>
-        <v>0.1</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="H20" s="4">
         <f>utilities!$D$11</f>
-        <v>0.05</v>
-      </c>
-      <c r="I20" s="10">
-        <f>utilities!$E$11</f>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="I20" s="9">
+        <f>utilities!$E$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21">
         <f>utilities!$B$8</f>
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C21">
         <f>utilities!$C$8</f>
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="D21">
         <f>utilities!$D$8</f>
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="E21">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="F21" s="4">
         <f>utilities!$B$11</f>
-        <v>0.15625</v>
+        <v>0.69444444444444453</v>
       </c>
       <c r="G21" s="4">
         <f>utilities!$C$11</f>
-        <v>0.1</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="H21" s="4">
         <f>utilities!$D$11</f>
-        <v>0.05</v>
-      </c>
-      <c r="I21" s="10">
-        <f>utilities!$E$11</f>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="I21" s="9">
+        <f>utilities!$E$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22">
+        <f>utilities!$B$8</f>
+        <v>6</v>
+      </c>
+      <c r="C22">
+        <f>utilities!$C$8</f>
+        <v>8</v>
+      </c>
+      <c r="D22">
+        <f>utilities!$D$8</f>
+        <v>9</v>
+      </c>
+      <c r="E22">
+        <v>10</v>
+      </c>
+      <c r="F22" s="4">
+        <f>utilities!$B$11</f>
+        <v>0.69444444444444453</v>
+      </c>
+      <c r="G22" s="4">
+        <f>utilities!$C$11</f>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="H22" s="4">
+        <f>utilities!$D$11</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="I22" s="9">
+        <f>utilities!$E$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23">
         <v>21</v>
-      </c>
-      <c r="B22">
-        <f>utilities!$H$8</f>
-        <v>13</v>
-      </c>
-      <c r="C22">
-        <f>utilities!$I$8</f>
-        <v>16</v>
-      </c>
-      <c r="D22">
-        <f>utilities!$J$8</f>
-        <v>18</v>
-      </c>
-      <c r="E22">
-        <v>0</v>
-      </c>
-      <c r="F22" s="4">
-        <f>utilities!$H$11</f>
-        <v>9.6153846153846159E-2</v>
-      </c>
-      <c r="G22" s="4">
-        <f>utilities!$I$11</f>
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="H22" s="4">
-        <f>utilities!$J$11</f>
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="I22" s="10">
-        <f>utilities!$K$11</f>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23">
-        <v>22</v>
       </c>
       <c r="B23">
         <f>utilities!$H$8</f>
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="C23">
         <f>utilities!$I$8</f>
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="D23">
         <f>utilities!$J$8</f>
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="E23">
         <v>0</v>
       </c>
-      <c r="F23" s="4">
+      <c r="F23" s="4" t="e">
         <f>utilities!$H$11</f>
-        <v>9.6153846153846159E-2</v>
-      </c>
-      <c r="G23" s="4">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G23" s="4" t="e">
         <f>utilities!$I$11</f>
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="H23" s="4">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H23" s="4" t="e">
         <f>utilities!$J$11</f>
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="I23" s="10">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I23" s="9">
         <f>utilities!$K$11</f>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24">
         <f>utilities!$H$8</f>
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="C24">
         <f>utilities!$I$8</f>
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="D24">
         <f>utilities!$J$8</f>
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="E24">
         <v>0</v>
       </c>
-      <c r="F24" s="4">
+      <c r="F24" s="4" t="e">
         <f>utilities!$H$11</f>
-        <v>9.6153846153846159E-2</v>
-      </c>
-      <c r="G24" s="4">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G24" s="4" t="e">
         <f>utilities!$I$11</f>
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="H24" s="4">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H24" s="4" t="e">
         <f>utilities!$J$11</f>
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="I24" s="10">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I24" s="9">
         <f>utilities!$K$11</f>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25">
         <f>utilities!$H$8</f>
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="C25">
         <f>utilities!$I$8</f>
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="D25">
         <f>utilities!$J$8</f>
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="E25">
         <v>0</v>
       </c>
-      <c r="F25" s="4">
+      <c r="F25" s="4" t="e">
         <f>utilities!$H$11</f>
-        <v>9.6153846153846159E-2</v>
-      </c>
-      <c r="G25" s="4">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G25" s="4" t="e">
         <f>utilities!$I$11</f>
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="H25" s="4">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H25" s="4" t="e">
         <f>utilities!$J$11</f>
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="I25" s="10">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I25" s="9">
         <f>utilities!$K$11</f>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26">
         <f>utilities!$H$8</f>
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="C26">
         <f>utilities!$I$8</f>
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="D26">
         <f>utilities!$J$8</f>
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="E26">
         <v>0</v>
       </c>
-      <c r="F26" s="4">
+      <c r="F26" s="4" t="e">
         <f>utilities!$H$11</f>
-        <v>9.6153846153846159E-2</v>
-      </c>
-      <c r="G26" s="4">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G26" s="4" t="e">
         <f>utilities!$I$11</f>
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="H26" s="4">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H26" s="4" t="e">
         <f>utilities!$J$11</f>
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="I26" s="10">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I26" s="9">
         <f>utilities!$K$11</f>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27">
         <f>utilities!$H$8</f>
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="C27">
         <f>utilities!$I$8</f>
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="D27">
         <f>utilities!$J$8</f>
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="E27">
         <v>0</v>
       </c>
-      <c r="F27" s="4">
+      <c r="F27" s="4" t="e">
         <f>utilities!$H$11</f>
-        <v>9.6153846153846159E-2</v>
-      </c>
-      <c r="G27" s="4">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G27" s="4" t="e">
         <f>utilities!$I$11</f>
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="H27" s="4">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H27" s="4" t="e">
         <f>utilities!$J$11</f>
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="I27" s="10">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I27" s="9">
         <f>utilities!$K$11</f>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28">
         <f>utilities!$H$8</f>
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="C28">
         <f>utilities!$I$8</f>
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="D28">
         <f>utilities!$J$8</f>
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="E28">
         <v>0</v>
       </c>
-      <c r="F28" s="4">
+      <c r="F28" s="4" t="e">
         <f>utilities!$H$11</f>
-        <v>9.6153846153846159E-2</v>
-      </c>
-      <c r="G28" s="4">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G28" s="4" t="e">
         <f>utilities!$I$11</f>
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="H28" s="4">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H28" s="4" t="e">
         <f>utilities!$J$11</f>
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="I28" s="10">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I28" s="9">
         <f>utilities!$K$11</f>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29">
         <f>utilities!$H$8</f>
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="C29">
         <f>utilities!$I$8</f>
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="D29">
         <f>utilities!$J$8</f>
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="E29">
         <v>0</v>
       </c>
-      <c r="F29" s="4">
+      <c r="F29" s="4" t="e">
         <f>utilities!$H$11</f>
-        <v>9.6153846153846159E-2</v>
-      </c>
-      <c r="G29" s="4">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G29" s="4" t="e">
         <f>utilities!$I$11</f>
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="H29" s="4">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H29" s="4" t="e">
         <f>utilities!$J$11</f>
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="I29" s="10">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I29" s="9">
         <f>utilities!$K$11</f>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30">
         <f>utilities!$H$8</f>
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="C30">
         <f>utilities!$I$8</f>
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="D30">
         <f>utilities!$J$8</f>
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="E30">
         <v>0</v>
       </c>
-      <c r="F30" s="4">
+      <c r="F30" s="4" t="e">
         <f>utilities!$H$11</f>
-        <v>9.6153846153846159E-2</v>
-      </c>
-      <c r="G30" s="4">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G30" s="4" t="e">
         <f>utilities!$I$11</f>
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="H30" s="4">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H30" s="4" t="e">
         <f>utilities!$J$11</f>
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="I30" s="10">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I30" s="9">
         <f>utilities!$K$11</f>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31">
         <f>utilities!$H$8</f>
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="C31">
         <f>utilities!$I$8</f>
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="D31">
         <f>utilities!$J$8</f>
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="E31">
         <v>0</v>
       </c>
-      <c r="F31" s="4">
+      <c r="F31" s="4" t="e">
         <f>utilities!$H$11</f>
-        <v>9.6153846153846159E-2</v>
-      </c>
-      <c r="G31" s="4">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G31" s="4" t="e">
         <f>utilities!$I$11</f>
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="H31" s="4">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H31" s="4" t="e">
         <f>utilities!$J$11</f>
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="I31" s="10">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I31" s="9">
         <f>utilities!$K$11</f>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B32">
         <f>utilities!$H$8</f>
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="C32">
         <f>utilities!$I$8</f>
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="D32">
         <f>utilities!$J$8</f>
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="E32">
         <v>0</v>
       </c>
-      <c r="F32" s="4">
+      <c r="F32" s="4" t="e">
         <f>utilities!$H$11</f>
-        <v>9.6153846153846159E-2</v>
-      </c>
-      <c r="G32" s="4">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G32" s="4" t="e">
         <f>utilities!$I$11</f>
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="H32" s="4">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H32" s="4" t="e">
         <f>utilities!$J$11</f>
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="I32" s="10">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I32" s="9">
         <f>utilities!$K$11</f>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B33">
         <f>utilities!$H$8</f>
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="C33">
         <f>utilities!$I$8</f>
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="D33">
         <f>utilities!$J$8</f>
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="E33">
         <v>0</v>
       </c>
-      <c r="F33" s="4">
+      <c r="F33" s="4" t="e">
         <f>utilities!$H$11</f>
-        <v>9.6153846153846159E-2</v>
-      </c>
-      <c r="G33" s="4">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G33" s="4" t="e">
         <f>utilities!$I$11</f>
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="H33" s="4">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H33" s="4" t="e">
         <f>utilities!$J$11</f>
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="I33" s="10">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I33" s="9">
         <f>utilities!$K$11</f>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B34">
         <f>utilities!$H$8</f>
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="C34">
         <f>utilities!$I$8</f>
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="D34">
         <f>utilities!$J$8</f>
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="E34">
         <v>0</v>
       </c>
-      <c r="F34" s="4">
+      <c r="F34" s="4" t="e">
         <f>utilities!$H$11</f>
-        <v>9.6153846153846159E-2</v>
-      </c>
-      <c r="G34" s="4">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G34" s="4" t="e">
         <f>utilities!$I$11</f>
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="H34" s="4">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H34" s="4" t="e">
         <f>utilities!$J$11</f>
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="I34" s="10">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I34" s="9">
         <f>utilities!$K$11</f>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B35">
         <f>utilities!$H$8</f>
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="C35">
         <f>utilities!$I$8</f>
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="D35">
         <f>utilities!$J$8</f>
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="E35">
         <v>0</v>
       </c>
-      <c r="F35" s="4">
+      <c r="F35" s="4" t="e">
         <f>utilities!$H$11</f>
-        <v>9.6153846153846159E-2</v>
-      </c>
-      <c r="G35" s="4">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G35" s="4" t="e">
         <f>utilities!$I$11</f>
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="H35" s="4">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H35" s="4" t="e">
         <f>utilities!$J$11</f>
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="I35" s="10">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I35" s="9">
         <f>utilities!$K$11</f>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B36">
         <f>utilities!$H$8</f>
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="C36">
         <f>utilities!$I$8</f>
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="D36">
         <f>utilities!$J$8</f>
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="E36">
         <v>0</v>
       </c>
-      <c r="F36" s="4">
+      <c r="F36" s="4" t="e">
         <f>utilities!$H$11</f>
-        <v>9.6153846153846159E-2</v>
-      </c>
-      <c r="G36" s="4">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G36" s="4" t="e">
         <f>utilities!$I$11</f>
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="H36" s="4">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H36" s="4" t="e">
         <f>utilities!$J$11</f>
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="I36" s="10">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I36" s="9">
         <f>utilities!$K$11</f>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B37">
         <f>utilities!$H$8</f>
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="C37">
         <f>utilities!$I$8</f>
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="D37">
         <f>utilities!$J$8</f>
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="E37">
         <v>0</v>
       </c>
-      <c r="F37" s="4">
+      <c r="F37" s="4" t="e">
         <f>utilities!$H$11</f>
-        <v>9.6153846153846159E-2</v>
-      </c>
-      <c r="G37" s="4">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G37" s="4" t="e">
         <f>utilities!$I$11</f>
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="H37" s="4">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H37" s="4" t="e">
         <f>utilities!$J$11</f>
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="I37" s="10">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I37" s="9">
         <f>utilities!$K$11</f>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B38">
         <f>utilities!$H$8</f>
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="C38">
         <f>utilities!$I$8</f>
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="D38">
         <f>utilities!$J$8</f>
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="E38">
         <v>0</v>
       </c>
-      <c r="F38" s="4">
+      <c r="F38" s="4" t="e">
         <f>utilities!$H$11</f>
-        <v>9.6153846153846159E-2</v>
-      </c>
-      <c r="G38" s="4">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G38" s="4" t="e">
         <f>utilities!$I$11</f>
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="H38" s="4">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H38" s="4" t="e">
         <f>utilities!$J$11</f>
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="I38" s="10">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I38" s="9">
         <f>utilities!$K$11</f>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B39">
         <f>utilities!$H$8</f>
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="C39">
         <f>utilities!$I$8</f>
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="D39">
         <f>utilities!$J$8</f>
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="E39">
         <v>0</v>
       </c>
-      <c r="F39" s="4">
+      <c r="F39" s="4" t="e">
         <f>utilities!$H$11</f>
-        <v>9.6153846153846159E-2</v>
-      </c>
-      <c r="G39" s="4">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G39" s="4" t="e">
         <f>utilities!$I$11</f>
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="H39" s="4">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H39" s="4" t="e">
         <f>utilities!$J$11</f>
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="I39" s="10">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I39" s="9">
         <f>utilities!$K$11</f>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B40">
         <f>utilities!$H$8</f>
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="C40">
         <f>utilities!$I$8</f>
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="D40">
         <f>utilities!$J$8</f>
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="E40">
         <v>0</v>
       </c>
-      <c r="F40" s="4">
+      <c r="F40" s="4" t="e">
         <f>utilities!$H$11</f>
-        <v>9.6153846153846159E-2</v>
-      </c>
-      <c r="G40" s="4">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G40" s="4" t="e">
         <f>utilities!$I$11</f>
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="H40" s="4">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H40" s="4" t="e">
         <f>utilities!$J$11</f>
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="I40" s="10">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I40" s="9">
         <f>utilities!$K$11</f>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B41">
         <f>utilities!$H$8</f>
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="C41">
         <f>utilities!$I$8</f>
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="D41">
         <f>utilities!$J$8</f>
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="E41">
         <v>0</v>
       </c>
-      <c r="F41" s="4">
+      <c r="F41" s="4" t="e">
         <f>utilities!$H$11</f>
-        <v>9.6153846153846159E-2</v>
-      </c>
-      <c r="G41" s="4">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G41" s="4" t="e">
         <f>utilities!$I$11</f>
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="H41" s="4">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H41" s="4" t="e">
         <f>utilities!$J$11</f>
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="I41" s="10">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I41" s="9">
+        <f>utilities!$K$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>40</v>
+      </c>
+      <c r="B42">
+        <f>utilities!$H$8</f>
+        <v>0</v>
+      </c>
+      <c r="C42">
+        <f>utilities!$I$8</f>
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <f>utilities!$J$8</f>
+        <v>0</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="F42" s="4" t="e">
+        <f>utilities!$H$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G42" s="4" t="e">
+        <f>utilities!$I$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H42" s="4" t="e">
+        <f>utilities!$J$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I42" s="9">
         <f>utilities!$K$11</f>
         <v>1E-3</v>
       </c>
@@ -2023,29 +2062,1553 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{117A8B26-635D-4B40-A90B-7735D1F1002F}">
-  <dimension ref="A1:Q21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FDEC06F-4DC9-4E7F-88C9-C6F486A3E573}">
+  <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.109375" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.77734375" customWidth="1"/>
-    <col min="16" max="16" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <f>utilities!$B$8</f>
+        <v>6</v>
+      </c>
+      <c r="C2">
+        <f>utilities!$C$8</f>
+        <v>8</v>
+      </c>
+      <c r="D2">
+        <f>utilities!$D$8</f>
+        <v>9</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2" s="4">
+        <f>utilities!$B$11</f>
+        <v>0.69444444444444453</v>
+      </c>
+      <c r="G2" s="4">
+        <f>utilities!$C$11</f>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="H2" s="4">
+        <f>utilities!$D$11</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="I2" s="9">
+        <f>utilities!$E$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <f>utilities!$B$8</f>
+        <v>6</v>
+      </c>
+      <c r="C3">
+        <f>utilities!$C$8</f>
+        <v>8</v>
+      </c>
+      <c r="D3">
+        <f>utilities!$D$8</f>
+        <v>9</v>
+      </c>
+      <c r="E3">
+        <v>10</v>
+      </c>
+      <c r="F3" s="4">
+        <f>utilities!$B$11</f>
+        <v>0.69444444444444453</v>
+      </c>
+      <c r="G3" s="4">
+        <f>utilities!$C$11</f>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="H3" s="4">
+        <f>utilities!$D$11</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="I3" s="9">
+        <f>utilities!$E$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <f>utilities!$B$8</f>
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <f>utilities!$C$8</f>
+        <v>8</v>
+      </c>
+      <c r="D4">
+        <f>utilities!$D$8</f>
+        <v>9</v>
+      </c>
+      <c r="E4">
+        <v>10</v>
+      </c>
+      <c r="F4" s="4">
+        <f>utilities!$B$11</f>
+        <v>0.69444444444444453</v>
+      </c>
+      <c r="G4" s="4">
+        <f>utilities!$C$11</f>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="H4" s="4">
+        <f>utilities!$D$11</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="I4" s="9">
+        <f>utilities!$E$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <f>utilities!$B$8</f>
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <f>utilities!$C$8</f>
+        <v>8</v>
+      </c>
+      <c r="D5">
+        <f>utilities!$D$8</f>
+        <v>9</v>
+      </c>
+      <c r="E5">
+        <v>10</v>
+      </c>
+      <c r="F5" s="4">
+        <f>utilities!$B$11</f>
+        <v>0.69444444444444453</v>
+      </c>
+      <c r="G5" s="4">
+        <f>utilities!$C$11</f>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="H5" s="4">
+        <f>utilities!$D$11</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="I5" s="9">
+        <f>utilities!$E$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <f>utilities!$B$8</f>
+        <v>6</v>
+      </c>
+      <c r="C6">
+        <f>utilities!$C$8</f>
+        <v>8</v>
+      </c>
+      <c r="D6">
+        <f>utilities!$D$8</f>
+        <v>9</v>
+      </c>
+      <c r="E6">
+        <v>10</v>
+      </c>
+      <c r="F6" s="4">
+        <f>utilities!$B$11</f>
+        <v>0.69444444444444453</v>
+      </c>
+      <c r="G6" s="4">
+        <f>utilities!$C$11</f>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="H6" s="4">
+        <f>utilities!$D$11</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="I6" s="9">
+        <f>utilities!$E$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <f>utilities!$B$8</f>
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <f>utilities!$C$8</f>
+        <v>8</v>
+      </c>
+      <c r="D7">
+        <f>utilities!$D$8</f>
+        <v>9</v>
+      </c>
+      <c r="E7">
+        <v>10</v>
+      </c>
+      <c r="F7" s="4">
+        <f>utilities!$B$11</f>
+        <v>0.69444444444444453</v>
+      </c>
+      <c r="G7" s="4">
+        <f>utilities!$C$11</f>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="H7" s="4">
+        <f>utilities!$D$11</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="I7" s="9">
+        <f>utilities!$E$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <f>utilities!$N$8</f>
+        <v>56</v>
+      </c>
+      <c r="C8">
+        <f>utilities!$O$8</f>
+        <v>98</v>
+      </c>
+      <c r="D8">
+        <f>utilities!$P$8</f>
+        <v>109</v>
+      </c>
+      <c r="E8">
+        <v>10</v>
+      </c>
+      <c r="F8" s="4">
+        <f>utilities!N11</f>
+        <v>0.46875</v>
+      </c>
+      <c r="G8" s="4">
+        <f>utilities!O11</f>
+        <v>0.125</v>
+      </c>
+      <c r="H8" s="4">
+        <f>utilities!P11</f>
+        <v>9.5454545454545459E-2</v>
+      </c>
+      <c r="I8" s="9">
+        <f>utilities!$E$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <f>utilities!$B$8</f>
+        <v>6</v>
+      </c>
+      <c r="C9">
+        <f>utilities!$C$8</f>
+        <v>8</v>
+      </c>
+      <c r="D9">
+        <f>utilities!$D$8</f>
+        <v>9</v>
+      </c>
+      <c r="E9">
+        <v>10</v>
+      </c>
+      <c r="F9" s="4">
+        <f>utilities!$B$11</f>
+        <v>0.69444444444444453</v>
+      </c>
+      <c r="G9" s="4">
+        <f>utilities!$C$11</f>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="H9" s="4">
+        <f>utilities!$D$11</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="I9" s="9">
+        <f>utilities!$E$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <f>utilities!$B$8</f>
+        <v>6</v>
+      </c>
+      <c r="C10">
+        <f>utilities!$C$8</f>
+        <v>8</v>
+      </c>
+      <c r="D10">
+        <f>utilities!$D$8</f>
+        <v>9</v>
+      </c>
+      <c r="E10">
+        <v>10</v>
+      </c>
+      <c r="F10" s="4">
+        <f>utilities!$B$11</f>
+        <v>0.69444444444444453</v>
+      </c>
+      <c r="G10" s="4">
+        <f>utilities!$C$11</f>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="H10" s="4">
+        <f>utilities!$D$11</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="I10" s="9">
+        <f>utilities!$E$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <f>utilities!$B$8</f>
+        <v>6</v>
+      </c>
+      <c r="C11">
+        <f>utilities!$C$8</f>
+        <v>8</v>
+      </c>
+      <c r="D11">
+        <f>utilities!$D$8</f>
+        <v>9</v>
+      </c>
+      <c r="E11">
+        <v>10</v>
+      </c>
+      <c r="F11" s="4">
+        <f>utilities!$B$11</f>
+        <v>0.69444444444444453</v>
+      </c>
+      <c r="G11" s="4">
+        <f>utilities!$C$11</f>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="H11" s="4">
+        <f>utilities!$D$11</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="I11" s="9">
+        <f>utilities!$E$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <f>utilities!$B$8</f>
+        <v>6</v>
+      </c>
+      <c r="C12">
+        <f>utilities!$C$8</f>
+        <v>8</v>
+      </c>
+      <c r="D12">
+        <f>utilities!$D$8</f>
+        <v>9</v>
+      </c>
+      <c r="E12">
+        <v>10</v>
+      </c>
+      <c r="F12" s="4">
+        <f>utilities!$B$11</f>
+        <v>0.69444444444444453</v>
+      </c>
+      <c r="G12" s="4">
+        <f>utilities!$C$11</f>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="H12" s="4">
+        <f>utilities!$D$11</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="I12" s="9">
+        <f>utilities!$E$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <f>utilities!$B$8</f>
+        <v>6</v>
+      </c>
+      <c r="C13">
+        <f>utilities!$C$8</f>
+        <v>8</v>
+      </c>
+      <c r="D13">
+        <f>utilities!$D$8</f>
+        <v>9</v>
+      </c>
+      <c r="E13">
+        <v>10</v>
+      </c>
+      <c r="F13" s="4">
+        <f>utilities!$B$11</f>
+        <v>0.69444444444444453</v>
+      </c>
+      <c r="G13" s="4">
+        <f>utilities!$C$11</f>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="H13" s="4">
+        <f>utilities!$D$11</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="I13" s="9">
+        <f>utilities!$E$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <f>utilities!T8</f>
+        <v>81</v>
+      </c>
+      <c r="C14">
+        <f>utilities!U8</f>
+        <v>143</v>
+      </c>
+      <c r="D14">
+        <f>utilities!V8</f>
+        <v>159</v>
+      </c>
+      <c r="E14">
+        <v>10</v>
+      </c>
+      <c r="F14" s="4">
+        <f>utilities!T11</f>
+        <v>0.32407407407407407</v>
+      </c>
+      <c r="G14" s="4">
+        <f>utilities!U11</f>
+        <v>8.4677419354838704E-2</v>
+      </c>
+      <c r="H14" s="4">
+        <f>utilities!V11</f>
+        <v>6.5625000000000003E-2</v>
+      </c>
+      <c r="I14" s="9">
+        <f>utilities!$E$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <f>utilities!$B$8</f>
+        <v>6</v>
+      </c>
+      <c r="C15">
+        <f>utilities!$C$8</f>
+        <v>8</v>
+      </c>
+      <c r="D15">
+        <f>utilities!$D$8</f>
+        <v>9</v>
+      </c>
+      <c r="E15">
+        <v>10</v>
+      </c>
+      <c r="F15" s="4">
+        <f>utilities!$B$11</f>
+        <v>0.69444444444444453</v>
+      </c>
+      <c r="G15" s="4">
+        <f>utilities!$C$11</f>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="H15" s="4">
+        <f>utilities!$D$11</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="I15" s="9">
+        <f>utilities!$E$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <f>utilities!$B$8</f>
+        <v>6</v>
+      </c>
+      <c r="C16">
+        <f>utilities!$C$8</f>
+        <v>8</v>
+      </c>
+      <c r="D16">
+        <f>utilities!$D$8</f>
+        <v>9</v>
+      </c>
+      <c r="E16">
+        <v>10</v>
+      </c>
+      <c r="F16" s="4">
+        <f>utilities!$B$11</f>
+        <v>0.69444444444444453</v>
+      </c>
+      <c r="G16" s="4">
+        <f>utilities!$C$11</f>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="H16" s="4">
+        <f>utilities!$D$11</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="I16" s="9">
+        <f>utilities!$E$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <f>utilities!$B$8</f>
+        <v>6</v>
+      </c>
+      <c r="C17">
+        <f>utilities!$C$8</f>
+        <v>8</v>
+      </c>
+      <c r="D17">
+        <f>utilities!$D$8</f>
+        <v>9</v>
+      </c>
+      <c r="E17">
+        <v>10</v>
+      </c>
+      <c r="F17" s="4">
+        <f>utilities!$B$11</f>
+        <v>0.69444444444444453</v>
+      </c>
+      <c r="G17" s="4">
+        <f>utilities!$C$11</f>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="H17" s="4">
+        <f>utilities!$D$11</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="I17" s="9">
+        <f>utilities!$E$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <f>utilities!$B$8</f>
+        <v>6</v>
+      </c>
+      <c r="C18">
+        <f>utilities!$C$8</f>
+        <v>8</v>
+      </c>
+      <c r="D18">
+        <f>utilities!$D$8</f>
+        <v>9</v>
+      </c>
+      <c r="E18">
+        <v>10</v>
+      </c>
+      <c r="F18" s="4">
+        <f>utilities!$B$11</f>
+        <v>0.69444444444444453</v>
+      </c>
+      <c r="G18" s="4">
+        <f>utilities!$C$11</f>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="H18" s="4">
+        <f>utilities!$D$11</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="I18" s="9">
+        <f>utilities!$E$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <f>utilities!$B$8</f>
+        <v>6</v>
+      </c>
+      <c r="C19">
+        <f>utilities!$C$8</f>
+        <v>8</v>
+      </c>
+      <c r="D19">
+        <f>utilities!$D$8</f>
+        <v>9</v>
+      </c>
+      <c r="E19">
+        <v>10</v>
+      </c>
+      <c r="F19" s="4">
+        <f>utilities!$B$11</f>
+        <v>0.69444444444444453</v>
+      </c>
+      <c r="G19" s="4">
+        <f>utilities!$C$11</f>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="H19" s="4">
+        <f>utilities!$D$11</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="I19" s="9">
+        <f>utilities!$E$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <f>utilities!$B$8</f>
+        <v>6</v>
+      </c>
+      <c r="C20">
+        <f>utilities!$C$8</f>
+        <v>8</v>
+      </c>
+      <c r="D20">
+        <f>utilities!$D$8</f>
+        <v>9</v>
+      </c>
+      <c r="E20">
+        <v>10</v>
+      </c>
+      <c r="F20" s="4">
+        <f>utilities!$B$11</f>
+        <v>0.69444444444444453</v>
+      </c>
+      <c r="G20" s="4">
+        <f>utilities!$C$11</f>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="H20" s="4">
+        <f>utilities!$D$11</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="I20" s="9">
+        <f>utilities!$E$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <f>utilities!$B$8</f>
+        <v>6</v>
+      </c>
+      <c r="C21">
+        <f>utilities!$C$8</f>
+        <v>8</v>
+      </c>
+      <c r="D21">
+        <f>utilities!$D$8</f>
+        <v>9</v>
+      </c>
+      <c r="E21">
+        <v>10</v>
+      </c>
+      <c r="F21" s="4">
+        <f>utilities!$B$11</f>
+        <v>0.69444444444444453</v>
+      </c>
+      <c r="G21" s="4">
+        <f>utilities!$C$11</f>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="H21" s="4">
+        <f>utilities!$D$11</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="I21" s="9">
+        <f>utilities!$E$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22">
+        <f>utilities!$B$8</f>
+        <v>6</v>
+      </c>
+      <c r="C22">
+        <f>utilities!$C$8</f>
+        <v>8</v>
+      </c>
+      <c r="D22">
+        <f>utilities!$D$8</f>
+        <v>9</v>
+      </c>
+      <c r="E22">
+        <v>10</v>
+      </c>
+      <c r="F22" s="4">
+        <f>utilities!$B$11</f>
+        <v>0.69444444444444453</v>
+      </c>
+      <c r="G22" s="4">
+        <f>utilities!$C$11</f>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="H22" s="4">
+        <f>utilities!$D$11</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="I22" s="9">
+        <f>utilities!$E$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23">
+        <f>utilities!$H$8</f>
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <f>utilities!$I$8</f>
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <f>utilities!$J$8</f>
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23" s="4" t="e">
+        <f>utilities!$H$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G23" s="4" t="e">
+        <f>utilities!$I$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H23" s="4" t="e">
+        <f>utilities!$J$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I23" s="9">
+        <f>utilities!$K$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24">
+        <f>utilities!$H$8</f>
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <f>utilities!$I$8</f>
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <f>utilities!$J$8</f>
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24" s="4" t="e">
+        <f>utilities!$H$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G24" s="4" t="e">
+        <f>utilities!$I$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H24" s="4" t="e">
+        <f>utilities!$J$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I24" s="9">
+        <f>utilities!$K$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25">
+        <f>utilities!$H$8</f>
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <f>utilities!$I$8</f>
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <f>utilities!$J$8</f>
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25" s="4" t="e">
+        <f>utilities!$H$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G25" s="4" t="e">
+        <f>utilities!$I$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H25" s="4" t="e">
+        <f>utilities!$J$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I25" s="9">
+        <f>utilities!$K$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26">
+        <f>utilities!$H$8</f>
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <f>utilities!$I$8</f>
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <f>utilities!$J$8</f>
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26" s="4" t="e">
+        <f>utilities!$H$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G26" s="4" t="e">
+        <f>utilities!$I$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H26" s="4" t="e">
+        <f>utilities!$J$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I26" s="9">
+        <f>utilities!$K$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27">
+        <f>utilities!$H$8</f>
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <f>utilities!$I$8</f>
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <f>utilities!$J$8</f>
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27" s="4" t="e">
+        <f>utilities!$H$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G27" s="4" t="e">
+        <f>utilities!$I$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H27" s="4" t="e">
+        <f>utilities!$J$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I27" s="9">
+        <f>utilities!$K$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="B28">
+        <f>utilities!$H$8</f>
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <f>utilities!$I$8</f>
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <f>utilities!$J$8</f>
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28" s="4" t="e">
+        <f>utilities!$H$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G28" s="4" t="e">
+        <f>utilities!$I$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H28" s="4" t="e">
+        <f>utilities!$J$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I28" s="9">
+        <f>utilities!$K$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="B29">
+        <f>utilities!$H$8</f>
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <f>utilities!$I$8</f>
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <f>utilities!$J$8</f>
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29" s="4" t="e">
+        <f>utilities!$H$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G29" s="4" t="e">
+        <f>utilities!$I$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H29" s="4" t="e">
+        <f>utilities!$J$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I29" s="9">
+        <f>utilities!$K$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>28</v>
+      </c>
+      <c r="B30">
+        <f>utilities!$H$8</f>
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <f>utilities!$I$8</f>
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <f>utilities!$J$8</f>
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30" s="4" t="e">
+        <f>utilities!$H$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G30" s="4" t="e">
+        <f>utilities!$I$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H30" s="4" t="e">
+        <f>utilities!$J$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I30" s="9">
+        <f>utilities!$K$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="B31">
+        <f>utilities!$H$8</f>
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <f>utilities!$I$8</f>
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <f>utilities!$J$8</f>
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31" s="4" t="e">
+        <f>utilities!$H$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G31" s="4" t="e">
+        <f>utilities!$I$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H31" s="4" t="e">
+        <f>utilities!$J$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I31" s="9">
+        <f>utilities!$K$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>30</v>
+      </c>
+      <c r="B32">
+        <f>utilities!$H$8</f>
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <f>utilities!$I$8</f>
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <f>utilities!$J$8</f>
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32" s="4" t="e">
+        <f>utilities!$H$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G32" s="4" t="e">
+        <f>utilities!$I$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H32" s="4" t="e">
+        <f>utilities!$J$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I32" s="9">
+        <f>utilities!$K$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>31</v>
+      </c>
+      <c r="B33">
+        <f>utilities!$H$8</f>
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <f>utilities!$I$8</f>
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <f>utilities!$J$8</f>
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33" s="4" t="e">
+        <f>utilities!$H$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G33" s="4" t="e">
+        <f>utilities!$I$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H33" s="4" t="e">
+        <f>utilities!$J$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I33" s="9">
+        <f>utilities!$K$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>32</v>
+      </c>
+      <c r="B34">
+        <f>utilities!$H$8</f>
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <f>utilities!$I$8</f>
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <f>utilities!$J$8</f>
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34" s="4" t="e">
+        <f>utilities!$H$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G34" s="4" t="e">
+        <f>utilities!$I$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H34" s="4" t="e">
+        <f>utilities!$J$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I34" s="9">
+        <f>utilities!$K$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>33</v>
+      </c>
+      <c r="B35">
+        <f>utilities!$H$8</f>
+        <v>0</v>
+      </c>
+      <c r="C35">
+        <f>utilities!$I$8</f>
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <f>utilities!$J$8</f>
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35" s="4" t="e">
+        <f>utilities!$H$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G35" s="4" t="e">
+        <f>utilities!$I$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H35" s="4" t="e">
+        <f>utilities!$J$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I35" s="9">
+        <f>utilities!$K$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>34</v>
+      </c>
+      <c r="B36">
+        <f>utilities!$H$8</f>
+        <v>0</v>
+      </c>
+      <c r="C36">
+        <f>utilities!$I$8</f>
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <f>utilities!$J$8</f>
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36" s="4" t="e">
+        <f>utilities!$H$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G36" s="4" t="e">
+        <f>utilities!$I$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H36" s="4" t="e">
+        <f>utilities!$J$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I36" s="9">
+        <f>utilities!$K$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>35</v>
+      </c>
+      <c r="B37">
+        <f>utilities!$H$8</f>
+        <v>0</v>
+      </c>
+      <c r="C37">
+        <f>utilities!$I$8</f>
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <f>utilities!$J$8</f>
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37" s="4" t="e">
+        <f>utilities!$H$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G37" s="4" t="e">
+        <f>utilities!$I$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H37" s="4" t="e">
+        <f>utilities!$J$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I37" s="9">
+        <f>utilities!$K$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>36</v>
+      </c>
+      <c r="B38">
+        <f>utilities!$H$8</f>
+        <v>0</v>
+      </c>
+      <c r="C38">
+        <f>utilities!$I$8</f>
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <f>utilities!$J$8</f>
+        <v>0</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="F38" s="4" t="e">
+        <f>utilities!$H$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G38" s="4" t="e">
+        <f>utilities!$I$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H38" s="4" t="e">
+        <f>utilities!$J$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I38" s="9">
+        <f>utilities!$K$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>37</v>
+      </c>
+      <c r="B39">
+        <f>utilities!$H$8</f>
+        <v>0</v>
+      </c>
+      <c r="C39">
+        <f>utilities!$I$8</f>
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <f>utilities!$J$8</f>
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39" s="4" t="e">
+        <f>utilities!$H$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G39" s="4" t="e">
+        <f>utilities!$I$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H39" s="4" t="e">
+        <f>utilities!$J$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I39" s="9">
+        <f>utilities!$K$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>38</v>
+      </c>
+      <c r="B40">
+        <f>utilities!$H$8</f>
+        <v>0</v>
+      </c>
+      <c r="C40">
+        <f>utilities!$I$8</f>
+        <v>0</v>
+      </c>
+      <c r="D40">
+        <f>utilities!$J$8</f>
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40" s="4" t="e">
+        <f>utilities!$H$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G40" s="4" t="e">
+        <f>utilities!$I$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H40" s="4" t="e">
+        <f>utilities!$J$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I40" s="9">
+        <f>utilities!$K$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>39</v>
+      </c>
+      <c r="B41">
+        <f>utilities!$H$8</f>
+        <v>0</v>
+      </c>
+      <c r="C41">
+        <f>utilities!$I$8</f>
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <f>utilities!$J$8</f>
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41" s="4" t="e">
+        <f>utilities!$H$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G41" s="4" t="e">
+        <f>utilities!$I$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H41" s="4" t="e">
+        <f>utilities!$J$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I41" s="9">
+        <f>utilities!$K$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>40</v>
+      </c>
+      <c r="B42">
+        <f>utilities!$H$8</f>
+        <v>0</v>
+      </c>
+      <c r="C42">
+        <f>utilities!$I$8</f>
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <f>utilities!$J$8</f>
+        <v>0</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="F42" s="4" t="e">
+        <f>utilities!$H$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G42" s="4" t="e">
+        <f>utilities!$I$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H42" s="4" t="e">
+        <f>utilities!$J$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I42" s="9">
+        <f>utilities!$K$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{117A8B26-635D-4B40-A90B-7735D1F1002F}">
+  <dimension ref="A1:W21"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="V9" sqref="V9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.140625" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" customWidth="1"/>
+    <col min="16" max="16" width="9.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D1" s="2"/>
       <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -2056,7 +3619,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>25</v>
       </c>
@@ -2070,13 +3633,13 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A4" s="9"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A4" s="8"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
       <c r="D4" s="5"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -2086,8 +3649,11 @@
       <c r="M6" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="S6" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>17</v>
       </c>
@@ -2124,49 +3690,74 @@
       <c r="Q7" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="T7" t="s">
+        <v>17</v>
+      </c>
+      <c r="U7" t="s">
+        <v>12</v>
+      </c>
+      <c r="V7" t="s">
+        <v>13</v>
+      </c>
+      <c r="W7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
       <c r="B8">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C8">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="D8">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="G8" t="s">
         <v>14</v>
       </c>
       <c r="H8">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="I8">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="J8">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="M8" t="s">
         <v>14</v>
       </c>
       <c r="N8">
         <f>50+B8</f>
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="O8">
-        <f>100+C8</f>
-        <v>121</v>
+        <v>98</v>
       </c>
       <c r="P8">
-        <f>125+D8</f>
-        <v>148</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+        <v>109</v>
+      </c>
+      <c r="S8" t="s">
+        <v>14</v>
+      </c>
+      <c r="T8">
+        <f>75+B8</f>
+        <v>81</v>
+      </c>
+      <c r="U8">
+        <f>135+C8</f>
+        <v>143</v>
+      </c>
+      <c r="V8">
+        <f>150+D8</f>
+        <v>159</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -2185,22 +3776,28 @@
       <c r="N9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="S9" t="s">
+        <v>25</v>
+      </c>
+      <c r="T9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>22</v>
       </c>
       <c r="B10" s="3">
         <f>A3/$B$12*B$9</f>
-        <v>2.5</v>
+        <v>4.166666666666667</v>
       </c>
       <c r="C10" s="3">
         <f>B3/$B$12*B9</f>
-        <v>0.5</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="D10" s="3">
         <f>C3/$B$12*B9</f>
-        <v>0.1</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="E10" s="6">
         <f>D3</f>
@@ -2228,15 +3825,15 @@
       <c r="M10" t="s">
         <v>16</v>
       </c>
-      <c r="N10" s="8">
+      <c r="N10" s="3">
         <f>A3/$N$12+H10</f>
         <v>26.25</v>
       </c>
-      <c r="O10" s="8">
+      <c r="O10" s="3">
         <f>B3/$N$12+I10</f>
         <v>5.25</v>
       </c>
-      <c r="P10" s="8">
+      <c r="P10" s="3">
         <f>C3/$N$12+J10</f>
         <v>1.05</v>
       </c>
@@ -2244,43 +3841,62 @@
         <f>K10</f>
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="S10" t="s">
+        <v>16</v>
+      </c>
+      <c r="T10" s="3">
+        <f>G3/$N$12+N10</f>
+        <v>26.25</v>
+      </c>
+      <c r="U10" s="3">
+        <f>H3/$N$12+O10</f>
+        <v>5.25</v>
+      </c>
+      <c r="V10" s="3">
+        <f>I3/$N$12+P10</f>
+        <v>1.05</v>
+      </c>
+      <c r="W10" s="6">
+        <f>Q10</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="4">
         <f>B10/B8</f>
-        <v>0.15625</v>
+        <v>0.69444444444444453</v>
       </c>
       <c r="C11" s="7">
         <f>C10/(C8-B8)</f>
-        <v>0.1</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="D11" s="7">
         <f>D10/(D8-C8)</f>
-        <v>0.05</v>
-      </c>
-      <c r="E11" s="10">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="E11" s="9">
         <f>E10</f>
         <v>1E-3</v>
       </c>
       <c r="G11" t="s">
         <v>15</v>
       </c>
-      <c r="H11" s="4">
+      <c r="H11" s="4" t="e">
         <f>H10/H8</f>
-        <v>9.6153846153846159E-2</v>
-      </c>
-      <c r="I11" s="7">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I11" s="7" t="e">
         <f>I10/(I8-H8)</f>
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="J11" s="7">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J11" s="7" t="e">
         <f>J10/(J8-I8)</f>
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="K11" s="10">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K11" s="9">
         <f>K10</f>
         <v>1E-3</v>
       </c>
@@ -2289,28 +3905,47 @@
       </c>
       <c r="N11" s="4">
         <f>N10/N8</f>
-        <v>0.39772727272727271</v>
+        <v>0.46875</v>
       </c>
       <c r="O11" s="7">
         <f>O10/(O8-N8)</f>
-        <v>9.5454545454545459E-2</v>
+        <v>0.125</v>
       </c>
       <c r="P11" s="7">
         <f>P10/(P8-O8)</f>
-        <v>3.888888888888889E-2</v>
-      </c>
-      <c r="Q11" s="10">
+        <v>9.5454545454545459E-2</v>
+      </c>
+      <c r="Q11" s="9">
         <f>Q10</f>
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="S11" t="s">
+        <v>15</v>
+      </c>
+      <c r="T11" s="4">
+        <f>T10/T8</f>
+        <v>0.32407407407407407</v>
+      </c>
+      <c r="U11" s="7">
+        <f>U10/(U8-T8)</f>
+        <v>8.4677419354838704E-2</v>
+      </c>
+      <c r="V11" s="7">
+        <f>V10/(V8-U8)</f>
+        <v>6.5625000000000003E-2</v>
+      </c>
+      <c r="W11" s="9">
+        <f>W10</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
       <c r="B12">
         <f>B14-B13+1</f>
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="G12" t="s">
         <v>18</v>
@@ -2326,8 +3961,15 @@
         <f>N14-N13+1</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="S12" t="s">
+        <v>18</v>
+      </c>
+      <c r="T12">
+        <f>T14-T13+1</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -2344,15 +3986,21 @@
         <v>20</v>
       </c>
       <c r="N13">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+      <c r="S13" t="s">
+        <v>20</v>
+      </c>
+      <c r="T13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>21</v>
       </c>
       <c r="B14">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C14" s="7"/>
       <c r="G14" t="s">
@@ -2365,16 +4013,22 @@
         <v>21</v>
       </c>
       <c r="N14">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+      <c r="S14" t="s">
+        <v>21</v>
+      </c>
+      <c r="T14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>24</v>
       </c>
       <c r="E15" s="4">
         <f>SUM(B10:E10)*B12</f>
-        <v>62.019999999999996</v>
+        <v>62.012000000000008</v>
       </c>
       <c r="G15" t="s">
         <v>24</v>
@@ -2390,21 +4044,28 @@
         <f>SUM(N10:Q10)*N12</f>
         <v>32.550999999999995</v>
       </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="S15" t="s">
+        <v>24</v>
+      </c>
+      <c r="W15" s="4">
+        <f>SUM(T10:W10)*T12</f>
+        <v>32.550999999999995</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B17" s="7">
-        <f>E15+K15+Q15</f>
-        <v>125.59099999999998</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+        <f>E15+Q15+W15</f>
+        <v>127.114</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B18" s="7"/>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="P21" s="11"/>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P21" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
sddp merton longer stages
</commit_message>
<xml_diff>
--- a/julia_msp/goal_data.xlsx
+++ b/julia_msp/goal_data.xlsx
@@ -2,19 +2,19 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matsz\programowanie\Optymalizacja portfela\julia_msp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D125E526-1F36-4648-8480-172C1D1A898A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C1553553-A96B-4DCF-8C56-D44851FF15BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E8CF1CA2-D953-46E5-99F4-DA96611E7E6D}"/>
   </bookViews>
   <sheets>
     <sheet name="goal_data" sheetId="1" r:id="rId1"/>
-    <sheet name="goal_data (2)" sheetId="3" r:id="rId2"/>
+    <sheet name="goal_data s12" sheetId="4" r:id="rId2"/>
     <sheet name="utilities" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="28">
   <si>
     <t>minimum_limit</t>
   </si>
@@ -120,6 +120,9 @@
   <si>
     <t>goal34</t>
   </si>
+  <si>
+    <t>S12</t>
+  </si>
 </sst>
 </file>
 
@@ -133,7 +136,7 @@
     <numFmt numFmtId="167" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="168" formatCode="_-* #,##0.0000\ _z_ł_-;\-* #,##0.0000\ _z_ł_-;_-* &quot;-&quot;????\ _z_ł_-;_-@_-"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -165,6 +168,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -174,7 +184,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -182,12 +192,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -203,6 +228,9 @@
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -539,10 +567,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FFE0B56-DF8B-44CF-9758-6EDE70A13051}">
-  <dimension ref="A1:I42"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -585,31 +613,25 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <f>utilities!$B$8</f>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C2">
-        <f>utilities!$C$8</f>
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D2">
-        <f>utilities!$D$8</f>
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F2" s="4">
-        <f>utilities!$B$11</f>
-        <v>0.69444444444444453</v>
+        <v>1.0416666666666667</v>
       </c>
       <c r="G2" s="4">
-        <f>utilities!$C$11</f>
-        <v>0.41666666666666669</v>
+        <v>0.625</v>
       </c>
       <c r="H2" s="4">
-        <f>utilities!$D$11</f>
-        <v>0.16666666666666666</v>
+        <v>0.25</v>
       </c>
       <c r="I2" s="9">
         <f>utilities!$E$11</f>
@@ -622,22 +644,22 @@
       </c>
       <c r="B3">
         <f>utilities!$B$8</f>
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C3">
         <f>utilities!$C$8</f>
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="D3">
         <f>utilities!$D$8</f>
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="E3">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="F3" s="4">
         <f>utilities!$B$11</f>
-        <v>0.69444444444444453</v>
+        <v>0.69444444444444442</v>
       </c>
       <c r="G3" s="4">
         <f>utilities!$C$11</f>
@@ -657,59 +679,59 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <f>utilities!$B$8</f>
-        <v>6</v>
+        <f>utilities!$N$8</f>
+        <v>68</v>
       </c>
       <c r="C4">
-        <f>utilities!$C$8</f>
-        <v>8</v>
+        <f>utilities!$O$8</f>
+        <v>114</v>
       </c>
       <c r="D4">
-        <f>utilities!$D$8</f>
-        <v>9</v>
+        <f>utilities!$P$8</f>
+        <v>127</v>
       </c>
       <c r="E4">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="F4" s="4">
-        <f>utilities!$B$11</f>
-        <v>0.69444444444444453</v>
+        <f>utilities!N11</f>
+        <v>0.3860294117647059</v>
       </c>
       <c r="G4" s="4">
-        <f>utilities!$C$11</f>
-        <v>0.41666666666666669</v>
+        <f>utilities!O11</f>
+        <v>0.11413043478260869</v>
       </c>
       <c r="H4" s="4">
-        <f>utilities!$D$11</f>
-        <v>0.16666666666666666</v>
+        <f>utilities!P11</f>
+        <v>8.0769230769230774E-2</v>
       </c>
       <c r="I4" s="9">
         <f>utilities!$E$11</f>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
         <f>utilities!$B$8</f>
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C5">
         <f>utilities!$C$8</f>
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="D5">
         <f>utilities!$D$8</f>
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="E5">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="F5" s="4">
         <f>utilities!$B$11</f>
-        <v>0.69444444444444453</v>
+        <v>0.69444444444444442</v>
       </c>
       <c r="G5" s="4">
         <f>utilities!$C$11</f>
@@ -724,36 +746,33 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6">
-        <f>utilities!$B$8</f>
-        <v>6</v>
-      </c>
-      <c r="C6">
-        <f>utilities!$C$8</f>
-        <v>8</v>
-      </c>
-      <c r="D6">
-        <f>utilities!$D$8</f>
-        <v>9</v>
+      <c r="B6" s="12">
+        <v>87</v>
+      </c>
+      <c r="C6" s="12">
+        <v>151</v>
+      </c>
+      <c r="D6" s="12">
+        <v>168</v>
       </c>
       <c r="E6">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F6" s="4">
-        <f>utilities!$B$11</f>
-        <v>0.69444444444444453</v>
+        <f>utilities!T11</f>
+        <v>0.30172413793103448</v>
       </c>
       <c r="G6" s="4">
-        <f>utilities!$C$11</f>
-        <v>0.41666666666666669</v>
+        <f>utilities!U11</f>
+        <v>8.203125E-2</v>
       </c>
       <c r="H6" s="4">
-        <f>utilities!$D$11</f>
-        <v>0.16666666666666666</v>
+        <f>utilities!V11</f>
+        <v>6.1764705882352944E-2</v>
       </c>
       <c r="I6" s="9">
         <f>utilities!$E$11</f>
@@ -762,26 +781,26 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B7">
-        <f>utilities!$B$8</f>
-        <v>6</v>
+        <f>utilities!$H$8</f>
+        <v>0</v>
       </c>
       <c r="C7">
-        <f>utilities!$C$8</f>
-        <v>8</v>
+        <f>utilities!$I$8</f>
+        <v>0</v>
       </c>
       <c r="D7">
-        <f>utilities!$D$8</f>
-        <v>9</v>
+        <f>utilities!$J$8</f>
+        <v>0</v>
       </c>
       <c r="E7">
-        <v>10</v>
+        <v>-8</v>
       </c>
       <c r="F7" s="4">
         <f>utilities!$B$11</f>
-        <v>0.69444444444444453</v>
+        <v>0.69444444444444442</v>
       </c>
       <c r="G7" s="4">
         <f>utilities!$C$11</f>
@@ -798,34 +817,34 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B8">
-        <f>utilities!$N$8</f>
-        <v>56</v>
+        <f>utilities!$H$8</f>
+        <v>0</v>
       </c>
       <c r="C8">
-        <f>utilities!$O$8</f>
-        <v>98</v>
+        <f>utilities!$I$8</f>
+        <v>0</v>
       </c>
       <c r="D8">
-        <f>utilities!$P$8</f>
-        <v>109</v>
+        <f>utilities!$J$8</f>
+        <v>0</v>
       </c>
       <c r="E8">
-        <v>10</v>
+        <v>-7</v>
       </c>
       <c r="F8" s="4">
-        <f>utilities!N11</f>
-        <v>0.46875</v>
+        <f>utilities!$B$11</f>
+        <v>0.69444444444444442</v>
       </c>
       <c r="G8" s="4">
-        <f>utilities!O11</f>
-        <v>0.125</v>
+        <f>utilities!$C$11</f>
+        <v>0.41666666666666669</v>
       </c>
       <c r="H8" s="4">
-        <f>utilities!P11</f>
-        <v>9.5454545454545459E-2</v>
+        <f>utilities!$D$11</f>
+        <v>0.16666666666666666</v>
       </c>
       <c r="I8" s="9">
         <f>utilities!$E$11</f>
@@ -834,26 +853,26 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B9">
-        <f>utilities!$B$8</f>
-        <v>6</v>
+        <f>utilities!$H$8</f>
+        <v>0</v>
       </c>
       <c r="C9">
-        <f>utilities!$C$8</f>
-        <v>8</v>
+        <f>utilities!$I$8</f>
+        <v>0</v>
       </c>
       <c r="D9">
-        <f>utilities!$D$8</f>
-        <v>9</v>
+        <f>utilities!$J$8</f>
+        <v>0</v>
       </c>
       <c r="E9">
-        <v>10</v>
+        <v>-6</v>
       </c>
       <c r="F9" s="4">
         <f>utilities!$B$11</f>
-        <v>0.69444444444444453</v>
+        <v>0.69444444444444442</v>
       </c>
       <c r="G9" s="4">
         <f>utilities!$C$11</f>
@@ -870,26 +889,26 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B10">
-        <f>utilities!$B$8</f>
-        <v>6</v>
+        <f>utilities!$H$8</f>
+        <v>0</v>
       </c>
       <c r="C10">
-        <f>utilities!$C$8</f>
-        <v>8</v>
+        <f>utilities!$I$8</f>
+        <v>0</v>
       </c>
       <c r="D10">
-        <f>utilities!$D$8</f>
-        <v>9</v>
+        <f>utilities!$J$8</f>
+        <v>0</v>
       </c>
       <c r="E10">
-        <v>10</v>
+        <v>-5</v>
       </c>
       <c r="F10" s="4">
         <f>utilities!$B$11</f>
-        <v>0.69444444444444453</v>
+        <v>0.69444444444444442</v>
       </c>
       <c r="G10" s="4">
         <f>utilities!$C$11</f>
@@ -906,26 +925,26 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B11">
-        <f>utilities!$B$8</f>
-        <v>6</v>
+        <f>utilities!$H$8</f>
+        <v>0</v>
       </c>
       <c r="C11">
-        <f>utilities!$C$8</f>
-        <v>8</v>
+        <f>utilities!$I$8</f>
+        <v>0</v>
       </c>
       <c r="D11">
-        <f>utilities!$D$8</f>
-        <v>9</v>
+        <f>utilities!$J$8</f>
+        <v>0</v>
       </c>
       <c r="E11">
-        <v>10</v>
+        <v>-4</v>
       </c>
       <c r="F11" s="4">
         <f>utilities!$B$11</f>
-        <v>0.69444444444444453</v>
+        <v>0.69444444444444442</v>
       </c>
       <c r="G11" s="4">
         <f>utilities!$C$11</f>
@@ -942,26 +961,26 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B12">
-        <f>utilities!$B$8</f>
-        <v>6</v>
+        <f>utilities!$H$8</f>
+        <v>0</v>
       </c>
       <c r="C12">
-        <f>utilities!$C$8</f>
-        <v>8</v>
+        <f>utilities!$I$8</f>
+        <v>0</v>
       </c>
       <c r="D12">
-        <f>utilities!$D$8</f>
-        <v>9</v>
+        <f>utilities!$J$8</f>
+        <v>0</v>
       </c>
       <c r="E12">
-        <v>10</v>
+        <v>-3</v>
       </c>
       <c r="F12" s="4">
         <f>utilities!$B$11</f>
-        <v>0.69444444444444453</v>
+        <v>0.69444444444444442</v>
       </c>
       <c r="G12" s="4">
         <f>utilities!$C$11</f>
@@ -978,26 +997,26 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B13">
-        <f>utilities!$B$8</f>
-        <v>6</v>
+        <f>utilities!$H$8</f>
+        <v>0</v>
       </c>
       <c r="C13">
-        <f>utilities!$C$8</f>
-        <v>8</v>
+        <f>utilities!$I$8</f>
+        <v>0</v>
       </c>
       <c r="D13">
-        <f>utilities!$D$8</f>
-        <v>9</v>
+        <f>utilities!$J$8</f>
+        <v>0</v>
       </c>
       <c r="E13">
-        <v>10</v>
+        <v>-2</v>
       </c>
       <c r="F13" s="4">
         <f>utilities!$B$11</f>
-        <v>0.69444444444444453</v>
+        <v>0.69444444444444442</v>
       </c>
       <c r="G13" s="4">
         <f>utilities!$C$11</f>
@@ -1014,34 +1033,34 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B14">
-        <f>utilities!T8</f>
-        <v>81</v>
+        <f>utilities!$H$8</f>
+        <v>0</v>
       </c>
       <c r="C14">
-        <f>utilities!U8</f>
-        <v>143</v>
+        <f>utilities!$I$8</f>
+        <v>0</v>
       </c>
       <c r="D14">
-        <f>utilities!V8</f>
-        <v>159</v>
+        <f>utilities!$J$8</f>
+        <v>0</v>
       </c>
       <c r="E14">
-        <v>10</v>
+        <v>-1</v>
       </c>
       <c r="F14" s="4">
-        <f>utilities!T11</f>
-        <v>0.32407407407407407</v>
+        <f>utilities!$B$11</f>
+        <v>0.69444444444444442</v>
       </c>
       <c r="G14" s="4">
-        <f>utilities!U11</f>
-        <v>8.4677419354838704E-2</v>
+        <f>utilities!$C$11</f>
+        <v>0.41666666666666669</v>
       </c>
       <c r="H14" s="4">
-        <f>utilities!V11</f>
-        <v>6.5625000000000003E-2</v>
+        <f>utilities!$D$11</f>
+        <v>0.16666666666666666</v>
       </c>
       <c r="I14" s="9">
         <f>utilities!$E$11</f>
@@ -1050,295 +1069,295 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B15">
-        <f>utilities!$B$8</f>
-        <v>6</v>
+        <f>utilities!$H$8</f>
+        <v>0</v>
       </c>
       <c r="C15">
-        <f>utilities!$C$8</f>
-        <v>8</v>
+        <f>utilities!$I$8</f>
+        <v>0</v>
       </c>
       <c r="D15">
-        <f>utilities!$D$8</f>
-        <v>9</v>
+        <f>utilities!$J$8</f>
+        <v>0</v>
       </c>
       <c r="E15">
-        <v>10</v>
-      </c>
-      <c r="F15" s="4">
-        <f>utilities!$B$11</f>
-        <v>0.69444444444444453</v>
-      </c>
-      <c r="G15" s="4">
-        <f>utilities!$C$11</f>
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="H15" s="4">
-        <f>utilities!$D$11</f>
-        <v>0.16666666666666666</v>
+        <v>0</v>
+      </c>
+      <c r="F15" s="4" t="e">
+        <f>utilities!$H$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G15" s="4" t="e">
+        <f>utilities!$I$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H15" s="4" t="e">
+        <f>utilities!$J$11</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="I15" s="9">
-        <f>utilities!$E$11</f>
+        <f>utilities!$K$11</f>
         <v>1E-3</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B16">
-        <f>utilities!$B$8</f>
-        <v>6</v>
+        <f>utilities!$H$8</f>
+        <v>0</v>
       </c>
       <c r="C16">
-        <f>utilities!$C$8</f>
-        <v>8</v>
+        <f>utilities!$I$8</f>
+        <v>0</v>
       </c>
       <c r="D16">
-        <f>utilities!$D$8</f>
-        <v>9</v>
+        <f>utilities!$J$8</f>
+        <v>0</v>
       </c>
       <c r="E16">
-        <v>10</v>
-      </c>
-      <c r="F16" s="4">
-        <f>utilities!$B$11</f>
-        <v>0.69444444444444453</v>
-      </c>
-      <c r="G16" s="4">
-        <f>utilities!$C$11</f>
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="H16" s="4">
-        <f>utilities!$D$11</f>
-        <v>0.16666666666666666</v>
+        <v>0</v>
+      </c>
+      <c r="F16" s="4" t="e">
+        <f>utilities!$H$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G16" s="4" t="e">
+        <f>utilities!$I$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H16" s="4" t="e">
+        <f>utilities!$J$11</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="I16" s="9">
-        <f>utilities!$E$11</f>
+        <f>utilities!$K$11</f>
         <v>1E-3</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="B17">
-        <f>utilities!$B$8</f>
-        <v>6</v>
+        <f>utilities!$H$8</f>
+        <v>0</v>
       </c>
       <c r="C17">
-        <f>utilities!$C$8</f>
-        <v>8</v>
+        <f>utilities!$I$8</f>
+        <v>0</v>
       </c>
       <c r="D17">
-        <f>utilities!$D$8</f>
-        <v>9</v>
+        <f>utilities!$J$8</f>
+        <v>0</v>
       </c>
       <c r="E17">
-        <v>10</v>
-      </c>
-      <c r="F17" s="4">
-        <f>utilities!$B$11</f>
-        <v>0.69444444444444453</v>
-      </c>
-      <c r="G17" s="4">
-        <f>utilities!$C$11</f>
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="H17" s="4">
-        <f>utilities!$D$11</f>
-        <v>0.16666666666666666</v>
+        <v>0</v>
+      </c>
+      <c r="F17" s="4" t="e">
+        <f>utilities!$H$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G17" s="4" t="e">
+        <f>utilities!$I$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H17" s="4" t="e">
+        <f>utilities!$J$11</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="I17" s="9">
-        <f>utilities!$E$11</f>
+        <f>utilities!$K$11</f>
         <v>1E-3</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="B18">
-        <f>utilities!$B$8</f>
-        <v>6</v>
+        <f>utilities!$H$8</f>
+        <v>0</v>
       </c>
       <c r="C18">
-        <f>utilities!$C$8</f>
-        <v>8</v>
+        <f>utilities!$I$8</f>
+        <v>0</v>
       </c>
       <c r="D18">
-        <f>utilities!$D$8</f>
-        <v>9</v>
+        <f>utilities!$J$8</f>
+        <v>0</v>
       </c>
       <c r="E18">
-        <v>10</v>
-      </c>
-      <c r="F18" s="4">
-        <f>utilities!$B$11</f>
-        <v>0.69444444444444453</v>
-      </c>
-      <c r="G18" s="4">
-        <f>utilities!$C$11</f>
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="H18" s="4">
-        <f>utilities!$D$11</f>
-        <v>0.16666666666666666</v>
+        <v>0</v>
+      </c>
+      <c r="F18" s="4" t="e">
+        <f>utilities!$H$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G18" s="4" t="e">
+        <f>utilities!$I$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H18" s="4" t="e">
+        <f>utilities!$J$11</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="I18" s="9">
-        <f>utilities!$E$11</f>
+        <f>utilities!$K$11</f>
         <v>1E-3</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="B19">
-        <f>utilities!$B$8</f>
-        <v>6</v>
+        <f>utilities!$H$8</f>
+        <v>0</v>
       </c>
       <c r="C19">
-        <f>utilities!$C$8</f>
-        <v>8</v>
+        <f>utilities!$I$8</f>
+        <v>0</v>
       </c>
       <c r="D19">
-        <f>utilities!$D$8</f>
-        <v>9</v>
+        <f>utilities!$J$8</f>
+        <v>0</v>
       </c>
       <c r="E19">
-        <v>10</v>
-      </c>
-      <c r="F19" s="4">
-        <f>utilities!$B$11</f>
-        <v>0.69444444444444453</v>
-      </c>
-      <c r="G19" s="4">
-        <f>utilities!$C$11</f>
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="H19" s="4">
-        <f>utilities!$D$11</f>
-        <v>0.16666666666666666</v>
+        <v>0</v>
+      </c>
+      <c r="F19" s="4" t="e">
+        <f>utilities!$H$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G19" s="4" t="e">
+        <f>utilities!$I$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H19" s="4" t="e">
+        <f>utilities!$J$11</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="I19" s="9">
-        <f>utilities!$E$11</f>
+        <f>utilities!$K$11</f>
         <v>1E-3</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="B20">
-        <f>utilities!$B$8</f>
-        <v>6</v>
+        <f>utilities!$H$8</f>
+        <v>0</v>
       </c>
       <c r="C20">
-        <f>utilities!$C$8</f>
-        <v>8</v>
+        <f>utilities!$I$8</f>
+        <v>0</v>
       </c>
       <c r="D20">
-        <f>utilities!$D$8</f>
-        <v>9</v>
+        <f>utilities!$J$8</f>
+        <v>0</v>
       </c>
       <c r="E20">
-        <v>10</v>
-      </c>
-      <c r="F20" s="4">
-        <f>utilities!$B$11</f>
-        <v>0.69444444444444453</v>
-      </c>
-      <c r="G20" s="4">
-        <f>utilities!$C$11</f>
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="H20" s="4">
-        <f>utilities!$D$11</f>
-        <v>0.16666666666666666</v>
+        <v>0</v>
+      </c>
+      <c r="F20" s="4" t="e">
+        <f>utilities!$H$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G20" s="4" t="e">
+        <f>utilities!$I$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H20" s="4" t="e">
+        <f>utilities!$J$11</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="I20" s="9">
-        <f>utilities!$E$11</f>
+        <f>utilities!$K$11</f>
         <v>1E-3</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B21">
-        <f>utilities!$B$8</f>
-        <v>6</v>
+        <f>utilities!$H$8</f>
+        <v>0</v>
       </c>
       <c r="C21">
-        <f>utilities!$C$8</f>
-        <v>8</v>
+        <f>utilities!$I$8</f>
+        <v>0</v>
       </c>
       <c r="D21">
-        <f>utilities!$D$8</f>
-        <v>9</v>
+        <f>utilities!$J$8</f>
+        <v>0</v>
       </c>
       <c r="E21">
-        <v>10</v>
-      </c>
-      <c r="F21" s="4">
-        <f>utilities!$B$11</f>
-        <v>0.69444444444444453</v>
-      </c>
-      <c r="G21" s="4">
-        <f>utilities!$C$11</f>
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="H21" s="4">
-        <f>utilities!$D$11</f>
-        <v>0.16666666666666666</v>
+        <v>0</v>
+      </c>
+      <c r="F21" s="4" t="e">
+        <f>utilities!$H$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G21" s="4" t="e">
+        <f>utilities!$I$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H21" s="4" t="e">
+        <f>utilities!$J$11</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="I21" s="9">
-        <f>utilities!$E$11</f>
+        <f>utilities!$K$11</f>
         <v>1E-3</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="B22">
-        <f>utilities!$B$8</f>
-        <v>6</v>
+        <f>utilities!$H$8</f>
+        <v>0</v>
       </c>
       <c r="C22">
-        <f>utilities!$C$8</f>
-        <v>8</v>
+        <f>utilities!$I$8</f>
+        <v>0</v>
       </c>
       <c r="D22">
-        <f>utilities!$D$8</f>
-        <v>9</v>
+        <f>utilities!$J$8</f>
+        <v>0</v>
       </c>
       <c r="E22">
-        <v>10</v>
-      </c>
-      <c r="F22" s="4">
-        <f>utilities!$B$11</f>
-        <v>0.69444444444444453</v>
-      </c>
-      <c r="G22" s="4">
-        <f>utilities!$C$11</f>
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="H22" s="4">
-        <f>utilities!$D$11</f>
-        <v>0.16666666666666666</v>
+        <v>0</v>
+      </c>
+      <c r="F22" s="4" t="e">
+        <f>utilities!$H$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G22" s="4" t="e">
+        <f>utilities!$I$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H22" s="4" t="e">
+        <f>utilities!$J$11</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="I22" s="9">
-        <f>utilities!$E$11</f>
+        <f>utilities!$K$11</f>
         <v>1E-3</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="B23">
         <f>utilities!$H$8</f>
@@ -1374,7 +1393,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="B24">
         <f>utilities!$H$8</f>
@@ -1410,7 +1429,7 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="B25">
         <f>utilities!$H$8</f>
@@ -1446,7 +1465,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="B26">
         <f>utilities!$H$8</f>
@@ -1482,7 +1501,7 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="B27">
         <f>utilities!$H$8</f>
@@ -1518,7 +1537,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="B28">
         <f>utilities!$H$8</f>
@@ -1554,7 +1573,7 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="B29">
         <f>utilities!$H$8</f>
@@ -1590,7 +1609,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="B30">
         <f>utilities!$H$8</f>
@@ -1626,7 +1645,7 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="B31">
         <f>utilities!$H$8</f>
@@ -1662,7 +1681,7 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="B32">
         <f>utilities!$H$8</f>
@@ -1698,7 +1717,7 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="B33">
         <f>utilities!$H$8</f>
@@ -1734,7 +1753,7 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="B34">
         <f>utilities!$H$8</f>
@@ -1764,294 +1783,6 @@
         <v>#DIV/0!</v>
       </c>
       <c r="I34" s="9">
-        <f>utilities!$K$11</f>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>33</v>
-      </c>
-      <c r="B35">
-        <f>utilities!$H$8</f>
-        <v>0</v>
-      </c>
-      <c r="C35">
-        <f>utilities!$I$8</f>
-        <v>0</v>
-      </c>
-      <c r="D35">
-        <f>utilities!$J$8</f>
-        <v>0</v>
-      </c>
-      <c r="E35">
-        <v>0</v>
-      </c>
-      <c r="F35" s="4" t="e">
-        <f>utilities!$H$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G35" s="4" t="e">
-        <f>utilities!$I$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H35" s="4" t="e">
-        <f>utilities!$J$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I35" s="9">
-        <f>utilities!$K$11</f>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>34</v>
-      </c>
-      <c r="B36">
-        <f>utilities!$H$8</f>
-        <v>0</v>
-      </c>
-      <c r="C36">
-        <f>utilities!$I$8</f>
-        <v>0</v>
-      </c>
-      <c r="D36">
-        <f>utilities!$J$8</f>
-        <v>0</v>
-      </c>
-      <c r="E36">
-        <v>0</v>
-      </c>
-      <c r="F36" s="4" t="e">
-        <f>utilities!$H$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G36" s="4" t="e">
-        <f>utilities!$I$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H36" s="4" t="e">
-        <f>utilities!$J$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I36" s="9">
-        <f>utilities!$K$11</f>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>35</v>
-      </c>
-      <c r="B37">
-        <f>utilities!$H$8</f>
-        <v>0</v>
-      </c>
-      <c r="C37">
-        <f>utilities!$I$8</f>
-        <v>0</v>
-      </c>
-      <c r="D37">
-        <f>utilities!$J$8</f>
-        <v>0</v>
-      </c>
-      <c r="E37">
-        <v>0</v>
-      </c>
-      <c r="F37" s="4" t="e">
-        <f>utilities!$H$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G37" s="4" t="e">
-        <f>utilities!$I$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H37" s="4" t="e">
-        <f>utilities!$J$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I37" s="9">
-        <f>utilities!$K$11</f>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>36</v>
-      </c>
-      <c r="B38">
-        <f>utilities!$H$8</f>
-        <v>0</v>
-      </c>
-      <c r="C38">
-        <f>utilities!$I$8</f>
-        <v>0</v>
-      </c>
-      <c r="D38">
-        <f>utilities!$J$8</f>
-        <v>0</v>
-      </c>
-      <c r="E38">
-        <v>0</v>
-      </c>
-      <c r="F38" s="4" t="e">
-        <f>utilities!$H$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G38" s="4" t="e">
-        <f>utilities!$I$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H38" s="4" t="e">
-        <f>utilities!$J$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I38" s="9">
-        <f>utilities!$K$11</f>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>37</v>
-      </c>
-      <c r="B39">
-        <f>utilities!$H$8</f>
-        <v>0</v>
-      </c>
-      <c r="C39">
-        <f>utilities!$I$8</f>
-        <v>0</v>
-      </c>
-      <c r="D39">
-        <f>utilities!$J$8</f>
-        <v>0</v>
-      </c>
-      <c r="E39">
-        <v>0</v>
-      </c>
-      <c r="F39" s="4" t="e">
-        <f>utilities!$H$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G39" s="4" t="e">
-        <f>utilities!$I$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H39" s="4" t="e">
-        <f>utilities!$J$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I39" s="9">
-        <f>utilities!$K$11</f>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>38</v>
-      </c>
-      <c r="B40">
-        <f>utilities!$H$8</f>
-        <v>0</v>
-      </c>
-      <c r="C40">
-        <f>utilities!$I$8</f>
-        <v>0</v>
-      </c>
-      <c r="D40">
-        <f>utilities!$J$8</f>
-        <v>0</v>
-      </c>
-      <c r="E40">
-        <v>0</v>
-      </c>
-      <c r="F40" s="4" t="e">
-        <f>utilities!$H$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G40" s="4" t="e">
-        <f>utilities!$I$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H40" s="4" t="e">
-        <f>utilities!$J$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I40" s="9">
-        <f>utilities!$K$11</f>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>39</v>
-      </c>
-      <c r="B41">
-        <f>utilities!$H$8</f>
-        <v>0</v>
-      </c>
-      <c r="C41">
-        <f>utilities!$I$8</f>
-        <v>0</v>
-      </c>
-      <c r="D41">
-        <f>utilities!$J$8</f>
-        <v>0</v>
-      </c>
-      <c r="E41">
-        <v>0</v>
-      </c>
-      <c r="F41" s="4" t="e">
-        <f>utilities!$H$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G41" s="4" t="e">
-        <f>utilities!$I$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H41" s="4" t="e">
-        <f>utilities!$J$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I41" s="9">
-        <f>utilities!$K$11</f>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>40</v>
-      </c>
-      <c r="B42">
-        <f>utilities!$H$8</f>
-        <v>0</v>
-      </c>
-      <c r="C42">
-        <f>utilities!$I$8</f>
-        <v>0</v>
-      </c>
-      <c r="D42">
-        <f>utilities!$J$8</f>
-        <v>0</v>
-      </c>
-      <c r="E42">
-        <v>0</v>
-      </c>
-      <c r="F42" s="4" t="e">
-        <f>utilities!$H$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G42" s="4" t="e">
-        <f>utilities!$I$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H42" s="4" t="e">
-        <f>utilities!$J$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I42" s="9">
         <f>utilities!$K$11</f>
         <v>1E-3</v>
       </c>
@@ -2062,17 +1793,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FDEC06F-4DC9-4E7F-88C9-C6F486A3E573}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67C203FD-C9AE-45F0-8773-EECC728085CE}">
   <dimension ref="A1:I42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection sqref="A1:I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="6" max="6" width="16.7109375" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="9"/>
+    <col min="9" max="9" width="8.7109375" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -2110,22 +1841,22 @@
       </c>
       <c r="B2">
         <f>utilities!$B$8</f>
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C2">
         <f>utilities!$C$8</f>
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="D2">
         <f>utilities!$D$8</f>
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2" s="4">
         <f>utilities!$B$11</f>
-        <v>0.69444444444444453</v>
+        <v>0.69444444444444442</v>
       </c>
       <c r="G2" s="4">
         <f>utilities!$C$11</f>
@@ -2146,22 +1877,22 @@
       </c>
       <c r="B3">
         <f>utilities!$B$8</f>
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C3">
         <f>utilities!$C$8</f>
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="D3">
         <f>utilities!$D$8</f>
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="E3">
         <v>10</v>
       </c>
       <c r="F3" s="4">
         <f>utilities!$B$11</f>
-        <v>0.69444444444444453</v>
+        <v>0.69444444444444442</v>
       </c>
       <c r="G3" s="4">
         <f>utilities!$C$11</f>
@@ -2182,22 +1913,22 @@
       </c>
       <c r="B4">
         <f>utilities!$B$8</f>
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C4">
         <f>utilities!$C$8</f>
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="D4">
         <f>utilities!$D$8</f>
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="E4">
         <v>10</v>
       </c>
       <c r="F4" s="4">
         <f>utilities!$B$11</f>
-        <v>0.69444444444444453</v>
+        <v>0.69444444444444442</v>
       </c>
       <c r="G4" s="4">
         <f>utilities!$C$11</f>
@@ -2218,22 +1949,22 @@
       </c>
       <c r="B5">
         <f>utilities!$B$8</f>
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C5">
         <f>utilities!$C$8</f>
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="D5">
         <f>utilities!$D$8</f>
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="E5">
         <v>10</v>
       </c>
       <c r="F5" s="4">
         <f>utilities!$B$11</f>
-        <v>0.69444444444444453</v>
+        <v>0.69444444444444442</v>
       </c>
       <c r="G5" s="4">
         <f>utilities!$C$11</f>
@@ -2254,22 +1985,22 @@
       </c>
       <c r="B6">
         <f>utilities!$B$8</f>
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C6">
         <f>utilities!$C$8</f>
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="D6">
         <f>utilities!$D$8</f>
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="E6">
         <v>10</v>
       </c>
       <c r="F6" s="4">
         <f>utilities!$B$11</f>
-        <v>0.69444444444444453</v>
+        <v>0.69444444444444442</v>
       </c>
       <c r="G6" s="4">
         <f>utilities!$C$11</f>
@@ -2290,22 +2021,22 @@
       </c>
       <c r="B7">
         <f>utilities!$B$8</f>
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C7">
         <f>utilities!$C$8</f>
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="D7">
         <f>utilities!$D$8</f>
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="E7">
         <v>10</v>
       </c>
       <c r="F7" s="4">
         <f>utilities!$B$11</f>
-        <v>0.69444444444444453</v>
+        <v>0.69444444444444442</v>
       </c>
       <c r="G7" s="4">
         <f>utilities!$C$11</f>
@@ -2326,30 +2057,30 @@
       </c>
       <c r="B8">
         <f>utilities!$N$8</f>
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="C8">
         <f>utilities!$O$8</f>
-        <v>98</v>
+        <v>114</v>
       </c>
       <c r="D8">
         <f>utilities!$P$8</f>
-        <v>109</v>
+        <v>127</v>
       </c>
       <c r="E8">
         <v>10</v>
       </c>
       <c r="F8" s="4">
         <f>utilities!N11</f>
-        <v>0.46875</v>
+        <v>0.3860294117647059</v>
       </c>
       <c r="G8" s="4">
         <f>utilities!O11</f>
-        <v>0.125</v>
+        <v>0.11413043478260869</v>
       </c>
       <c r="H8" s="4">
         <f>utilities!P11</f>
-        <v>9.5454545454545459E-2</v>
+        <v>8.0769230769230774E-2</v>
       </c>
       <c r="I8" s="9">
         <f>utilities!$E$11</f>
@@ -2362,22 +2093,22 @@
       </c>
       <c r="B9">
         <f>utilities!$B$8</f>
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C9">
         <f>utilities!$C$8</f>
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="D9">
         <f>utilities!$D$8</f>
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="E9">
         <v>10</v>
       </c>
       <c r="F9" s="4">
         <f>utilities!$B$11</f>
-        <v>0.69444444444444453</v>
+        <v>0.69444444444444442</v>
       </c>
       <c r="G9" s="4">
         <f>utilities!$C$11</f>
@@ -2398,22 +2129,22 @@
       </c>
       <c r="B10">
         <f>utilities!$B$8</f>
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C10">
         <f>utilities!$C$8</f>
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="D10">
         <f>utilities!$D$8</f>
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="E10">
         <v>10</v>
       </c>
       <c r="F10" s="4">
         <f>utilities!$B$11</f>
-        <v>0.69444444444444453</v>
+        <v>0.69444444444444442</v>
       </c>
       <c r="G10" s="4">
         <f>utilities!$C$11</f>
@@ -2434,22 +2165,22 @@
       </c>
       <c r="B11">
         <f>utilities!$B$8</f>
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C11">
         <f>utilities!$C$8</f>
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="D11">
         <f>utilities!$D$8</f>
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="E11">
         <v>10</v>
       </c>
       <c r="F11" s="4">
         <f>utilities!$B$11</f>
-        <v>0.69444444444444453</v>
+        <v>0.69444444444444442</v>
       </c>
       <c r="G11" s="4">
         <f>utilities!$C$11</f>
@@ -2470,22 +2201,22 @@
       </c>
       <c r="B12">
         <f>utilities!$B$8</f>
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C12">
         <f>utilities!$C$8</f>
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="D12">
         <f>utilities!$D$8</f>
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="E12">
         <v>10</v>
       </c>
       <c r="F12" s="4">
         <f>utilities!$B$11</f>
-        <v>0.69444444444444453</v>
+        <v>0.69444444444444442</v>
       </c>
       <c r="G12" s="4">
         <f>utilities!$C$11</f>
@@ -2506,22 +2237,22 @@
       </c>
       <c r="B13">
         <f>utilities!$B$8</f>
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C13">
         <f>utilities!$C$8</f>
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="D13">
         <f>utilities!$D$8</f>
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="E13">
         <v>10</v>
       </c>
       <c r="F13" s="4">
         <f>utilities!$B$11</f>
-        <v>0.69444444444444453</v>
+        <v>0.69444444444444442</v>
       </c>
       <c r="G13" s="4">
         <f>utilities!$C$11</f>
@@ -2542,30 +2273,30 @@
       </c>
       <c r="B14">
         <f>utilities!T8</f>
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="C14">
         <f>utilities!U8</f>
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="D14">
         <f>utilities!V8</f>
-        <v>159</v>
+        <v>168</v>
       </c>
       <c r="E14">
         <v>10</v>
       </c>
       <c r="F14" s="4">
         <f>utilities!T11</f>
-        <v>0.32407407407407407</v>
+        <v>0.30172413793103448</v>
       </c>
       <c r="G14" s="4">
         <f>utilities!U11</f>
-        <v>8.4677419354838704E-2</v>
+        <v>8.203125E-2</v>
       </c>
       <c r="H14" s="4">
         <f>utilities!V11</f>
-        <v>6.5625000000000003E-2</v>
+        <v>6.1764705882352944E-2</v>
       </c>
       <c r="I14" s="9">
         <f>utilities!$E$11</f>
@@ -2578,22 +2309,22 @@
       </c>
       <c r="B15">
         <f>utilities!$B$8</f>
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C15">
         <f>utilities!$C$8</f>
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="D15">
         <f>utilities!$D$8</f>
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="E15">
         <v>10</v>
       </c>
       <c r="F15" s="4">
         <f>utilities!$B$11</f>
-        <v>0.69444444444444453</v>
+        <v>0.69444444444444442</v>
       </c>
       <c r="G15" s="4">
         <f>utilities!$C$11</f>
@@ -2614,22 +2345,22 @@
       </c>
       <c r="B16">
         <f>utilities!$B$8</f>
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C16">
         <f>utilities!$C$8</f>
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="D16">
         <f>utilities!$D$8</f>
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="E16">
         <v>10</v>
       </c>
       <c r="F16" s="4">
         <f>utilities!$B$11</f>
-        <v>0.69444444444444453</v>
+        <v>0.69444444444444442</v>
       </c>
       <c r="G16" s="4">
         <f>utilities!$C$11</f>
@@ -2650,22 +2381,22 @@
       </c>
       <c r="B17">
         <f>utilities!$B$8</f>
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C17">
         <f>utilities!$C$8</f>
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="D17">
         <f>utilities!$D$8</f>
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="E17">
         <v>10</v>
       </c>
       <c r="F17" s="4">
         <f>utilities!$B$11</f>
-        <v>0.69444444444444453</v>
+        <v>0.69444444444444442</v>
       </c>
       <c r="G17" s="4">
         <f>utilities!$C$11</f>
@@ -2686,22 +2417,22 @@
       </c>
       <c r="B18">
         <f>utilities!$B$8</f>
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C18">
         <f>utilities!$C$8</f>
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="D18">
         <f>utilities!$D$8</f>
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="E18">
         <v>10</v>
       </c>
       <c r="F18" s="4">
         <f>utilities!$B$11</f>
-        <v>0.69444444444444453</v>
+        <v>0.69444444444444442</v>
       </c>
       <c r="G18" s="4">
         <f>utilities!$C$11</f>
@@ -2722,22 +2453,22 @@
       </c>
       <c r="B19">
         <f>utilities!$B$8</f>
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C19">
         <f>utilities!$C$8</f>
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="D19">
         <f>utilities!$D$8</f>
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="E19">
         <v>10</v>
       </c>
       <c r="F19" s="4">
         <f>utilities!$B$11</f>
-        <v>0.69444444444444453</v>
+        <v>0.69444444444444442</v>
       </c>
       <c r="G19" s="4">
         <f>utilities!$C$11</f>
@@ -2758,22 +2489,22 @@
       </c>
       <c r="B20">
         <f>utilities!$B$8</f>
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C20">
         <f>utilities!$C$8</f>
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="D20">
         <f>utilities!$D$8</f>
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="E20">
         <v>10</v>
       </c>
       <c r="F20" s="4">
         <f>utilities!$B$11</f>
-        <v>0.69444444444444453</v>
+        <v>0.69444444444444442</v>
       </c>
       <c r="G20" s="4">
         <f>utilities!$C$11</f>
@@ -2794,22 +2525,22 @@
       </c>
       <c r="B21">
         <f>utilities!$B$8</f>
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C21">
         <f>utilities!$C$8</f>
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="D21">
         <f>utilities!$D$8</f>
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="E21">
         <v>10</v>
       </c>
       <c r="F21" s="4">
         <f>utilities!$B$11</f>
-        <v>0.69444444444444453</v>
+        <v>0.69444444444444442</v>
       </c>
       <c r="G21" s="4">
         <f>utilities!$C$11</f>
@@ -2830,22 +2561,22 @@
       </c>
       <c r="B22">
         <f>utilities!$B$8</f>
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C22">
         <f>utilities!$C$8</f>
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="D22">
         <f>utilities!$D$8</f>
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="E22">
         <v>10</v>
       </c>
       <c r="F22" s="4">
         <f>utilities!$B$11</f>
-        <v>0.69444444444444453</v>
+        <v>0.69444444444444442</v>
       </c>
       <c r="G22" s="4">
         <f>utilities!$C$11</f>
@@ -3587,10 +3318,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{117A8B26-635D-4B40-A90B-7735D1F1002F}">
-  <dimension ref="A1:W21"/>
+  <dimension ref="A1:W33"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="V9" sqref="V9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3653,7 +3384,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>17</v>
       </c>
@@ -3703,18 +3434,21 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
       <c r="B8">
-        <v>6</v>
+        <f>6*3</f>
+        <v>18</v>
       </c>
       <c r="C8">
-        <v>8</v>
+        <f>8*3</f>
+        <v>24</v>
       </c>
       <c r="D8">
-        <v>9</v>
+        <f>9*3</f>
+        <v>27</v>
       </c>
       <c r="G8" t="s">
         <v>14</v>
@@ -3733,28 +3467,27 @@
       </c>
       <c r="N8">
         <f>50+B8</f>
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="O8">
-        <v>98</v>
+        <f>90+C8</f>
+        <v>114</v>
       </c>
       <c r="P8">
-        <v>109</v>
+        <f>100+D8</f>
+        <v>127</v>
       </c>
       <c r="S8" t="s">
         <v>14</v>
       </c>
-      <c r="T8">
-        <f>75+B8</f>
-        <v>81</v>
-      </c>
-      <c r="U8">
-        <f>135+C8</f>
-        <v>143</v>
-      </c>
-      <c r="V8">
-        <f>150+D8</f>
-        <v>159</v>
+      <c r="T8" s="12">
+        <v>87</v>
+      </c>
+      <c r="U8" s="12">
+        <v>151</v>
+      </c>
+      <c r="V8" s="12">
+        <v>168</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
@@ -3789,15 +3522,15 @@
       </c>
       <c r="B10" s="3">
         <f>A3/$B$12*B$9</f>
-        <v>4.166666666666667</v>
+        <v>12.5</v>
       </c>
       <c r="C10" s="3">
         <f>B3/$B$12*B9</f>
-        <v>0.83333333333333337</v>
+        <v>2.5</v>
       </c>
       <c r="D10" s="3">
         <f>C3/$B$12*B9</f>
-        <v>0.16666666666666666</v>
+        <v>0.5</v>
       </c>
       <c r="E10" s="6">
         <f>D3</f>
@@ -3867,7 +3600,7 @@
       </c>
       <c r="B11" s="4">
         <f>B10/B8</f>
-        <v>0.69444444444444453</v>
+        <v>0.69444444444444442</v>
       </c>
       <c r="C11" s="7">
         <f>C10/(C8-B8)</f>
@@ -3905,15 +3638,15 @@
       </c>
       <c r="N11" s="4">
         <f>N10/N8</f>
-        <v>0.46875</v>
+        <v>0.3860294117647059</v>
       </c>
       <c r="O11" s="7">
         <f>O10/(O8-N8)</f>
-        <v>0.125</v>
+        <v>0.11413043478260869</v>
       </c>
       <c r="P11" s="7">
         <f>P10/(P8-O8)</f>
-        <v>9.5454545454545459E-2</v>
+        <v>8.0769230769230774E-2</v>
       </c>
       <c r="Q11" s="9">
         <f>Q10</f>
@@ -3924,15 +3657,15 @@
       </c>
       <c r="T11" s="4">
         <f>T10/T8</f>
-        <v>0.32407407407407407</v>
+        <v>0.30172413793103448</v>
       </c>
       <c r="U11" s="7">
         <f>U10/(U8-T8)</f>
-        <v>8.4677419354838704E-2</v>
+        <v>8.203125E-2</v>
       </c>
       <c r="V11" s="7">
         <f>V10/(V8-U8)</f>
-        <v>6.5625000000000003E-2</v>
+        <v>6.1764705882352944E-2</v>
       </c>
       <c r="W11" s="9">
         <f>W10</f>
@@ -3945,7 +3678,7 @@
       </c>
       <c r="B12">
         <f>B14-B13+1</f>
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="G12" t="s">
         <v>18</v>
@@ -3986,13 +3719,13 @@
         <v>20</v>
       </c>
       <c r="N13">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="S13" t="s">
         <v>20</v>
       </c>
       <c r="T13">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
@@ -4000,7 +3733,7 @@
         <v>21</v>
       </c>
       <c r="B14">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C14" s="7"/>
       <c r="G14" t="s">
@@ -4013,13 +3746,13 @@
         <v>21</v>
       </c>
       <c r="N14">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="S14" t="s">
         <v>21</v>
       </c>
       <c r="T14">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
@@ -4028,7 +3761,7 @@
       </c>
       <c r="E15" s="4">
         <f>SUM(B10:E10)*B12</f>
-        <v>62.012000000000008</v>
+        <v>62.003999999999998</v>
       </c>
       <c r="G15" t="s">
         <v>24</v>
@@ -4052,20 +3785,399 @@
         <v>32.550999999999995</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B17" s="7">
         <f>E15+Q15+W15</f>
+        <v>127.10599999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B18" s="7"/>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>27</v>
+      </c>
+      <c r="P21" s="10"/>
+    </row>
+    <row r="22" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M22" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="S22" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E23" t="s">
+        <v>19</v>
+      </c>
+      <c r="H23" t="s">
+        <v>17</v>
+      </c>
+      <c r="I23" t="s">
+        <v>12</v>
+      </c>
+      <c r="J23" t="s">
+        <v>13</v>
+      </c>
+      <c r="K23" t="s">
+        <v>19</v>
+      </c>
+      <c r="N23" t="s">
+        <v>17</v>
+      </c>
+      <c r="O23" t="s">
+        <v>12</v>
+      </c>
+      <c r="P23" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>19</v>
+      </c>
+      <c r="T23" t="s">
+        <v>17</v>
+      </c>
+      <c r="U23" t="s">
+        <v>12</v>
+      </c>
+      <c r="V23" t="s">
+        <v>13</v>
+      </c>
+      <c r="W23" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24">
+        <v>6</v>
+      </c>
+      <c r="C24">
+        <v>8</v>
+      </c>
+      <c r="D24">
+        <v>9</v>
+      </c>
+      <c r="G24" t="s">
+        <v>14</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="M24" t="s">
+        <v>14</v>
+      </c>
+      <c r="N24">
+        <v>56</v>
+      </c>
+      <c r="O24">
+        <v>98</v>
+      </c>
+      <c r="P24">
+        <v>109</v>
+      </c>
+      <c r="S24" t="s">
+        <v>14</v>
+      </c>
+      <c r="T24">
+        <v>81</v>
+      </c>
+      <c r="U24">
+        <v>143</v>
+      </c>
+      <c r="V24">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25">
+        <v>2</v>
+      </c>
+      <c r="G25" t="s">
+        <v>25</v>
+      </c>
+      <c r="H25">
+        <v>1</v>
+      </c>
+      <c r="M25" t="s">
+        <v>25</v>
+      </c>
+      <c r="N25">
+        <v>1</v>
+      </c>
+      <c r="S25" t="s">
+        <v>25</v>
+      </c>
+      <c r="T25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>22</v>
+      </c>
+      <c r="B26">
+        <v>4.166666666666667</v>
+      </c>
+      <c r="C26">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="D26">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="E26">
+        <v>1E-3</v>
+      </c>
+      <c r="G26" t="s">
+        <v>16</v>
+      </c>
+      <c r="H26">
+        <v>1.25</v>
+      </c>
+      <c r="I26">
+        <v>0.25</v>
+      </c>
+      <c r="J26">
+        <v>0.05</v>
+      </c>
+      <c r="K26">
+        <v>1E-3</v>
+      </c>
+      <c r="M26" t="s">
+        <v>16</v>
+      </c>
+      <c r="N26">
+        <v>26.25</v>
+      </c>
+      <c r="O26">
+        <v>5.25</v>
+      </c>
+      <c r="P26">
+        <v>1.05</v>
+      </c>
+      <c r="Q26">
+        <v>1E-3</v>
+      </c>
+      <c r="S26" t="s">
+        <v>16</v>
+      </c>
+      <c r="T26">
+        <v>26.25</v>
+      </c>
+      <c r="U26">
+        <v>5.25</v>
+      </c>
+      <c r="V26">
+        <v>1.05</v>
+      </c>
+      <c r="W26">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27">
+        <v>0.69444444444444453</v>
+      </c>
+      <c r="C27">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D27">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="E27">
+        <v>1E-3</v>
+      </c>
+      <c r="G27" t="s">
+        <v>15</v>
+      </c>
+      <c r="H27" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I27" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J27" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K27">
+        <v>1E-3</v>
+      </c>
+      <c r="M27" t="s">
+        <v>15</v>
+      </c>
+      <c r="N27">
+        <v>0.46875</v>
+      </c>
+      <c r="O27">
+        <v>0.125</v>
+      </c>
+      <c r="P27">
+        <v>9.5454545454545459E-2</v>
+      </c>
+      <c r="Q27">
+        <v>1E-3</v>
+      </c>
+      <c r="S27" t="s">
+        <v>15</v>
+      </c>
+      <c r="T27">
+        <v>0.32407407407407407</v>
+      </c>
+      <c r="U27">
+        <v>8.4677419354838704E-2</v>
+      </c>
+      <c r="V27">
+        <v>6.5625000000000003E-2</v>
+      </c>
+      <c r="W27">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>18</v>
+      </c>
+      <c r="B28">
+        <v>12</v>
+      </c>
+      <c r="G28" t="s">
+        <v>18</v>
+      </c>
+      <c r="H28">
+        <v>20</v>
+      </c>
+      <c r="M28" t="s">
+        <v>18</v>
+      </c>
+      <c r="N28">
+        <v>1</v>
+      </c>
+      <c r="S28" t="s">
+        <v>18</v>
+      </c>
+      <c r="T28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>20</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="G29" t="s">
+        <v>20</v>
+      </c>
+      <c r="H29">
+        <v>21</v>
+      </c>
+      <c r="M29" t="s">
+        <v>20</v>
+      </c>
+      <c r="N29">
+        <v>6</v>
+      </c>
+      <c r="S29" t="s">
+        <v>20</v>
+      </c>
+      <c r="T29">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>21</v>
+      </c>
+      <c r="B30">
+        <v>12</v>
+      </c>
+      <c r="G30" t="s">
+        <v>21</v>
+      </c>
+      <c r="H30">
+        <v>40</v>
+      </c>
+      <c r="M30" t="s">
+        <v>21</v>
+      </c>
+      <c r="N30">
+        <v>6</v>
+      </c>
+      <c r="S30" t="s">
+        <v>21</v>
+      </c>
+      <c r="T30">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>24</v>
+      </c>
+      <c r="E31">
+        <v>62.012000000000008</v>
+      </c>
+      <c r="G31" t="s">
+        <v>24</v>
+      </c>
+      <c r="K31">
+        <v>31.02</v>
+      </c>
+      <c r="M31" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q31">
+        <v>32.550999999999995</v>
+      </c>
+      <c r="S31" t="s">
+        <v>24</v>
+      </c>
+      <c r="W31">
+        <v>32.550999999999995</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>23</v>
+      </c>
+      <c r="B33">
         <v>127.114</v>
       </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B18" s="7"/>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="P21" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
sddp merton print html report
</commit_message>
<xml_diff>
--- a/julia_msp/goal_data.xlsx
+++ b/julia_msp/goal_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matsz\programowanie\Optymalizacja portfela\julia_msp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C1553553-A96B-4DCF-8C56-D44851FF15BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEBAE5D7-696C-4188-9AB1-C7CA2652F150}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E8CF1CA2-D953-46E5-99F4-DA96611E7E6D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{E8CF1CA2-D953-46E5-99F4-DA96611E7E6D}"/>
   </bookViews>
   <sheets>
     <sheet name="goal_data" sheetId="1" r:id="rId1"/>
@@ -569,7 +569,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FFE0B56-DF8B-44CF-9758-6EDE70A13051}">
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -3320,8 +3320,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{117A8B26-635D-4B40-A90B-7735D1F1002F}">
   <dimension ref="A1:W33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
sddp 25 vs 5 stages comparison
</commit_message>
<xml_diff>
--- a/julia_msp/goal_data.xlsx
+++ b/julia_msp/goal_data.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matsz\programowanie\Optymalizacja_portfela\julia_msp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D0D5803-A85A-46A6-BFA2-D7AF91DE9DAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2877D288-B80F-4CE6-A9CB-C45CC8837513}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E8CF1CA2-D953-46E5-99F4-DA96611E7E6D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{E8CF1CA2-D953-46E5-99F4-DA96611E7E6D}"/>
   </bookViews>
   <sheets>
-    <sheet name="goal_data" sheetId="4" r:id="rId1"/>
-    <sheet name="goal_data_5" sheetId="1" r:id="rId2"/>
+    <sheet name="goal_data_25" sheetId="4" r:id="rId1"/>
+    <sheet name="goal_data" sheetId="5" r:id="rId2"/>
     <sheet name="utilities" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="31">
   <si>
     <t>minimum_limit</t>
   </si>
@@ -122,6 +122,15 @@
   </si>
   <si>
     <t>S12</t>
+  </si>
+  <si>
+    <t>razem</t>
+  </si>
+  <si>
+    <t>years</t>
+  </si>
+  <si>
+    <t>cashflow desired</t>
   </si>
 </sst>
 </file>
@@ -212,7 +221,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -232,6 +241,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Dziesiętny" xfId="1" builtinId="3"/>
@@ -567,19 +578,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67C203FD-C9AE-45F0-8773-EECC728085CE}">
-  <dimension ref="A1:I42"/>
+  <dimension ref="A1:L43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12:H15"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="16.7109375" customWidth="1"/>
-    <col min="9" max="9" width="8.7109375" style="9"/>
+    <col min="7" max="7" width="16.7109375" customWidth="1"/>
+    <col min="10" max="10" width="8.7109375" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -595,994 +606,1013 @@
       <c r="E1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="J1" s="11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <f>utilities!$B$8</f>
         <v>6</v>
       </c>
       <c r="C2">
-        <f>utilities!$C$8</f>
         <v>8</v>
       </c>
       <c r="D2">
-        <f>utilities!$D$8</f>
         <v>9</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
-      <c r="F2" s="4">
-        <f>utilities!$B$11</f>
+      <c r="F2">
+        <f>1/25</f>
+        <v>0.04</v>
+      </c>
+      <c r="G2" s="4">
+        <f>(25*F2)/B2</f>
         <v>0.16666666666666666</v>
       </c>
-      <c r="G2" s="4">
-        <f>utilities!$C$11</f>
+      <c r="H2" s="4">
+        <f>(5*F2)/(C2-B2)</f>
         <v>0.1</v>
       </c>
-      <c r="H2" s="4">
-        <f>utilities!$D$11</f>
-        <v>0.04</v>
-      </c>
-      <c r="I2" s="9">
+      <c r="I2" s="4">
+        <f>(1*F2)/(D2-C2)</f>
+        <v>0.04</v>
+      </c>
+      <c r="J2" s="9">
         <f>utilities!$E$11</f>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <f>utilities!$B$8</f>
         <v>6</v>
       </c>
       <c r="C3">
-        <f>utilities!$C$8</f>
         <v>8</v>
       </c>
       <c r="D3">
-        <f>utilities!$D$8</f>
         <v>9</v>
       </c>
       <c r="E3">
         <v>11</v>
       </c>
-      <c r="F3" s="4">
-        <f>utilities!$B$11</f>
+      <c r="F3">
+        <f t="shared" ref="F3:F43" si="0">1/25</f>
+        <v>0.04</v>
+      </c>
+      <c r="G3" s="4">
+        <f t="shared" ref="G3:G27" si="1">(25*F3)/B3</f>
         <v>0.16666666666666666</v>
       </c>
-      <c r="G3" s="4">
-        <f>utilities!$C$11</f>
+      <c r="H3" s="4">
+        <f t="shared" ref="H3:H27" si="2">(5*F3)/(C3-B3)</f>
         <v>0.1</v>
       </c>
-      <c r="H3" s="4">
-        <f>utilities!$D$11</f>
-        <v>0.04</v>
-      </c>
-      <c r="I3" s="9">
+      <c r="I3" s="4">
+        <f t="shared" ref="I3:I27" si="3">(1*F3)/(D3-C3)</f>
+        <v>0.04</v>
+      </c>
+      <c r="J3" s="9">
         <f>utilities!$E$11</f>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
-        <f>utilities!$B$8</f>
         <v>6</v>
       </c>
       <c r="C4">
-        <f>utilities!$C$8</f>
         <v>8</v>
       </c>
       <c r="D4">
-        <f>utilities!$D$8</f>
         <v>9</v>
       </c>
       <c r="E4">
         <v>11</v>
       </c>
-      <c r="F4" s="4">
-        <f>utilities!$B$11</f>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="G4" s="4">
+        <f t="shared" si="1"/>
         <v>0.16666666666666666</v>
       </c>
-      <c r="G4" s="4">
-        <f>utilities!$C$11</f>
+      <c r="H4" s="4">
+        <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
-      <c r="H4" s="4">
-        <f>utilities!$D$11</f>
-        <v>0.04</v>
-      </c>
-      <c r="I4" s="9">
+      <c r="I4" s="4">
+        <f t="shared" si="3"/>
+        <v>0.04</v>
+      </c>
+      <c r="J4" s="9">
         <f>utilities!$E$11</f>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
-        <f>utilities!$B$8</f>
         <v>6</v>
       </c>
       <c r="C5">
-        <f>utilities!$C$8</f>
         <v>8</v>
       </c>
       <c r="D5">
-        <f>utilities!$D$8</f>
         <v>9</v>
       </c>
       <c r="E5">
         <v>11</v>
       </c>
-      <c r="F5" s="4">
-        <f>utilities!$B$11</f>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="G5" s="4">
+        <f t="shared" si="1"/>
         <v>0.16666666666666666</v>
       </c>
-      <c r="G5" s="4">
-        <f>utilities!$C$11</f>
+      <c r="H5" s="4">
+        <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
-      <c r="H5" s="4">
-        <f>utilities!$D$11</f>
-        <v>0.04</v>
-      </c>
-      <c r="I5" s="9">
+      <c r="I5" s="4">
+        <f t="shared" si="3"/>
+        <v>0.04</v>
+      </c>
+      <c r="J5" s="9">
         <f>utilities!$E$11</f>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
-        <f>utilities!$B$8</f>
         <v>6</v>
       </c>
       <c r="C6">
-        <f>utilities!$C$8</f>
         <v>8</v>
       </c>
       <c r="D6">
-        <f>utilities!$D$8</f>
         <v>9</v>
       </c>
       <c r="E6">
         <v>11</v>
       </c>
-      <c r="F6" s="4">
-        <f>utilities!$B$11</f>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="G6" s="4">
+        <f t="shared" si="1"/>
         <v>0.16666666666666666</v>
       </c>
-      <c r="G6" s="4">
-        <f>utilities!$C$11</f>
+      <c r="H6" s="4">
+        <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
-      <c r="H6" s="4">
-        <f>utilities!$D$11</f>
-        <v>0.04</v>
-      </c>
-      <c r="I6" s="9">
+      <c r="I6" s="4">
+        <f t="shared" si="3"/>
+        <v>0.04</v>
+      </c>
+      <c r="J6" s="9">
         <f>utilities!$E$11</f>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7">
-        <f>utilities!$B$8</f>
         <v>6</v>
       </c>
       <c r="C7">
-        <f>utilities!$C$8</f>
         <v>8</v>
       </c>
       <c r="D7">
-        <f>utilities!$D$8</f>
         <v>9</v>
       </c>
       <c r="E7">
         <v>11</v>
       </c>
-      <c r="F7" s="4">
-        <f>utilities!$B$11</f>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="G7" s="4">
+        <f t="shared" si="1"/>
         <v>0.16666666666666666</v>
       </c>
-      <c r="G7" s="4">
-        <f>utilities!$C$11</f>
+      <c r="H7" s="4">
+        <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
-      <c r="H7" s="4">
-        <f>utilities!$D$11</f>
-        <v>0.04</v>
-      </c>
-      <c r="I7" s="9">
+      <c r="I7" s="4">
+        <f t="shared" si="3"/>
+        <v>0.04</v>
+      </c>
+      <c r="J7" s="9">
         <f>utilities!$E$11</f>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8">
-        <f>utilities!$B$8</f>
         <v>6</v>
       </c>
       <c r="C8">
-        <f>utilities!$C$8</f>
         <v>8</v>
       </c>
       <c r="D8">
-        <f>utilities!$D$8</f>
         <v>9</v>
       </c>
       <c r="E8">
         <v>11</v>
       </c>
-      <c r="F8" s="4">
-        <f>utilities!$B$11</f>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="G8" s="4">
+        <f t="shared" si="1"/>
         <v>0.16666666666666666</v>
       </c>
-      <c r="G8" s="4">
-        <f>utilities!$C$11</f>
+      <c r="H8" s="4">
+        <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
-      <c r="H8" s="4">
-        <f>utilities!$D$11</f>
-        <v>0.04</v>
-      </c>
-      <c r="I8" s="9">
+      <c r="I8" s="4">
+        <f t="shared" si="3"/>
+        <v>0.04</v>
+      </c>
+      <c r="J8" s="9">
         <f>utilities!$E$11</f>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9">
-        <f>utilities!$B$8</f>
         <v>6</v>
       </c>
       <c r="C9">
-        <f>utilities!$C$8</f>
         <v>8</v>
       </c>
       <c r="D9">
-        <f>utilities!$D$8</f>
         <v>9</v>
       </c>
       <c r="E9">
         <v>11</v>
       </c>
-      <c r="F9" s="4">
-        <f>utilities!$B$11</f>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="G9" s="4">
+        <f t="shared" si="1"/>
         <v>0.16666666666666666</v>
       </c>
-      <c r="G9" s="4">
-        <f>utilities!$C$11</f>
+      <c r="H9" s="4">
+        <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
-      <c r="H9" s="4">
-        <f>utilities!$D$11</f>
-        <v>0.04</v>
-      </c>
-      <c r="I9" s="9">
+      <c r="I9" s="4">
+        <f t="shared" si="3"/>
+        <v>0.04</v>
+      </c>
+      <c r="J9" s="9">
         <f>utilities!$E$11</f>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10">
-        <f>utilities!$B$8</f>
         <v>6</v>
       </c>
       <c r="C10">
-        <f>utilities!$C$8</f>
         <v>8</v>
       </c>
       <c r="D10">
-        <f>utilities!$D$8</f>
         <v>9</v>
       </c>
       <c r="E10">
         <v>11</v>
       </c>
-      <c r="F10" s="4">
-        <f>utilities!$B$11</f>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="G10" s="4">
+        <f t="shared" si="1"/>
         <v>0.16666666666666666</v>
       </c>
-      <c r="G10" s="4">
-        <f>utilities!$C$11</f>
+      <c r="H10" s="4">
+        <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
-      <c r="H10" s="4">
-        <f>utilities!$D$11</f>
-        <v>0.04</v>
-      </c>
-      <c r="I10" s="9">
+      <c r="I10" s="4">
+        <f t="shared" si="3"/>
+        <v>0.04</v>
+      </c>
+      <c r="J10" s="9">
         <f>utilities!$E$11</f>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11">
-        <f>utilities!$N$8</f>
         <v>66</v>
       </c>
       <c r="C11">
-        <f>utilities!$O$8</f>
         <v>98</v>
       </c>
       <c r="D11">
-        <f>utilities!$P$8</f>
         <v>159</v>
       </c>
       <c r="E11">
         <v>11</v>
       </c>
-      <c r="F11" s="4">
-        <f>utilities!$N$11</f>
-        <v>0.39772727272727271</v>
+      <c r="F11">
+        <v>1</v>
       </c>
       <c r="G11" s="4">
-        <f>utilities!$O$11</f>
-        <v>0.1640625</v>
+        <f t="shared" si="1"/>
+        <v>0.37878787878787878</v>
       </c>
       <c r="H11" s="4">
-        <f>utilities!$P$11</f>
-        <v>1.7213114754098362E-2</v>
-      </c>
-      <c r="I11" s="9">
+        <f t="shared" si="2"/>
+        <v>0.15625</v>
+      </c>
+      <c r="I11" s="4">
+        <f t="shared" si="3"/>
+        <v>1.6393442622950821E-2</v>
+      </c>
+      <c r="J11" s="9">
         <f>utilities!$E$11</f>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12">
-        <f>utilities!$B$8</f>
         <v>6</v>
       </c>
       <c r="C12">
-        <f>utilities!$C$8</f>
         <v>8</v>
       </c>
       <c r="D12">
-        <f>utilities!$D$8</f>
         <v>9</v>
       </c>
       <c r="E12">
         <v>11</v>
       </c>
-      <c r="F12" s="4">
-        <f>utilities!$B$11</f>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="G12" s="4">
+        <f t="shared" si="1"/>
         <v>0.16666666666666666</v>
       </c>
-      <c r="G12" s="4">
-        <f>utilities!$C$11</f>
+      <c r="H12" s="4">
+        <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
-      <c r="H12" s="4">
-        <f>utilities!$D$11</f>
-        <v>0.04</v>
-      </c>
-      <c r="I12" s="9">
+      <c r="I12" s="4">
+        <f t="shared" si="3"/>
+        <v>0.04</v>
+      </c>
+      <c r="J12" s="9">
         <f>utilities!$E$11</f>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13">
-        <f>utilities!$B$8</f>
         <v>6</v>
       </c>
       <c r="C13">
-        <f>utilities!$C$8</f>
         <v>8</v>
       </c>
       <c r="D13">
-        <f>utilities!$D$8</f>
         <v>9</v>
       </c>
       <c r="E13">
         <v>11</v>
       </c>
-      <c r="F13" s="4">
-        <f>utilities!$B$11</f>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="G13" s="4">
+        <f t="shared" si="1"/>
         <v>0.16666666666666666</v>
       </c>
-      <c r="G13" s="4">
-        <f>utilities!$C$11</f>
+      <c r="H13" s="4">
+        <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
-      <c r="H13" s="4">
-        <f>utilities!$D$11</f>
-        <v>0.04</v>
-      </c>
-      <c r="I13" s="9">
+      <c r="I13" s="4">
+        <f t="shared" si="3"/>
+        <v>0.04</v>
+      </c>
+      <c r="J13" s="9">
         <f>utilities!$E$11</f>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14">
-        <f>utilities!$B$8</f>
         <v>6</v>
       </c>
       <c r="C14">
-        <f>utilities!$C$8</f>
         <v>8</v>
       </c>
       <c r="D14">
-        <f>utilities!$D$8</f>
         <v>9</v>
       </c>
       <c r="E14">
         <v>11</v>
       </c>
-      <c r="F14" s="4">
-        <f>utilities!$B$11</f>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="G14" s="4">
+        <f t="shared" si="1"/>
         <v>0.16666666666666666</v>
       </c>
-      <c r="G14" s="4">
-        <f>utilities!$C$11</f>
+      <c r="H14" s="4">
+        <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
-      <c r="H14" s="4">
-        <f>utilities!$D$11</f>
-        <v>0.04</v>
-      </c>
-      <c r="I14" s="9">
+      <c r="I14" s="4">
+        <f t="shared" si="3"/>
+        <v>0.04</v>
+      </c>
+      <c r="J14" s="9">
         <f>utilities!$E$11</f>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
       <c r="B15">
-        <f>utilities!$B$8</f>
         <v>6</v>
       </c>
       <c r="C15">
-        <f>utilities!$C$8</f>
         <v>8</v>
       </c>
       <c r="D15">
-        <f>utilities!$D$8</f>
         <v>9</v>
       </c>
       <c r="E15">
         <v>11</v>
       </c>
-      <c r="F15" s="4">
-        <f>utilities!$B$11</f>
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="G15" s="4">
+        <f t="shared" si="1"/>
         <v>0.16666666666666666</v>
       </c>
-      <c r="G15" s="4">
-        <f>utilities!$C$11</f>
+      <c r="H15" s="4">
+        <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
-      <c r="H15" s="4">
-        <f>utilities!$D$11</f>
-        <v>0.04</v>
-      </c>
-      <c r="I15" s="9">
+      <c r="I15" s="4">
+        <f t="shared" si="3"/>
+        <v>0.04</v>
+      </c>
+      <c r="J15" s="9">
         <f>utilities!$E$11</f>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
       <c r="B16">
-        <f>utilities!$B$8</f>
         <v>6</v>
       </c>
       <c r="C16">
-        <f>utilities!$C$8</f>
         <v>8</v>
       </c>
       <c r="D16">
-        <f>utilities!$D$8</f>
         <v>9</v>
       </c>
       <c r="E16">
         <v>11</v>
       </c>
-      <c r="F16" s="4">
-        <f>utilities!$B$11</f>
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="G16" s="4">
+        <f t="shared" si="1"/>
         <v>0.16666666666666666</v>
       </c>
-      <c r="G16" s="4">
-        <f>utilities!$C$11</f>
+      <c r="H16" s="4">
+        <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
-      <c r="H16" s="4">
-        <f>utilities!$D$11</f>
-        <v>0.04</v>
-      </c>
-      <c r="I16" s="9">
+      <c r="I16" s="4">
+        <f t="shared" si="3"/>
+        <v>0.04</v>
+      </c>
+      <c r="J16" s="9">
         <f>utilities!$E$11</f>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
       <c r="B17">
-        <f>utilities!$B$8</f>
         <v>6</v>
       </c>
       <c r="C17">
-        <f>utilities!$C$8</f>
         <v>8</v>
       </c>
       <c r="D17">
-        <f>utilities!$D$8</f>
         <v>9</v>
       </c>
       <c r="E17">
         <v>11</v>
       </c>
-      <c r="F17" s="4">
-        <f>utilities!$B$11</f>
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="G17" s="4">
+        <f t="shared" si="1"/>
         <v>0.16666666666666666</v>
       </c>
-      <c r="G17" s="4">
-        <f>utilities!$C$11</f>
+      <c r="H17" s="4">
+        <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
-      <c r="H17" s="4">
-        <f>utilities!$D$11</f>
-        <v>0.04</v>
-      </c>
-      <c r="I17" s="9">
+      <c r="I17" s="4">
+        <f t="shared" si="3"/>
+        <v>0.04</v>
+      </c>
+      <c r="J17" s="9">
         <f>utilities!$E$11</f>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
       <c r="B18">
-        <f>utilities!$B$8</f>
         <v>6</v>
       </c>
       <c r="C18">
-        <f>utilities!$C$8</f>
         <v>8</v>
       </c>
       <c r="D18">
-        <f>utilities!$D$8</f>
         <v>9</v>
       </c>
       <c r="E18">
         <v>11</v>
       </c>
-      <c r="F18" s="4">
-        <f>utilities!$B$11</f>
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="G18" s="4">
+        <f t="shared" si="1"/>
         <v>0.16666666666666666</v>
       </c>
-      <c r="G18" s="4">
-        <f>utilities!$C$11</f>
+      <c r="H18" s="4">
+        <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
-      <c r="H18" s="4">
-        <f>utilities!$D$11</f>
-        <v>0.04</v>
-      </c>
-      <c r="I18" s="9">
+      <c r="I18" s="4">
+        <f t="shared" si="3"/>
+        <v>0.04</v>
+      </c>
+      <c r="J18" s="9">
         <f>utilities!$E$11</f>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
       <c r="B19">
-        <f>utilities!$B$8</f>
         <v>6</v>
       </c>
       <c r="C19">
-        <f>utilities!$C$8</f>
         <v>8</v>
       </c>
       <c r="D19">
-        <f>utilities!$D$8</f>
         <v>9</v>
       </c>
       <c r="E19">
         <v>11</v>
       </c>
-      <c r="F19" s="4">
-        <f>utilities!$B$11</f>
+      <c r="F19">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="G19" s="4">
+        <f t="shared" si="1"/>
         <v>0.16666666666666666</v>
       </c>
-      <c r="G19" s="4">
-        <f>utilities!$C$11</f>
+      <c r="H19" s="4">
+        <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
-      <c r="H19" s="4">
-        <f>utilities!$D$11</f>
-        <v>0.04</v>
-      </c>
-      <c r="I19" s="9">
+      <c r="I19" s="4">
+        <f t="shared" si="3"/>
+        <v>0.04</v>
+      </c>
+      <c r="J19" s="9">
         <f>utilities!$E$11</f>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
       <c r="B20">
-        <f>utilities!$B$8</f>
         <v>6</v>
       </c>
       <c r="C20">
-        <f>utilities!$C$8</f>
         <v>8</v>
       </c>
       <c r="D20">
-        <f>utilities!$D$8</f>
         <v>9</v>
       </c>
       <c r="E20">
         <v>11</v>
       </c>
-      <c r="F20" s="4">
-        <f>utilities!$B$11</f>
+      <c r="F20">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="G20" s="4">
+        <f t="shared" si="1"/>
         <v>0.16666666666666666</v>
       </c>
-      <c r="G20" s="4">
-        <f>utilities!$C$11</f>
+      <c r="H20" s="4">
+        <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
-      <c r="H20" s="4">
-        <f>utilities!$D$11</f>
-        <v>0.04</v>
-      </c>
-      <c r="I20" s="9">
+      <c r="I20" s="4">
+        <f t="shared" si="3"/>
+        <v>0.04</v>
+      </c>
+      <c r="J20" s="9">
         <f>utilities!$E$11</f>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
       <c r="B21">
-        <f>utilities!$B$8</f>
         <v>6</v>
       </c>
       <c r="C21">
-        <f>utilities!$C$8</f>
         <v>8</v>
       </c>
       <c r="D21">
-        <f>utilities!$D$8</f>
         <v>9</v>
       </c>
       <c r="E21">
         <v>11</v>
       </c>
-      <c r="F21" s="4">
-        <f>utilities!$B$11</f>
+      <c r="F21">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="G21" s="4">
+        <f t="shared" si="1"/>
         <v>0.16666666666666666</v>
       </c>
-      <c r="G21" s="4">
-        <f>utilities!$C$11</f>
+      <c r="H21" s="4">
+        <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
-      <c r="H21" s="4">
-        <f>utilities!$D$11</f>
-        <v>0.04</v>
-      </c>
-      <c r="I21" s="9">
+      <c r="I21" s="4">
+        <f t="shared" si="3"/>
+        <v>0.04</v>
+      </c>
+      <c r="J21" s="9">
         <f>utilities!$E$11</f>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
       <c r="B22">
-        <f>utilities!$B$8</f>
         <v>6</v>
       </c>
       <c r="C22">
-        <f>utilities!$C$8</f>
         <v>8</v>
       </c>
       <c r="D22">
-        <f>utilities!$D$8</f>
         <v>9</v>
       </c>
       <c r="E22">
         <v>11</v>
       </c>
-      <c r="F22" s="4">
-        <f>utilities!$B$11</f>
+      <c r="F22">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="G22" s="4">
+        <f t="shared" si="1"/>
         <v>0.16666666666666666</v>
       </c>
-      <c r="G22" s="4">
-        <f>utilities!$C$11</f>
+      <c r="H22" s="4">
+        <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
-      <c r="H22" s="4">
-        <f>utilities!$D$11</f>
-        <v>0.04</v>
-      </c>
-      <c r="I22" s="9">
+      <c r="I22" s="4">
+        <f t="shared" si="3"/>
+        <v>0.04</v>
+      </c>
+      <c r="J22" s="9">
         <f>utilities!$E$11</f>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
       <c r="B23">
-        <f>utilities!$B$8</f>
         <v>6</v>
       </c>
       <c r="C23">
-        <f>utilities!$C$8</f>
         <v>8</v>
       </c>
       <c r="D23">
-        <f>utilities!$D$8</f>
         <v>9</v>
       </c>
       <c r="E23">
         <v>11</v>
       </c>
-      <c r="F23" s="4">
-        <f>utilities!$B$11</f>
+      <c r="F23">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="G23" s="4">
+        <f t="shared" si="1"/>
         <v>0.16666666666666666</v>
       </c>
-      <c r="G23" s="4">
-        <f>utilities!$C$11</f>
+      <c r="H23" s="4">
+        <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
-      <c r="H23" s="4">
-        <f>utilities!$D$11</f>
-        <v>0.04</v>
-      </c>
-      <c r="I23" s="9">
+      <c r="I23" s="4">
+        <f t="shared" si="3"/>
+        <v>0.04</v>
+      </c>
+      <c r="J23" s="9">
         <f>utilities!$E$11</f>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
       <c r="B24">
-        <f>utilities!$B$8</f>
         <v>6</v>
       </c>
       <c r="C24">
-        <f>utilities!$C$8</f>
         <v>8</v>
       </c>
       <c r="D24">
-        <f>utilities!$D$8</f>
         <v>9</v>
       </c>
       <c r="E24">
         <v>11</v>
       </c>
-      <c r="F24" s="4">
-        <f>utilities!$B$11</f>
+      <c r="F24">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="G24" s="4">
+        <f t="shared" si="1"/>
         <v>0.16666666666666666</v>
       </c>
-      <c r="G24" s="4">
-        <f>utilities!$C$11</f>
+      <c r="H24" s="4">
+        <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
-      <c r="H24" s="4">
-        <f>utilities!$D$11</f>
-        <v>0.04</v>
-      </c>
-      <c r="I24" s="9">
+      <c r="I24" s="4">
+        <f t="shared" si="3"/>
+        <v>0.04</v>
+      </c>
+      <c r="J24" s="9">
         <f>utilities!$E$11</f>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
       <c r="B25">
-        <f>utilities!$B$8</f>
         <v>6</v>
       </c>
       <c r="C25">
-        <f>utilities!$C$8</f>
         <v>8</v>
       </c>
       <c r="D25">
-        <f>utilities!$D$8</f>
         <v>9</v>
       </c>
       <c r="E25">
         <v>11</v>
       </c>
-      <c r="F25" s="4">
-        <f>utilities!$B$11</f>
+      <c r="F25">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="G25" s="4">
+        <f t="shared" si="1"/>
         <v>0.16666666666666666</v>
       </c>
-      <c r="G25" s="4">
-        <f>utilities!$C$11</f>
+      <c r="H25" s="4">
+        <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
-      <c r="H25" s="4">
-        <f>utilities!$D$11</f>
-        <v>0.04</v>
-      </c>
-      <c r="I25" s="9">
+      <c r="I25" s="4">
+        <f t="shared" si="3"/>
+        <v>0.04</v>
+      </c>
+      <c r="J25" s="9">
         <f>utilities!$E$11</f>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
       <c r="B26">
-        <f>utilities!$B$8</f>
         <v>6</v>
       </c>
       <c r="C26">
-        <f>utilities!$C$8</f>
         <v>8</v>
       </c>
       <c r="D26">
-        <f>utilities!$D$8</f>
         <v>9</v>
       </c>
       <c r="E26">
         <v>11</v>
       </c>
-      <c r="F26" s="4">
-        <f>utilities!$B$11</f>
+      <c r="F26">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="G26" s="4">
+        <f t="shared" si="1"/>
         <v>0.16666666666666666</v>
       </c>
-      <c r="G26" s="4">
-        <f>utilities!$C$11</f>
+      <c r="H26" s="4">
+        <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
-      <c r="H26" s="4">
-        <f>utilities!$D$11</f>
-        <v>0.04</v>
-      </c>
-      <c r="I26" s="9">
+      <c r="I26" s="4">
+        <f t="shared" si="3"/>
+        <v>0.04</v>
+      </c>
+      <c r="J26" s="9">
         <f>utilities!$E$11</f>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>
       <c r="B27">
-        <f>utilities!$T$8</f>
         <v>96</v>
       </c>
       <c r="C27">
-        <f>utilities!$U$8</f>
         <v>143</v>
       </c>
       <c r="D27">
-        <f>utilities!$V$8</f>
         <v>259</v>
       </c>
       <c r="E27">
         <v>11</v>
       </c>
-      <c r="F27" s="4">
-        <f>utilities!T$11</f>
-        <v>0.2734375</v>
+      <c r="F27">
+        <v>1</v>
       </c>
       <c r="G27" s="4">
-        <f>utilities!$U$11</f>
-        <v>0.11170212765957446</v>
+        <f t="shared" si="1"/>
+        <v>0.26041666666666669</v>
       </c>
       <c r="H27" s="4">
-        <f>utilities!$V$11</f>
-        <v>9.0517241379310352E-3</v>
-      </c>
-      <c r="I27" s="9">
+        <f t="shared" si="2"/>
+        <v>0.10638297872340426</v>
+      </c>
+      <c r="I27" s="4">
+        <f t="shared" si="3"/>
+        <v>8.6206896551724137E-3</v>
+      </c>
+      <c r="J27" s="9">
         <f>utilities!$E$11</f>
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28">
+      <c r="L27">
+        <f>0.9*250</f>
+        <v>225</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28">
+        <f>SUM(B2:B27)</f>
+        <v>306</v>
+      </c>
+      <c r="C28">
+        <f t="shared" ref="C28:D28" si="4">SUM(C2:C27)</f>
+        <v>433</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="4"/>
+        <v>634</v>
+      </c>
+      <c r="E28">
+        <f>SUM(E2:E27)</f>
+        <v>275</v>
+      </c>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29">
         <v>26</v>
-      </c>
-      <c r="B28">
-        <f>utilities!$H$8</f>
-        <v>0</v>
-      </c>
-      <c r="C28">
-        <f>utilities!$I$8</f>
-        <v>0</v>
-      </c>
-      <c r="D28">
-        <f>utilities!$J$8</f>
-        <v>0</v>
-      </c>
-      <c r="E28">
-        <v>0</v>
-      </c>
-      <c r="F28" s="4" t="e">
-        <f>utilities!$H$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G28" s="4" t="e">
-        <f>utilities!$I$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H28" s="4" t="e">
-        <f>utilities!$J$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I28" s="9">
-        <f>utilities!$K$11</f>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>27</v>
       </c>
       <c r="B29">
         <f>utilities!$H$8</f>
@@ -1599,26 +1629,30 @@
       <c r="E29">
         <v>0</v>
       </c>
-      <c r="F29" s="4" t="e">
+      <c r="F29">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="G29" s="4" t="e">
         <f>utilities!$H$11</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G29" s="4" t="e">
+      <c r="H29" s="4" t="e">
         <f>utilities!$I$11</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H29" s="4" t="e">
+      <c r="I29" s="4" t="e">
         <f>utilities!$J$11</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I29" s="9">
+      <c r="J29" s="9">
         <f>utilities!$K$11</f>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B30">
         <f>utilities!$H$8</f>
@@ -1635,26 +1669,30 @@
       <c r="E30">
         <v>0</v>
       </c>
-      <c r="F30" s="4" t="e">
+      <c r="F30">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="G30" s="4" t="e">
         <f>utilities!$H$11</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G30" s="4" t="e">
+      <c r="H30" s="4" t="e">
         <f>utilities!$I$11</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H30" s="4" t="e">
+      <c r="I30" s="4" t="e">
         <f>utilities!$J$11</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I30" s="9">
+      <c r="J30" s="9">
         <f>utilities!$K$11</f>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B31">
         <f>utilities!$H$8</f>
@@ -1671,26 +1709,30 @@
       <c r="E31">
         <v>0</v>
       </c>
-      <c r="F31" s="4" t="e">
+      <c r="F31">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="G31" s="4" t="e">
         <f>utilities!$H$11</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G31" s="4" t="e">
+      <c r="H31" s="4" t="e">
         <f>utilities!$I$11</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H31" s="4" t="e">
+      <c r="I31" s="4" t="e">
         <f>utilities!$J$11</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I31" s="9">
+      <c r="J31" s="9">
         <f>utilities!$K$11</f>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B32">
         <f>utilities!$H$8</f>
@@ -1707,26 +1749,30 @@
       <c r="E32">
         <v>0</v>
       </c>
-      <c r="F32" s="4" t="e">
+      <c r="F32">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="G32" s="4" t="e">
         <f>utilities!$H$11</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G32" s="4" t="e">
+      <c r="H32" s="4" t="e">
         <f>utilities!$I$11</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H32" s="4" t="e">
+      <c r="I32" s="4" t="e">
         <f>utilities!$J$11</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I32" s="9">
+      <c r="J32" s="9">
         <f>utilities!$K$11</f>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B33">
         <f>utilities!$H$8</f>
@@ -1743,26 +1789,30 @@
       <c r="E33">
         <v>0</v>
       </c>
-      <c r="F33" s="4" t="e">
+      <c r="F33">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="G33" s="4" t="e">
         <f>utilities!$H$11</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G33" s="4" t="e">
+      <c r="H33" s="4" t="e">
         <f>utilities!$I$11</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H33" s="4" t="e">
+      <c r="I33" s="4" t="e">
         <f>utilities!$J$11</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I33" s="9">
+      <c r="J33" s="9">
         <f>utilities!$K$11</f>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B34">
         <f>utilities!$H$8</f>
@@ -1779,26 +1829,30 @@
       <c r="E34">
         <v>0</v>
       </c>
-      <c r="F34" s="4" t="e">
+      <c r="F34">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="G34" s="4" t="e">
         <f>utilities!$H$11</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G34" s="4" t="e">
+      <c r="H34" s="4" t="e">
         <f>utilities!$I$11</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H34" s="4" t="e">
+      <c r="I34" s="4" t="e">
         <f>utilities!$J$11</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I34" s="9">
+      <c r="J34" s="9">
         <f>utilities!$K$11</f>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B35">
         <f>utilities!$H$8</f>
@@ -1815,26 +1869,30 @@
       <c r="E35">
         <v>0</v>
       </c>
-      <c r="F35" s="4" t="e">
+      <c r="F35">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="G35" s="4" t="e">
         <f>utilities!$H$11</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G35" s="4" t="e">
+      <c r="H35" s="4" t="e">
         <f>utilities!$I$11</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H35" s="4" t="e">
+      <c r="I35" s="4" t="e">
         <f>utilities!$J$11</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I35" s="9">
+      <c r="J35" s="9">
         <f>utilities!$K$11</f>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B36">
         <f>utilities!$H$8</f>
@@ -1851,26 +1909,30 @@
       <c r="E36">
         <v>0</v>
       </c>
-      <c r="F36" s="4" t="e">
+      <c r="F36">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="G36" s="4" t="e">
         <f>utilities!$H$11</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G36" s="4" t="e">
+      <c r="H36" s="4" t="e">
         <f>utilities!$I$11</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H36" s="4" t="e">
+      <c r="I36" s="4" t="e">
         <f>utilities!$J$11</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I36" s="9">
+      <c r="J36" s="9">
         <f>utilities!$K$11</f>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B37">
         <f>utilities!$H$8</f>
@@ -1887,26 +1949,30 @@
       <c r="E37">
         <v>0</v>
       </c>
-      <c r="F37" s="4" t="e">
+      <c r="F37">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="G37" s="4" t="e">
         <f>utilities!$H$11</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G37" s="4" t="e">
+      <c r="H37" s="4" t="e">
         <f>utilities!$I$11</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H37" s="4" t="e">
+      <c r="I37" s="4" t="e">
         <f>utilities!$J$11</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I37" s="9">
+      <c r="J37" s="9">
         <f>utilities!$K$11</f>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B38">
         <f>utilities!$H$8</f>
@@ -1923,26 +1989,30 @@
       <c r="E38">
         <v>0</v>
       </c>
-      <c r="F38" s="4" t="e">
+      <c r="F38">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="G38" s="4" t="e">
         <f>utilities!$H$11</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G38" s="4" t="e">
+      <c r="H38" s="4" t="e">
         <f>utilities!$I$11</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H38" s="4" t="e">
+      <c r="I38" s="4" t="e">
         <f>utilities!$J$11</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I38" s="9">
+      <c r="J38" s="9">
         <f>utilities!$K$11</f>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B39">
         <f>utilities!$H$8</f>
@@ -1959,26 +2029,30 @@
       <c r="E39">
         <v>0</v>
       </c>
-      <c r="F39" s="4" t="e">
+      <c r="F39">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="G39" s="4" t="e">
         <f>utilities!$H$11</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G39" s="4" t="e">
+      <c r="H39" s="4" t="e">
         <f>utilities!$I$11</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H39" s="4" t="e">
+      <c r="I39" s="4" t="e">
         <f>utilities!$J$11</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I39" s="9">
+      <c r="J39" s="9">
         <f>utilities!$K$11</f>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B40">
         <f>utilities!$H$8</f>
@@ -1995,26 +2069,30 @@
       <c r="E40">
         <v>0</v>
       </c>
-      <c r="F40" s="4" t="e">
+      <c r="F40">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="G40" s="4" t="e">
         <f>utilities!$H$11</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G40" s="4" t="e">
+      <c r="H40" s="4" t="e">
         <f>utilities!$I$11</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H40" s="4" t="e">
+      <c r="I40" s="4" t="e">
         <f>utilities!$J$11</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I40" s="9">
+      <c r="J40" s="9">
         <f>utilities!$K$11</f>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B41">
         <f>utilities!$H$8</f>
@@ -2031,26 +2109,30 @@
       <c r="E41">
         <v>0</v>
       </c>
-      <c r="F41" s="4" t="e">
+      <c r="F41">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="G41" s="4" t="e">
         <f>utilities!$H$11</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G41" s="4" t="e">
+      <c r="H41" s="4" t="e">
         <f>utilities!$I$11</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H41" s="4" t="e">
+      <c r="I41" s="4" t="e">
         <f>utilities!$J$11</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I41" s="9">
+      <c r="J41" s="9">
         <f>utilities!$K$11</f>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B42">
         <f>utilities!$H$8</f>
@@ -2067,19 +2149,63 @@
       <c r="E42">
         <v>0</v>
       </c>
-      <c r="F42" s="4" t="e">
+      <c r="F42">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="G42" s="4" t="e">
         <f>utilities!$H$11</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G42" s="4" t="e">
+      <c r="H42" s="4" t="e">
         <f>utilities!$I$11</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H42" s="4" t="e">
+      <c r="I42" s="4" t="e">
         <f>utilities!$J$11</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I42" s="9">
+      <c r="J42" s="9">
+        <f>utilities!$K$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>40</v>
+      </c>
+      <c r="B43">
+        <f>utilities!$H$8</f>
+        <v>0</v>
+      </c>
+      <c r="C43">
+        <f>utilities!$I$8</f>
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <f>utilities!$J$8</f>
+        <v>0</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+      <c r="F43">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="G43" s="4" t="e">
+        <f>utilities!$H$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H43" s="4" t="e">
+        <f>utilities!$I$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I43" s="4" t="e">
+        <f>utilities!$J$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J43" s="9">
         <f>utilities!$K$11</f>
         <v>1E-3</v>
       </c>
@@ -2090,20 +2216,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FFE0B56-DF8B-44CF-9758-6EDE70A13051}">
-  <dimension ref="A1:I34"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F977CF0C-F948-4BB4-989B-6B75181A9A01}">
+  <dimension ref="A1:L43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="16.7109375" customWidth="1"/>
-    <col min="9" max="9" width="8.85546875" style="9"/>
+    <col min="7" max="7" width="16.7109375" customWidth="1"/>
+    <col min="10" max="10" width="9.5703125" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -2119,1199 +2245,1452 @@
       <c r="E1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="J1" s="11" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>12</v>
+        <f>6*3.5</f>
+        <v>21</v>
       </c>
       <c r="C2">
-        <v>16</v>
+        <f>8*3.5</f>
+        <v>28</v>
       </c>
       <c r="D2">
-        <v>18</v>
+        <f>9*3.5</f>
+        <v>31.5</v>
       </c>
       <c r="E2">
-        <v>10</v>
-      </c>
-      <c r="F2" s="4">
-        <f>1.04166666666667/1</f>
-        <v>1.0416666666666701</v>
-      </c>
-      <c r="G2" s="4">
-        <f>0.625/1</f>
-        <v>0.625</v>
-      </c>
-      <c r="H2" s="4">
-        <f>0.25/1</f>
-        <v>0.25</v>
-      </c>
-      <c r="I2" s="9">
-        <f>utilities!$E$11</f>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <f>27.5</f>
+        <v>27.5</v>
+      </c>
+      <c r="F2">
+        <f>1/25</f>
+        <v>0.04</v>
+      </c>
+      <c r="G2" s="13">
+        <f>(100*F2)/B2</f>
+        <v>0.19047619047619047</v>
+      </c>
+      <c r="H2" s="13">
+        <f>(20*F2)/(C2-B2)</f>
+        <v>0.1142857142857143</v>
+      </c>
+      <c r="I2" s="13">
+        <f>(1*F2)/(D2-C2)</f>
+        <v>1.1428571428571429E-2</v>
+      </c>
+      <c r="J2" s="9">
+        <v>1E-3</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <f>D2-E2</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <f>utilities!$B$8</f>
-        <v>6</v>
+        <f>6*5</f>
+        <v>30</v>
       </c>
       <c r="C3">
-        <f>utilities!$C$8</f>
-        <v>8</v>
+        <f>8*5</f>
+        <v>40</v>
       </c>
       <c r="D3">
-        <f>utilities!$D$8</f>
-        <v>9</v>
+        <f>9*5</f>
+        <v>45</v>
       </c>
       <c r="E3">
-        <v>30</v>
-      </c>
-      <c r="F3" s="4">
-        <f>utilities!$B$11</f>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="G3" s="4">
-        <f>utilities!$C$11</f>
-        <v>0.1</v>
-      </c>
-      <c r="H3" s="4">
-        <f>utilities!$D$11</f>
-        <v>0.04</v>
-      </c>
-      <c r="I3" s="9">
-        <f>utilities!$E$11</f>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F7" si="0">1/25</f>
+        <v>0.04</v>
+      </c>
+      <c r="G3" s="13">
+        <f t="shared" ref="G3:G7" si="1">(25*F3)/B3</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="H3" s="13">
+        <f t="shared" ref="H3:H7" si="2">(5*F3)/(C3-B3)</f>
+        <v>0.02</v>
+      </c>
+      <c r="I3" s="13">
+        <f t="shared" ref="I3:I7" si="3">(1*F3)/(D3-C3)</f>
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="J3" s="9">
+        <v>1E-3</v>
+      </c>
+      <c r="K3">
+        <v>5</v>
+      </c>
+      <c r="L3">
+        <f t="shared" ref="L3:L7" si="4">D3-E3</f>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
-        <f>utilities!$N$8</f>
-        <v>66</v>
+        <f>6*5+60</f>
+        <v>90</v>
       </c>
       <c r="C4">
-        <f>utilities!$O$8</f>
-        <v>98</v>
+        <f>8*5+90</f>
+        <v>130</v>
       </c>
       <c r="D4">
-        <f>utilities!$P$8</f>
-        <v>159</v>
+        <f>9*5+150</f>
+        <v>195</v>
       </c>
       <c r="E4">
-        <v>30</v>
-      </c>
-      <c r="F4" s="4">
-        <f>utilities!N11</f>
-        <v>0.39772727272727271</v>
-      </c>
-      <c r="G4" s="4">
-        <f>utilities!O11</f>
-        <v>0.1640625</v>
-      </c>
-      <c r="H4" s="4">
-        <f>utilities!P11</f>
-        <v>1.7213114754098362E-2</v>
-      </c>
-      <c r="I4" s="9">
-        <f>utilities!$E$11</f>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="G4" s="13">
+        <f t="shared" si="1"/>
+        <v>1.1111111111111112E-2</v>
+      </c>
+      <c r="H4" s="13">
+        <f t="shared" si="2"/>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="I4" s="13">
+        <f t="shared" si="3"/>
+        <v>6.1538461538461541E-4</v>
+      </c>
+      <c r="J4" s="9">
+        <v>1E-3</v>
+      </c>
+      <c r="K4">
+        <v>10</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="4"/>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
-        <f>utilities!$B$8</f>
-        <v>6</v>
+        <f>6*5</f>
+        <v>30</v>
       </c>
       <c r="C5">
-        <f>utilities!$C$8</f>
-        <v>8</v>
+        <f>8*5</f>
+        <v>40</v>
       </c>
       <c r="D5">
-        <f>utilities!$D$8</f>
-        <v>9</v>
+        <f>9*5</f>
+        <v>45</v>
       </c>
       <c r="E5">
-        <v>30</v>
-      </c>
-      <c r="F5" s="4">
-        <f>utilities!$B$11</f>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="G5" s="4">
-        <f>utilities!$C$11</f>
-        <v>0.1</v>
-      </c>
-      <c r="H5" s="4">
-        <f>utilities!$D$11</f>
-        <v>0.04</v>
-      </c>
-      <c r="I5" s="9">
-        <f>utilities!$E$11</f>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="G5" s="13">
+        <f t="shared" si="1"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="H5" s="13">
+        <f t="shared" si="2"/>
+        <v>0.02</v>
+      </c>
+      <c r="I5" s="13">
+        <f t="shared" si="3"/>
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="J5" s="9">
+        <v>1E-3</v>
+      </c>
+      <c r="K5">
+        <v>15</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="4"/>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="12">
-        <v>87</v>
-      </c>
-      <c r="C6" s="12">
-        <v>151</v>
-      </c>
-      <c r="D6" s="12">
-        <v>168</v>
+      <c r="B6">
+        <f>6*5</f>
+        <v>30</v>
+      </c>
+      <c r="C6">
+        <f>8*5</f>
+        <v>40</v>
+      </c>
+      <c r="D6">
+        <f t="shared" ref="D6" si="5">9*5</f>
+        <v>45</v>
       </c>
       <c r="E6">
+        <v>55</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="G6" s="13">
+        <f t="shared" si="1"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="H6" s="13">
+        <f t="shared" si="2"/>
+        <v>0.02</v>
+      </c>
+      <c r="I6" s="13">
+        <f t="shared" si="3"/>
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="J6" s="9">
+        <v>1E-3</v>
+      </c>
+      <c r="K6">
         <v>20</v>
       </c>
-      <c r="F6" s="4">
-        <f>utilities!T11</f>
-        <v>0.2734375</v>
-      </c>
-      <c r="G6" s="4">
-        <f>utilities!U11</f>
-        <v>0.11170212765957446</v>
-      </c>
-      <c r="H6" s="4">
-        <f>utilities!V11</f>
-        <v>9.0517241379310352E-3</v>
-      </c>
-      <c r="I6" s="9">
-        <f>utilities!$E$11</f>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L6">
+        <f t="shared" si="4"/>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <f>6*2.5+90</f>
+        <v>105</v>
+      </c>
+      <c r="C7">
+        <f>8*2.5+135</f>
+        <v>155</v>
+      </c>
+      <c r="D7">
+        <f>22.5+250</f>
+        <v>272.5</v>
+      </c>
+      <c r="E7">
+        <v>27.5</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="G7" s="13">
+        <f t="shared" si="1"/>
+        <v>9.5238095238095247E-3</v>
+      </c>
+      <c r="H7" s="13">
+        <f t="shared" si="2"/>
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="I7" s="13">
+        <f t="shared" si="3"/>
+        <v>3.4042553191489364E-4</v>
+      </c>
+      <c r="J7" s="9">
+        <v>1E-3</v>
+      </c>
+      <c r="K7">
+        <v>25</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="4"/>
+        <v>245</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <f t="shared" ref="B8:D8" si="6">SUM(B2:B7)</f>
+        <v>306</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="6"/>
+        <v>433</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="6"/>
+        <v>634</v>
+      </c>
+      <c r="E8">
+        <f>SUM(E2:E7)</f>
+        <v>275</v>
+      </c>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="L8" s="14" t="e">
+        <f>IRR(L2:L7)/5</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9" s="4">
+        <v>0</v>
+      </c>
+      <c r="H9" s="4">
+        <v>0</v>
+      </c>
+      <c r="I9" s="4">
+        <v>0</v>
+      </c>
+      <c r="J9" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10" s="4">
+        <v>0</v>
+      </c>
+      <c r="H10" s="4">
+        <v>0</v>
+      </c>
+      <c r="I10" s="4">
+        <v>0</v>
+      </c>
+      <c r="J10" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11" s="4">
+        <v>0</v>
+      </c>
+      <c r="H11" s="4">
+        <v>0</v>
+      </c>
+      <c r="I11" s="4">
+        <v>0</v>
+      </c>
+      <c r="J11" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12" s="4">
+        <v>0</v>
+      </c>
+      <c r="H12" s="4">
+        <v>0</v>
+      </c>
+      <c r="I12" s="4">
+        <v>0</v>
+      </c>
+      <c r="J12" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13" s="4">
+        <v>0</v>
+      </c>
+      <c r="H13" s="4">
+        <v>0</v>
+      </c>
+      <c r="I13" s="4">
+        <v>0</v>
+      </c>
+      <c r="J13" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14" s="4">
+        <v>0</v>
+      </c>
+      <c r="H14" s="4">
+        <v>0</v>
+      </c>
+      <c r="I14" s="4">
+        <v>0</v>
+      </c>
+      <c r="J14" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15">
         <v>13</v>
       </c>
-      <c r="B7">
-        <f>utilities!$H$8</f>
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <f>utilities!$I$8</f>
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <f>utilities!$J$8</f>
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>-8</v>
-      </c>
-      <c r="F7" s="4">
-        <f>utilities!$B$11</f>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="G7" s="4">
-        <f>utilities!$C$11</f>
-        <v>0.1</v>
-      </c>
-      <c r="H7" s="4">
-        <f>utilities!$D$11</f>
-        <v>0.04</v>
-      </c>
-      <c r="I7" s="9">
-        <f>utilities!$E$11</f>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15" s="4">
+        <v>0</v>
+      </c>
+      <c r="H15" s="4">
+        <v>0</v>
+      </c>
+      <c r="I15" s="4">
+        <v>0</v>
+      </c>
+      <c r="J15" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>13</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16" s="4">
+        <v>0</v>
+      </c>
+      <c r="H16" s="4">
+        <v>0</v>
+      </c>
+      <c r="I16" s="4">
+        <v>0</v>
+      </c>
+      <c r="J16" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17">
         <v>14</v>
       </c>
-      <c r="B8">
-        <f>utilities!$H$8</f>
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <f>utilities!$I$8</f>
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <f>utilities!$J$8</f>
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>-7</v>
-      </c>
-      <c r="F8" s="4">
-        <f>utilities!$B$11</f>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="G8" s="4">
-        <f>utilities!$C$11</f>
-        <v>0.1</v>
-      </c>
-      <c r="H8" s="4">
-        <f>utilities!$D$11</f>
-        <v>0.04</v>
-      </c>
-      <c r="I8" s="9">
-        <f>utilities!$E$11</f>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17" s="4">
+        <v>0</v>
+      </c>
+      <c r="H17" s="4">
+        <v>0</v>
+      </c>
+      <c r="I17" s="4">
+        <v>0</v>
+      </c>
+      <c r="J17" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18">
         <v>15</v>
       </c>
-      <c r="B9">
-        <f>utilities!$H$8</f>
-        <v>0</v>
-      </c>
-      <c r="C9">
-        <f>utilities!$I$8</f>
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <f>utilities!$J$8</f>
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>-6</v>
-      </c>
-      <c r="F9" s="4">
-        <f>utilities!$B$11</f>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="G9" s="4">
-        <f>utilities!$C$11</f>
-        <v>0.1</v>
-      </c>
-      <c r="H9" s="4">
-        <f>utilities!$D$11</f>
-        <v>0.04</v>
-      </c>
-      <c r="I9" s="9">
-        <f>utilities!$E$11</f>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18" s="4">
+        <v>0</v>
+      </c>
+      <c r="H18" s="4">
+        <v>0</v>
+      </c>
+      <c r="I18" s="4">
+        <v>0</v>
+      </c>
+      <c r="J18" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19">
         <v>16</v>
       </c>
-      <c r="B10">
-        <f>utilities!$H$8</f>
-        <v>0</v>
-      </c>
-      <c r="C10">
-        <f>utilities!$I$8</f>
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <f>utilities!$J$8</f>
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>-5</v>
-      </c>
-      <c r="F10" s="4">
-        <f>utilities!$B$11</f>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="G10" s="4">
-        <f>utilities!$C$11</f>
-        <v>0.1</v>
-      </c>
-      <c r="H10" s="4">
-        <f>utilities!$D$11</f>
-        <v>0.04</v>
-      </c>
-      <c r="I10" s="9">
-        <f>utilities!$E$11</f>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19" s="4">
+        <v>0</v>
+      </c>
+      <c r="H19" s="4">
+        <v>0</v>
+      </c>
+      <c r="I19" s="4">
+        <v>0</v>
+      </c>
+      <c r="J19" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20">
         <v>17</v>
       </c>
-      <c r="B11">
-        <f>utilities!$H$8</f>
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <f>utilities!$I$8</f>
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <f>utilities!$J$8</f>
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>-4</v>
-      </c>
-      <c r="F11" s="4">
-        <f>utilities!$B$11</f>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="G11" s="4">
-        <f>utilities!$C$11</f>
-        <v>0.1</v>
-      </c>
-      <c r="H11" s="4">
-        <f>utilities!$D$11</f>
-        <v>0.04</v>
-      </c>
-      <c r="I11" s="9">
-        <f>utilities!$E$11</f>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20" s="4">
+        <v>0</v>
+      </c>
+      <c r="H20" s="4">
+        <v>0</v>
+      </c>
+      <c r="I20" s="4">
+        <v>0</v>
+      </c>
+      <c r="J20" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21">
         <v>18</v>
       </c>
-      <c r="B12">
-        <f>utilities!$H$8</f>
-        <v>0</v>
-      </c>
-      <c r="C12">
-        <f>utilities!$I$8</f>
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <f>utilities!$J$8</f>
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>-3</v>
-      </c>
-      <c r="F12" s="4">
-        <f>utilities!$B$11</f>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="G12" s="4">
-        <f>utilities!$C$11</f>
-        <v>0.1</v>
-      </c>
-      <c r="H12" s="4">
-        <f>utilities!$D$11</f>
-        <v>0.04</v>
-      </c>
-      <c r="I12" s="9">
-        <f>utilities!$E$11</f>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21" s="4">
+        <v>0</v>
+      </c>
+      <c r="H21" s="4">
+        <v>0</v>
+      </c>
+      <c r="I21" s="4">
+        <v>0</v>
+      </c>
+      <c r="J21" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22">
         <v>19</v>
       </c>
-      <c r="B13">
-        <f>utilities!$H$8</f>
-        <v>0</v>
-      </c>
-      <c r="C13">
-        <f>utilities!$I$8</f>
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <f>utilities!$J$8</f>
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>-2</v>
-      </c>
-      <c r="F13" s="4">
-        <f>utilities!$B$11</f>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="G13" s="4">
-        <f>utilities!$C$11</f>
-        <v>0.1</v>
-      </c>
-      <c r="H13" s="4">
-        <f>utilities!$D$11</f>
-        <v>0.04</v>
-      </c>
-      <c r="I13" s="9">
-        <f>utilities!$E$11</f>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22" s="4">
+        <v>0</v>
+      </c>
+      <c r="H22" s="4">
+        <v>0</v>
+      </c>
+      <c r="I22" s="4">
+        <v>0</v>
+      </c>
+      <c r="J22" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23">
         <v>20</v>
       </c>
-      <c r="B14">
-        <f>utilities!$H$8</f>
-        <v>0</v>
-      </c>
-      <c r="C14">
-        <f>utilities!$I$8</f>
-        <v>0</v>
-      </c>
-      <c r="D14">
-        <f>utilities!$J$8</f>
-        <v>0</v>
-      </c>
-      <c r="E14">
-        <v>-1</v>
-      </c>
-      <c r="F14" s="4">
-        <f>utilities!$B$11</f>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="G14" s="4">
-        <f>utilities!$C$11</f>
-        <v>0.1</v>
-      </c>
-      <c r="H14" s="4">
-        <f>utilities!$D$11</f>
-        <v>0.04</v>
-      </c>
-      <c r="I14" s="9">
-        <f>utilities!$E$11</f>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23" s="4">
+        <v>0</v>
+      </c>
+      <c r="H23" s="4">
+        <v>0</v>
+      </c>
+      <c r="I23" s="4">
+        <v>0</v>
+      </c>
+      <c r="J23" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24">
         <v>21</v>
       </c>
-      <c r="B15">
-        <f>utilities!$H$8</f>
-        <v>0</v>
-      </c>
-      <c r="C15">
-        <f>utilities!$I$8</f>
-        <v>0</v>
-      </c>
-      <c r="D15">
-        <f>utilities!$J$8</f>
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15" s="4" t="e">
-        <f>utilities!$H$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G15" s="4" t="e">
-        <f>utilities!$I$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H15" s="4" t="e">
-        <f>utilities!$J$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I15" s="9">
-        <f>utilities!$K$11</f>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16">
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24" s="4">
+        <v>0</v>
+      </c>
+      <c r="H24" s="4">
+        <v>0</v>
+      </c>
+      <c r="I24" s="4">
+        <v>0</v>
+      </c>
+      <c r="J24" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25">
         <v>22</v>
       </c>
-      <c r="B16">
-        <f>utilities!$H$8</f>
-        <v>0</v>
-      </c>
-      <c r="C16">
-        <f>utilities!$I$8</f>
-        <v>0</v>
-      </c>
-      <c r="D16">
-        <f>utilities!$J$8</f>
-        <v>0</v>
-      </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-      <c r="F16" s="4" t="e">
-        <f>utilities!$H$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G16" s="4" t="e">
-        <f>utilities!$I$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H16" s="4" t="e">
-        <f>utilities!$J$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I16" s="9">
-        <f>utilities!$K$11</f>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17">
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25" s="4">
+        <v>0</v>
+      </c>
+      <c r="H25" s="4">
+        <v>0</v>
+      </c>
+      <c r="I25" s="4">
+        <v>0</v>
+      </c>
+      <c r="J25" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26">
         <v>23</v>
       </c>
-      <c r="B17">
-        <f>utilities!$H$8</f>
-        <v>0</v>
-      </c>
-      <c r="C17">
-        <f>utilities!$I$8</f>
-        <v>0</v>
-      </c>
-      <c r="D17">
-        <f>utilities!$J$8</f>
-        <v>0</v>
-      </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
-      <c r="F17" s="4" t="e">
-        <f>utilities!$H$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G17" s="4" t="e">
-        <f>utilities!$I$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H17" s="4" t="e">
-        <f>utilities!$J$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I17" s="9">
-        <f>utilities!$K$11</f>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18">
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26" s="4">
+        <v>0</v>
+      </c>
+      <c r="H26" s="4">
+        <v>0</v>
+      </c>
+      <c r="I26" s="4">
+        <v>0</v>
+      </c>
+      <c r="J26" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27">
         <v>24</v>
       </c>
-      <c r="B18">
-        <f>utilities!$H$8</f>
-        <v>0</v>
-      </c>
-      <c r="C18">
-        <f>utilities!$I$8</f>
-        <v>0</v>
-      </c>
-      <c r="D18">
-        <f>utilities!$J$8</f>
-        <v>0</v>
-      </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
-      <c r="F18" s="4" t="e">
-        <f>utilities!$H$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G18" s="4" t="e">
-        <f>utilities!$I$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H18" s="4" t="e">
-        <f>utilities!$J$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I18" s="9">
-        <f>utilities!$K$11</f>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19">
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27" s="4">
+        <v>0</v>
+      </c>
+      <c r="H27" s="4">
+        <v>0</v>
+      </c>
+      <c r="I27" s="4">
+        <v>0</v>
+      </c>
+      <c r="J27" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28">
         <v>25</v>
       </c>
-      <c r="B19">
-        <f>utilities!$H$8</f>
-        <v>0</v>
-      </c>
-      <c r="C19">
-        <f>utilities!$I$8</f>
-        <v>0</v>
-      </c>
-      <c r="D19">
-        <f>utilities!$J$8</f>
-        <v>0</v>
-      </c>
-      <c r="E19">
-        <v>0</v>
-      </c>
-      <c r="F19" s="4" t="e">
-        <f>utilities!$H$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G19" s="4" t="e">
-        <f>utilities!$I$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H19" s="4" t="e">
-        <f>utilities!$J$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I19" s="9">
-        <f>utilities!$K$11</f>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20">
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28" s="4">
+        <v>0</v>
+      </c>
+      <c r="H28" s="4">
+        <v>0</v>
+      </c>
+      <c r="I28" s="4">
+        <v>0</v>
+      </c>
+      <c r="J28" s="9">
+        <v>0</v>
+      </c>
+      <c r="L28">
+        <f>0.9*250</f>
+        <v>225</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29">
         <v>26</v>
       </c>
-      <c r="B20">
-        <f>utilities!$H$8</f>
-        <v>0</v>
-      </c>
-      <c r="C20">
-        <f>utilities!$I$8</f>
-        <v>0</v>
-      </c>
-      <c r="D20">
-        <f>utilities!$J$8</f>
-        <v>0</v>
-      </c>
-      <c r="E20">
-        <v>0</v>
-      </c>
-      <c r="F20" s="4" t="e">
-        <f>utilities!$H$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G20" s="4" t="e">
-        <f>utilities!$I$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H20" s="4" t="e">
-        <f>utilities!$J$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I20" s="9">
-        <f>utilities!$K$11</f>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21">
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29" s="4">
+        <v>0</v>
+      </c>
+      <c r="H29" s="4">
+        <v>0</v>
+      </c>
+      <c r="I29" s="4">
+        <v>0</v>
+      </c>
+      <c r="J29" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30">
         <v>27</v>
       </c>
-      <c r="B21">
-        <f>utilities!$H$8</f>
-        <v>0</v>
-      </c>
-      <c r="C21">
-        <f>utilities!$I$8</f>
-        <v>0</v>
-      </c>
-      <c r="D21">
-        <f>utilities!$J$8</f>
-        <v>0</v>
-      </c>
-      <c r="E21">
-        <v>0</v>
-      </c>
-      <c r="F21" s="4" t="e">
-        <f>utilities!$H$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G21" s="4" t="e">
-        <f>utilities!$I$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H21" s="4" t="e">
-        <f>utilities!$J$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I21" s="9">
-        <f>utilities!$K$11</f>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22">
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30" s="4">
+        <v>0</v>
+      </c>
+      <c r="H30" s="4">
+        <v>0</v>
+      </c>
+      <c r="I30" s="4">
+        <v>0</v>
+      </c>
+      <c r="J30" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31">
         <v>28</v>
       </c>
-      <c r="B22">
-        <f>utilities!$H$8</f>
-        <v>0</v>
-      </c>
-      <c r="C22">
-        <f>utilities!$I$8</f>
-        <v>0</v>
-      </c>
-      <c r="D22">
-        <f>utilities!$J$8</f>
-        <v>0</v>
-      </c>
-      <c r="E22">
-        <v>0</v>
-      </c>
-      <c r="F22" s="4" t="e">
-        <f>utilities!$H$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G22" s="4" t="e">
-        <f>utilities!$I$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H22" s="4" t="e">
-        <f>utilities!$J$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I22" s="9">
-        <f>utilities!$K$11</f>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23">
+      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31" s="4">
+        <v>0</v>
+      </c>
+      <c r="H31" s="4">
+        <v>0</v>
+      </c>
+      <c r="I31" s="4">
+        <v>0</v>
+      </c>
+      <c r="J31" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32">
         <v>29</v>
       </c>
-      <c r="B23">
-        <f>utilities!$H$8</f>
-        <v>0</v>
-      </c>
-      <c r="C23">
-        <f>utilities!$I$8</f>
-        <v>0</v>
-      </c>
-      <c r="D23">
-        <f>utilities!$J$8</f>
-        <v>0</v>
-      </c>
-      <c r="E23">
-        <v>0</v>
-      </c>
-      <c r="F23" s="4" t="e">
-        <f>utilities!$H$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G23" s="4" t="e">
-        <f>utilities!$I$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H23" s="4" t="e">
-        <f>utilities!$J$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I23" s="9">
-        <f>utilities!$K$11</f>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24">
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32" s="4">
+        <v>0</v>
+      </c>
+      <c r="H32" s="4">
+        <v>0</v>
+      </c>
+      <c r="I32" s="4">
+        <v>0</v>
+      </c>
+      <c r="J32" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33">
         <v>30</v>
       </c>
-      <c r="B24">
-        <f>utilities!$H$8</f>
-        <v>0</v>
-      </c>
-      <c r="C24">
-        <f>utilities!$I$8</f>
-        <v>0</v>
-      </c>
-      <c r="D24">
-        <f>utilities!$J$8</f>
-        <v>0</v>
-      </c>
-      <c r="E24">
-        <v>0</v>
-      </c>
-      <c r="F24" s="4" t="e">
-        <f>utilities!$H$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G24" s="4" t="e">
-        <f>utilities!$I$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H24" s="4" t="e">
-        <f>utilities!$J$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I24" s="9">
-        <f>utilities!$K$11</f>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25">
+      <c r="B33">
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33" s="4">
+        <v>0</v>
+      </c>
+      <c r="H33" s="4">
+        <v>0</v>
+      </c>
+      <c r="I33" s="4">
+        <v>0</v>
+      </c>
+      <c r="J33" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34">
         <v>31</v>
       </c>
-      <c r="B25">
-        <f>utilities!$H$8</f>
-        <v>0</v>
-      </c>
-      <c r="C25">
-        <f>utilities!$I$8</f>
-        <v>0</v>
-      </c>
-      <c r="D25">
-        <f>utilities!$J$8</f>
-        <v>0</v>
-      </c>
-      <c r="E25">
-        <v>0</v>
-      </c>
-      <c r="F25" s="4" t="e">
-        <f>utilities!$H$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G25" s="4" t="e">
-        <f>utilities!$I$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H25" s="4" t="e">
-        <f>utilities!$J$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I25" s="9">
-        <f>utilities!$K$11</f>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26">
+      <c r="B34">
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34" s="4">
+        <v>0</v>
+      </c>
+      <c r="H34" s="4">
+        <v>0</v>
+      </c>
+      <c r="I34" s="4">
+        <v>0</v>
+      </c>
+      <c r="J34" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35">
         <v>32</v>
       </c>
-      <c r="B26">
-        <f>utilities!$H$8</f>
-        <v>0</v>
-      </c>
-      <c r="C26">
-        <f>utilities!$I$8</f>
-        <v>0</v>
-      </c>
-      <c r="D26">
-        <f>utilities!$J$8</f>
-        <v>0</v>
-      </c>
-      <c r="E26">
-        <v>0</v>
-      </c>
-      <c r="F26" s="4" t="e">
-        <f>utilities!$H$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G26" s="4" t="e">
-        <f>utilities!$I$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H26" s="4" t="e">
-        <f>utilities!$J$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I26" s="9">
-        <f>utilities!$K$11</f>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27">
+      <c r="B35">
+        <v>0</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35" s="4">
+        <v>0</v>
+      </c>
+      <c r="H35" s="4">
+        <v>0</v>
+      </c>
+      <c r="I35" s="4">
+        <v>0</v>
+      </c>
+      <c r="J35" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36">
         <v>33</v>
       </c>
-      <c r="B27">
-        <f>utilities!$H$8</f>
-        <v>0</v>
-      </c>
-      <c r="C27">
-        <f>utilities!$I$8</f>
-        <v>0</v>
-      </c>
-      <c r="D27">
-        <f>utilities!$J$8</f>
-        <v>0</v>
-      </c>
-      <c r="E27">
-        <v>0</v>
-      </c>
-      <c r="F27" s="4" t="e">
-        <f>utilities!$H$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G27" s="4" t="e">
-        <f>utilities!$I$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H27" s="4" t="e">
-        <f>utilities!$J$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I27" s="9">
-        <f>utilities!$K$11</f>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28">
+      <c r="B36">
+        <v>0</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="G36" s="4">
+        <v>0</v>
+      </c>
+      <c r="H36" s="4">
+        <v>0</v>
+      </c>
+      <c r="I36" s="4">
+        <v>0</v>
+      </c>
+      <c r="J36" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37">
         <v>34</v>
       </c>
-      <c r="B28">
-        <f>utilities!$H$8</f>
-        <v>0</v>
-      </c>
-      <c r="C28">
-        <f>utilities!$I$8</f>
-        <v>0</v>
-      </c>
-      <c r="D28">
-        <f>utilities!$J$8</f>
-        <v>0</v>
-      </c>
-      <c r="E28">
-        <v>0</v>
-      </c>
-      <c r="F28" s="4" t="e">
-        <f>utilities!$H$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G28" s="4" t="e">
-        <f>utilities!$I$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H28" s="4" t="e">
-        <f>utilities!$J$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I28" s="9">
-        <f>utilities!$K$11</f>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29">
+      <c r="B37">
+        <v>0</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+      <c r="G37" s="4">
+        <v>0</v>
+      </c>
+      <c r="H37" s="4">
+        <v>0</v>
+      </c>
+      <c r="I37" s="4">
+        <v>0</v>
+      </c>
+      <c r="J37" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38">
         <v>35</v>
       </c>
-      <c r="B29">
-        <f>utilities!$H$8</f>
-        <v>0</v>
-      </c>
-      <c r="C29">
-        <f>utilities!$I$8</f>
-        <v>0</v>
-      </c>
-      <c r="D29">
-        <f>utilities!$J$8</f>
-        <v>0</v>
-      </c>
-      <c r="E29">
-        <v>0</v>
-      </c>
-      <c r="F29" s="4" t="e">
-        <f>utilities!$H$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G29" s="4" t="e">
-        <f>utilities!$I$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H29" s="4" t="e">
-        <f>utilities!$J$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I29" s="9">
-        <f>utilities!$K$11</f>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30">
+      <c r="B38">
+        <v>0</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="F38">
+        <v>0</v>
+      </c>
+      <c r="G38" s="4">
+        <v>0</v>
+      </c>
+      <c r="H38" s="4">
+        <v>0</v>
+      </c>
+      <c r="I38" s="4">
+        <v>0</v>
+      </c>
+      <c r="J38" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39">
         <v>36</v>
       </c>
-      <c r="B30">
-        <f>utilities!$H$8</f>
-        <v>0</v>
-      </c>
-      <c r="C30">
-        <f>utilities!$I$8</f>
-        <v>0</v>
-      </c>
-      <c r="D30">
-        <f>utilities!$J$8</f>
-        <v>0</v>
-      </c>
-      <c r="E30">
-        <v>0</v>
-      </c>
-      <c r="F30" s="4" t="e">
-        <f>utilities!$H$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G30" s="4" t="e">
-        <f>utilities!$I$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H30" s="4" t="e">
-        <f>utilities!$J$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I30" s="9">
-        <f>utilities!$K$11</f>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31">
+      <c r="B39">
+        <v>0</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+      <c r="G39" s="4">
+        <v>0</v>
+      </c>
+      <c r="H39" s="4">
+        <v>0</v>
+      </c>
+      <c r="I39" s="4">
+        <v>0</v>
+      </c>
+      <c r="J39" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40">
         <v>37</v>
       </c>
-      <c r="B31">
-        <f>utilities!$H$8</f>
-        <v>0</v>
-      </c>
-      <c r="C31">
-        <f>utilities!$I$8</f>
-        <v>0</v>
-      </c>
-      <c r="D31">
-        <f>utilities!$J$8</f>
-        <v>0</v>
-      </c>
-      <c r="E31">
-        <v>0</v>
-      </c>
-      <c r="F31" s="4" t="e">
-        <f>utilities!$H$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G31" s="4" t="e">
-        <f>utilities!$I$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H31" s="4" t="e">
-        <f>utilities!$J$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I31" s="9">
-        <f>utilities!$K$11</f>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32">
+      <c r="B40">
+        <v>0</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+      <c r="G40" s="4">
+        <v>0</v>
+      </c>
+      <c r="H40" s="4">
+        <v>0</v>
+      </c>
+      <c r="I40" s="4">
+        <v>0</v>
+      </c>
+      <c r="J40" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41">
         <v>38</v>
       </c>
-      <c r="B32">
-        <f>utilities!$H$8</f>
-        <v>0</v>
-      </c>
-      <c r="C32">
-        <f>utilities!$I$8</f>
-        <v>0</v>
-      </c>
-      <c r="D32">
-        <f>utilities!$J$8</f>
-        <v>0</v>
-      </c>
-      <c r="E32">
-        <v>0</v>
-      </c>
-      <c r="F32" s="4" t="e">
-        <f>utilities!$H$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G32" s="4" t="e">
-        <f>utilities!$I$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H32" s="4" t="e">
-        <f>utilities!$J$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I32" s="9">
-        <f>utilities!$K$11</f>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33">
+      <c r="B41">
+        <v>0</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+      <c r="G41" s="4">
+        <v>0</v>
+      </c>
+      <c r="H41" s="4">
+        <v>0</v>
+      </c>
+      <c r="I41" s="4">
+        <v>0</v>
+      </c>
+      <c r="J41" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42">
         <v>39</v>
       </c>
-      <c r="B33">
-        <f>utilities!$H$8</f>
-        <v>0</v>
-      </c>
-      <c r="C33">
-        <f>utilities!$I$8</f>
-        <v>0</v>
-      </c>
-      <c r="D33">
-        <f>utilities!$J$8</f>
-        <v>0</v>
-      </c>
-      <c r="E33">
-        <v>0</v>
-      </c>
-      <c r="F33" s="4" t="e">
-        <f>utilities!$H$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G33" s="4" t="e">
-        <f>utilities!$I$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H33" s="4" t="e">
-        <f>utilities!$J$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I33" s="9">
-        <f>utilities!$K$11</f>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34">
+      <c r="B42">
+        <v>0</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="F42">
+        <v>0</v>
+      </c>
+      <c r="G42" s="4">
+        <v>0</v>
+      </c>
+      <c r="H42" s="4">
+        <v>0</v>
+      </c>
+      <c r="I42" s="4">
+        <v>0</v>
+      </c>
+      <c r="J42" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43">
         <v>40</v>
       </c>
-      <c r="B34">
-        <f>utilities!$H$8</f>
-        <v>0</v>
-      </c>
-      <c r="C34">
-        <f>utilities!$I$8</f>
-        <v>0</v>
-      </c>
-      <c r="D34">
-        <f>utilities!$J$8</f>
-        <v>0</v>
-      </c>
-      <c r="E34">
-        <v>0</v>
-      </c>
-      <c r="F34" s="4" t="e">
-        <f>utilities!$H$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G34" s="4" t="e">
-        <f>utilities!$I$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H34" s="4" t="e">
-        <f>utilities!$J$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I34" s="9">
-        <f>utilities!$K$11</f>
-        <v>1E-3</v>
+      <c r="B43">
+        <v>0</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+      <c r="F43">
+        <v>0</v>
+      </c>
+      <c r="G43" s="4">
+        <v>0</v>
+      </c>
+      <c r="H43" s="4">
+        <v>0</v>
+      </c>
+      <c r="I43" s="4">
+        <v>0</v>
+      </c>
+      <c r="J43" s="9">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3323,7 +3702,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{117A8B26-635D-4B40-A90B-7735D1F1002F}">
   <dimension ref="A1:W33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
sddp with real rates
</commit_message>
<xml_diff>
--- a/julia_msp/goal_data.xlsx
+++ b/julia_msp/goal_data.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matsz\programowanie\Optymalizacja_portfela\julia_msp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2877D288-B80F-4CE6-A9CB-C45CC8837513}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01991B96-17E8-4EEC-9E54-C962BAD406D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{E8CF1CA2-D953-46E5-99F4-DA96611E7E6D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E8CF1CA2-D953-46E5-99F4-DA96611E7E6D}"/>
   </bookViews>
   <sheets>
-    <sheet name="goal_data_25" sheetId="4" r:id="rId1"/>
-    <sheet name="goal_data" sheetId="5" r:id="rId2"/>
+    <sheet name="goal_data" sheetId="4" r:id="rId1"/>
+    <sheet name="goal_data_5" sheetId="5" r:id="rId2"/>
     <sheet name="utilities" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="32">
   <si>
     <t>minimum_limit</t>
   </si>
@@ -132,6 +132,9 @@
   <si>
     <t>cashflow desired</t>
   </si>
+  <si>
+    <t>cashflows</t>
+  </si>
 </sst>
 </file>
 
@@ -221,7 +224,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -243,6 +246,7 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Dziesiętny" xfId="1" builtinId="3"/>
@@ -578,19 +582,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67C203FD-C9AE-45F0-8773-EECC728085CE}">
-  <dimension ref="A1:L43"/>
+  <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="7" max="7" width="16.7109375" customWidth="1"/>
-    <col min="10" max="10" width="8.7109375" style="9"/>
+    <col min="7" max="7" width="16.6640625" customWidth="1"/>
+    <col min="10" max="10" width="8.6640625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -621,8 +625,11 @@
       <c r="J1" s="11" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -658,8 +665,12 @@
         <f>utilities!$E$11</f>
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2">
+        <f>D2-E2</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -695,8 +706,12 @@
         <f>utilities!$E$11</f>
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K3">
+        <f t="shared" ref="K3:K27" si="4">D3-E3</f>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -732,8 +747,12 @@
         <f>utilities!$E$11</f>
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K4">
+        <f t="shared" si="4"/>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -769,8 +788,12 @@
         <f>utilities!$E$11</f>
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K5">
+        <f t="shared" si="4"/>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -806,8 +829,12 @@
         <f>utilities!$E$11</f>
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K6">
+        <f t="shared" si="4"/>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -843,8 +870,12 @@
         <f>utilities!$E$11</f>
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K7">
+        <f t="shared" si="4"/>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -880,8 +911,12 @@
         <f>utilities!$E$11</f>
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K8">
+        <f t="shared" si="4"/>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -917,8 +952,12 @@
         <f>utilities!$E$11</f>
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K9">
+        <f t="shared" si="4"/>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -954,8 +993,12 @@
         <f>utilities!$E$11</f>
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K10">
+        <f t="shared" si="4"/>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -990,8 +1033,12 @@
         <f>utilities!$E$11</f>
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K11">
+        <f t="shared" si="4"/>
+        <v>148</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1027,8 +1074,12 @@
         <f>utilities!$E$11</f>
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K12">
+        <f t="shared" si="4"/>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1064,8 +1115,12 @@
         <f>utilities!$E$11</f>
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K13">
+        <f t="shared" si="4"/>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1101,8 +1156,12 @@
         <f>utilities!$E$11</f>
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K14">
+        <f t="shared" si="4"/>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1138,8 +1197,12 @@
         <f>utilities!$E$11</f>
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K15">
+        <f t="shared" si="4"/>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1175,8 +1238,12 @@
         <f>utilities!$E$11</f>
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K16">
+        <f t="shared" si="4"/>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1212,8 +1279,12 @@
         <f>utilities!$E$11</f>
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K17">
+        <f t="shared" si="4"/>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1249,8 +1320,12 @@
         <f>utilities!$E$11</f>
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K18">
+        <f t="shared" si="4"/>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1286,8 +1361,12 @@
         <f>utilities!$E$11</f>
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K19">
+        <f t="shared" si="4"/>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1323,8 +1402,12 @@
         <f>utilities!$E$11</f>
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K20">
+        <f t="shared" si="4"/>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
@@ -1360,8 +1443,12 @@
         <f>utilities!$E$11</f>
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K21">
+        <f t="shared" si="4"/>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
@@ -1397,8 +1484,12 @@
         <f>utilities!$E$11</f>
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K22">
+        <f t="shared" si="4"/>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>21</v>
       </c>
@@ -1434,8 +1525,12 @@
         <f>utilities!$E$11</f>
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K23">
+        <f t="shared" si="4"/>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>22</v>
       </c>
@@ -1471,8 +1566,12 @@
         <f>utilities!$E$11</f>
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K24">
+        <f t="shared" si="4"/>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>23</v>
       </c>
@@ -1508,8 +1607,12 @@
         <f>utilities!$E$11</f>
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K25">
+        <f t="shared" si="4"/>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>24</v>
       </c>
@@ -1545,8 +1648,12 @@
         <f>utilities!$E$11</f>
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K26">
+        <f t="shared" si="4"/>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>25</v>
       </c>
@@ -1581,12 +1688,12 @@
         <f>utilities!$E$11</f>
         <v>1E-3</v>
       </c>
-      <c r="L27">
-        <f>0.9*250</f>
-        <v>225</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K27">
+        <f t="shared" si="4"/>
+        <v>248</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -1595,11 +1702,11 @@
         <v>306</v>
       </c>
       <c r="C28">
-        <f t="shared" ref="C28:D28" si="4">SUM(C2:C27)</f>
+        <f t="shared" ref="C28:D28" si="5">SUM(C2:C27)</f>
         <v>433</v>
       </c>
       <c r="D28">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>634</v>
       </c>
       <c r="E28">
@@ -1609,8 +1716,12 @@
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
       <c r="I28" s="4"/>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K28" s="15" t="e">
+        <f>IRR(K2:K27)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>26</v>
       </c>
@@ -1650,7 +1761,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>27</v>
       </c>
@@ -1690,7 +1801,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>28</v>
       </c>
@@ -1730,7 +1841,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>29</v>
       </c>
@@ -1770,7 +1881,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>30</v>
       </c>
@@ -1810,7 +1921,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>31</v>
       </c>
@@ -1850,7 +1961,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>32</v>
       </c>
@@ -1890,7 +2001,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>33</v>
       </c>
@@ -1930,7 +2041,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>34</v>
       </c>
@@ -1970,7 +2081,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>35</v>
       </c>
@@ -2010,7 +2121,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>36</v>
       </c>
@@ -2050,7 +2161,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>37</v>
       </c>
@@ -2090,7 +2201,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>38</v>
       </c>
@@ -2130,7 +2241,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>39</v>
       </c>
@@ -2170,7 +2281,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>40</v>
       </c>
@@ -2219,17 +2330,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F977CF0C-F948-4BB4-989B-6B75181A9A01}">
   <dimension ref="A1:L43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="7" max="7" width="16.7109375" customWidth="1"/>
-    <col min="10" max="10" width="9.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.6640625" customWidth="1"/>
+    <col min="10" max="10" width="9.5546875" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -2267,7 +2378,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2314,7 +2425,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2360,7 +2471,7 @@
         <v>-10</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2406,7 +2517,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2452,7 +2563,7 @@
         <v>-10</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2498,7 +2609,7 @@
         <v>-10</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2544,7 +2655,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B8">
         <f t="shared" ref="B8:D8" si="6">SUM(B2:B7)</f>
         <v>306</v>
@@ -2569,7 +2680,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -2601,7 +2712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -2633,7 +2744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -2665,7 +2776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -2697,7 +2808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -2729,7 +2840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
@@ -2761,7 +2872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
@@ -2793,7 +2904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>13</v>
       </c>
@@ -2825,7 +2936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>14</v>
       </c>
@@ -2857,7 +2968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>15</v>
       </c>
@@ -2889,7 +3000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>16</v>
       </c>
@@ -2921,7 +3032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>17</v>
       </c>
@@ -2953,7 +3064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>18</v>
       </c>
@@ -2985,7 +3096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>19</v>
       </c>
@@ -3017,7 +3128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>20</v>
       </c>
@@ -3049,7 +3160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>21</v>
       </c>
@@ -3081,7 +3192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>22</v>
       </c>
@@ -3113,7 +3224,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>23</v>
       </c>
@@ -3145,7 +3256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>24</v>
       </c>
@@ -3177,7 +3288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>25</v>
       </c>
@@ -3213,7 +3324,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>26</v>
       </c>
@@ -3245,7 +3356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>27</v>
       </c>
@@ -3277,7 +3388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>28</v>
       </c>
@@ -3309,7 +3420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>29</v>
       </c>
@@ -3341,7 +3452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>30</v>
       </c>
@@ -3373,7 +3484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>31</v>
       </c>
@@ -3405,7 +3516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>32</v>
       </c>
@@ -3437,7 +3548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>33</v>
       </c>
@@ -3469,7 +3580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>34</v>
       </c>
@@ -3501,7 +3612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>35</v>
       </c>
@@ -3533,7 +3644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>36</v>
       </c>
@@ -3565,7 +3676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>37</v>
       </c>
@@ -3597,7 +3708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>38</v>
       </c>
@@ -3629,7 +3740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>39</v>
       </c>
@@ -3661,7 +3772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>40</v>
       </c>
@@ -3706,22 +3817,22 @@
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.140625" customWidth="1"/>
-    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" customWidth="1"/>
-    <col min="16" max="16" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.109375" customWidth="1"/>
+    <col min="2" max="2" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" customWidth="1"/>
+    <col min="16" max="16" width="9.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D1" s="2"/>
       <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -3732,7 +3843,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>25</v>
       </c>
@@ -3746,13 +3857,13 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" s="8"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
       <c r="D4" s="5"/>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -3766,7 +3877,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>17</v>
       </c>
@@ -3816,7 +3927,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -3875,7 +3986,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -3901,7 +4012,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -3979,7 +4090,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -4057,7 +4168,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -4087,7 +4198,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -4113,7 +4224,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -4140,7 +4251,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -4170,7 +4281,7 @@
         <v>32.550999999999995</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>23</v>
       </c>
@@ -4179,16 +4290,16 @@
         <v>96.126999999999981</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B18" s="7"/>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>27</v>
       </c>
       <c r="P21" s="10"/>
     </row>
-    <row r="22" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>9</v>
       </c>
@@ -4202,7 +4313,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>17</v>
       </c>
@@ -4252,7 +4363,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>14</v>
       </c>
@@ -4302,7 +4413,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -4328,7 +4439,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>22</v>
       </c>
@@ -4390,7 +4501,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>15</v>
       </c>
@@ -4452,7 +4563,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>18</v>
       </c>
@@ -4478,7 +4589,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>20</v>
       </c>
@@ -4504,7 +4615,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>21</v>
       </c>
@@ -4530,7 +4641,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>24</v>
       </c>
@@ -4556,7 +4667,7 @@
         <v>32.550999999999995</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
sddp with inflation to improve
</commit_message>
<xml_diff>
--- a/julia_msp/goal_data.xlsx
+++ b/julia_msp/goal_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matsz\programowanie\Optymalizacja_portfela\julia_msp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01991B96-17E8-4EEC-9E54-C962BAD406D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{909FBC86-A192-4CBD-831B-588B89316E14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E8CF1CA2-D953-46E5-99F4-DA96611E7E6D}"/>
   </bookViews>
@@ -224,7 +224,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -247,6 +247,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Dziesiętny" xfId="1" builtinId="3"/>
@@ -585,7 +586,7 @@
   <dimension ref="A1:K43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E3" sqref="E3:E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -683,8 +684,9 @@
       <c r="D3">
         <v>9</v>
       </c>
-      <c r="E3">
-        <v>11</v>
+      <c r="E3" s="16">
+        <f>11*(1+2.5%)^(A3-1)</f>
+        <v>11.274999999999999</v>
       </c>
       <c r="F3">
         <f t="shared" ref="F3:F43" si="0">1/25</f>
@@ -708,7 +710,7 @@
       </c>
       <c r="K3">
         <f t="shared" ref="K3:K27" si="4">D3-E3</f>
-        <v>-2</v>
+        <v>-2.2749999999999986</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -724,8 +726,9 @@
       <c r="D4">
         <v>9</v>
       </c>
-      <c r="E4">
-        <v>11</v>
+      <c r="E4" s="16">
+        <f>11*(1+2.5%)^(A4-1)</f>
+        <v>11.556875</v>
       </c>
       <c r="F4">
         <f t="shared" si="0"/>
@@ -749,7 +752,7 @@
       </c>
       <c r="K4">
         <f t="shared" si="4"/>
-        <v>-2</v>
+        <v>-2.5568749999999998</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -765,8 +768,9 @@
       <c r="D5">
         <v>9</v>
       </c>
-      <c r="E5">
-        <v>11</v>
+      <c r="E5" s="16">
+        <f t="shared" ref="E5:E27" si="5">11*(1+2.5%)^(A5-1)</f>
+        <v>11.845796874999998</v>
       </c>
       <c r="F5">
         <f t="shared" si="0"/>
@@ -790,7 +794,7 @@
       </c>
       <c r="K5">
         <f t="shared" si="4"/>
-        <v>-2</v>
+        <v>-2.8457968749999978</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -806,8 +810,9 @@
       <c r="D6">
         <v>9</v>
       </c>
-      <c r="E6">
-        <v>11</v>
+      <c r="E6" s="16">
+        <f t="shared" si="5"/>
+        <v>12.141941796874997</v>
       </c>
       <c r="F6">
         <f t="shared" si="0"/>
@@ -831,7 +836,7 @@
       </c>
       <c r="K6">
         <f t="shared" si="4"/>
-        <v>-2</v>
+        <v>-3.1419417968749972</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -847,8 +852,9 @@
       <c r="D7">
         <v>9</v>
       </c>
-      <c r="E7">
-        <v>11</v>
+      <c r="E7" s="16">
+        <f t="shared" si="5"/>
+        <v>12.445490341796871</v>
       </c>
       <c r="F7">
         <f t="shared" si="0"/>
@@ -872,7 +878,7 @@
       </c>
       <c r="K7">
         <f t="shared" si="4"/>
-        <v>-2</v>
+        <v>-3.4454903417968712</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -888,8 +894,9 @@
       <c r="D8">
         <v>9</v>
       </c>
-      <c r="E8">
-        <v>11</v>
+      <c r="E8" s="16">
+        <f t="shared" si="5"/>
+        <v>12.756627600341792</v>
       </c>
       <c r="F8">
         <f t="shared" si="0"/>
@@ -913,7 +920,7 @@
       </c>
       <c r="K8">
         <f t="shared" si="4"/>
-        <v>-2</v>
+        <v>-3.7566276003417922</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -929,8 +936,9 @@
       <c r="D9">
         <v>9</v>
       </c>
-      <c r="E9">
-        <v>11</v>
+      <c r="E9" s="16">
+        <f t="shared" si="5"/>
+        <v>13.075543290350337</v>
       </c>
       <c r="F9">
         <f t="shared" si="0"/>
@@ -954,7 +962,7 @@
       </c>
       <c r="K9">
         <f t="shared" si="4"/>
-        <v>-2</v>
+        <v>-4.0755432903503372</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -970,8 +978,9 @@
       <c r="D10">
         <v>9</v>
       </c>
-      <c r="E10">
-        <v>11</v>
+      <c r="E10" s="16">
+        <f t="shared" si="5"/>
+        <v>13.402431872609094</v>
       </c>
       <c r="F10">
         <f t="shared" si="0"/>
@@ -995,7 +1004,7 @@
       </c>
       <c r="K10">
         <f t="shared" si="4"/>
-        <v>-2</v>
+        <v>-4.4024318726090943</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -1011,8 +1020,9 @@
       <c r="D11">
         <v>159</v>
       </c>
-      <c r="E11">
-        <v>11</v>
+      <c r="E11" s="16">
+        <f t="shared" si="5"/>
+        <v>13.73749266942432</v>
       </c>
       <c r="F11">
         <v>1</v>
@@ -1035,7 +1045,7 @@
       </c>
       <c r="K11">
         <f t="shared" si="4"/>
-        <v>148</v>
+        <v>145.26250733057569</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -1051,8 +1061,9 @@
       <c r="D12">
         <v>9</v>
       </c>
-      <c r="E12">
-        <v>11</v>
+      <c r="E12" s="16">
+        <f t="shared" si="5"/>
+        <v>14.080929986159928</v>
       </c>
       <c r="F12">
         <f t="shared" si="0"/>
@@ -1076,7 +1087,7 @@
       </c>
       <c r="K12">
         <f t="shared" si="4"/>
-        <v>-2</v>
+        <v>-5.0809299861599282</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -1092,8 +1103,9 @@
       <c r="D13">
         <v>9</v>
       </c>
-      <c r="E13">
-        <v>11</v>
+      <c r="E13" s="16">
+        <f t="shared" si="5"/>
+        <v>14.432953235813926</v>
       </c>
       <c r="F13">
         <f t="shared" si="0"/>
@@ -1117,7 +1129,7 @@
       </c>
       <c r="K13">
         <f t="shared" si="4"/>
-        <v>-2</v>
+        <v>-5.4329532358139261</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -1133,8 +1145,9 @@
       <c r="D14">
         <v>9</v>
       </c>
-      <c r="E14">
-        <v>11</v>
+      <c r="E14" s="16">
+        <f t="shared" si="5"/>
+        <v>14.793777066709273</v>
       </c>
       <c r="F14">
         <f t="shared" si="0"/>
@@ -1158,7 +1171,7 @@
       </c>
       <c r="K14">
         <f t="shared" si="4"/>
-        <v>-2</v>
+        <v>-5.7937770667092732</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -1174,8 +1187,9 @@
       <c r="D15">
         <v>9</v>
       </c>
-      <c r="E15">
-        <v>11</v>
+      <c r="E15" s="16">
+        <f t="shared" si="5"/>
+        <v>14.793777066709273</v>
       </c>
       <c r="F15">
         <f t="shared" si="0"/>
@@ -1199,7 +1213,7 @@
       </c>
       <c r="K15">
         <f t="shared" si="4"/>
-        <v>-2</v>
+        <v>-5.7937770667092732</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -1215,8 +1229,9 @@
       <c r="D16">
         <v>9</v>
       </c>
-      <c r="E16">
-        <v>11</v>
+      <c r="E16" s="16">
+        <f t="shared" si="5"/>
+        <v>15.163621493377004</v>
       </c>
       <c r="F16">
         <f t="shared" si="0"/>
@@ -1240,7 +1255,7 @@
       </c>
       <c r="K16">
         <f t="shared" si="4"/>
-        <v>-2</v>
+        <v>-6.1636214933770042</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
@@ -1256,8 +1271,9 @@
       <c r="D17">
         <v>9</v>
       </c>
-      <c r="E17">
-        <v>11</v>
+      <c r="E17" s="16">
+        <f t="shared" si="5"/>
+        <v>15.542712030711428</v>
       </c>
       <c r="F17">
         <f t="shared" si="0"/>
@@ -1281,7 +1297,7 @@
       </c>
       <c r="K17">
         <f t="shared" si="4"/>
-        <v>-2</v>
+        <v>-6.5427120307114279</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
@@ -1297,8 +1313,9 @@
       <c r="D18">
         <v>9</v>
       </c>
-      <c r="E18">
-        <v>11</v>
+      <c r="E18" s="16">
+        <f t="shared" si="5"/>
+        <v>15.931279831479216</v>
       </c>
       <c r="F18">
         <f t="shared" si="0"/>
@@ -1322,7 +1339,7 @@
       </c>
       <c r="K18">
         <f t="shared" si="4"/>
-        <v>-2</v>
+        <v>-6.9312798314792161</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
@@ -1338,8 +1355,9 @@
       <c r="D19">
         <v>9</v>
       </c>
-      <c r="E19">
-        <v>11</v>
+      <c r="E19" s="16">
+        <f t="shared" si="5"/>
+        <v>16.329561827266193</v>
       </c>
       <c r="F19">
         <f t="shared" si="0"/>
@@ -1363,7 +1381,7 @@
       </c>
       <c r="K19">
         <f t="shared" si="4"/>
-        <v>-2</v>
+        <v>-7.3295618272661933</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
@@ -1379,8 +1397,9 @@
       <c r="D20">
         <v>9</v>
       </c>
-      <c r="E20">
-        <v>11</v>
+      <c r="E20" s="16">
+        <f t="shared" si="5"/>
+        <v>16.737800872947847</v>
       </c>
       <c r="F20">
         <f t="shared" si="0"/>
@@ -1404,7 +1423,7 @@
       </c>
       <c r="K20">
         <f t="shared" si="4"/>
-        <v>-2</v>
+        <v>-7.7378008729478474</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
@@ -1420,8 +1439,9 @@
       <c r="D21">
         <v>9</v>
       </c>
-      <c r="E21">
-        <v>11</v>
+      <c r="E21" s="16">
+        <f t="shared" si="5"/>
+        <v>17.156245894771544</v>
       </c>
       <c r="F21">
         <f t="shared" si="0"/>
@@ -1445,7 +1465,7 @@
       </c>
       <c r="K21">
         <f t="shared" si="4"/>
-        <v>-2</v>
+        <v>-8.1562458947715442</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
@@ -1461,8 +1481,9 @@
       <c r="D22">
         <v>9</v>
       </c>
-      <c r="E22">
-        <v>11</v>
+      <c r="E22" s="16">
+        <f t="shared" si="5"/>
+        <v>17.585152042140834</v>
       </c>
       <c r="F22">
         <f t="shared" si="0"/>
@@ -1486,7 +1507,7 @@
       </c>
       <c r="K22">
         <f t="shared" si="4"/>
-        <v>-2</v>
+        <v>-8.5851520421408338</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
@@ -1502,8 +1523,9 @@
       <c r="D23">
         <v>9</v>
       </c>
-      <c r="E23">
-        <v>11</v>
+      <c r="E23" s="16">
+        <f t="shared" si="5"/>
+        <v>18.02478084319435</v>
       </c>
       <c r="F23">
         <f t="shared" si="0"/>
@@ -1527,7 +1549,7 @@
       </c>
       <c r="K23">
         <f t="shared" si="4"/>
-        <v>-2</v>
+        <v>-9.0247808431943497</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
@@ -1543,8 +1565,9 @@
       <c r="D24">
         <v>9</v>
       </c>
-      <c r="E24">
-        <v>11</v>
+      <c r="E24" s="16">
+        <f t="shared" si="5"/>
+        <v>18.475400364274208</v>
       </c>
       <c r="F24">
         <f t="shared" si="0"/>
@@ -1568,7 +1591,7 @@
       </c>
       <c r="K24">
         <f t="shared" si="4"/>
-        <v>-2</v>
+        <v>-9.4754003642742077</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
@@ -1584,8 +1607,9 @@
       <c r="D25">
         <v>9</v>
       </c>
-      <c r="E25">
-        <v>11</v>
+      <c r="E25" s="16">
+        <f t="shared" si="5"/>
+        <v>18.937285373381062</v>
       </c>
       <c r="F25">
         <f t="shared" si="0"/>
@@ -1609,7 +1633,7 @@
       </c>
       <c r="K25">
         <f t="shared" si="4"/>
-        <v>-2</v>
+        <v>-9.9372853733810622</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
@@ -1625,8 +1649,9 @@
       <c r="D26">
         <v>9</v>
       </c>
-      <c r="E26">
-        <v>11</v>
+      <c r="E26" s="16">
+        <f t="shared" si="5"/>
+        <v>19.410717507715589</v>
       </c>
       <c r="F26">
         <f t="shared" si="0"/>
@@ -1650,7 +1675,7 @@
       </c>
       <c r="K26">
         <f t="shared" si="4"/>
-        <v>-2</v>
+        <v>-10.410717507715589</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
@@ -1666,8 +1691,9 @@
       <c r="D27">
         <v>259</v>
       </c>
-      <c r="E27">
-        <v>11</v>
+      <c r="E27" s="16">
+        <f t="shared" si="5"/>
+        <v>19.895985445408478</v>
       </c>
       <c r="F27">
         <v>1</v>
@@ -1690,7 +1716,7 @@
       </c>
       <c r="K27">
         <f t="shared" si="4"/>
-        <v>248</v>
+        <v>239.10401455459152</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
@@ -1702,16 +1728,16 @@
         <v>306</v>
       </c>
       <c r="C28">
-        <f t="shared" ref="C28:D28" si="5">SUM(C2:C27)</f>
+        <f t="shared" ref="C28:D28" si="6">SUM(C2:C27)</f>
         <v>433</v>
       </c>
       <c r="D28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>634</v>
       </c>
       <c r="E28">
         <f>SUM(E2:E27)</f>
-        <v>275</v>
+        <v>379.52918032845758</v>
       </c>
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>

</xml_diff>

<commit_message>
refactor sdd goal investing
</commit_message>
<xml_diff>
--- a/julia_msp/goal_data.xlsx
+++ b/julia_msp/goal_data.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matsz\programowanie\Optymalizacja_portfela\julia_msp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF444372-507A-4518-A468-CFBB0D4D674D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D461FBA-EBA0-4AB1-A1E5-95AD43F59EAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{E8CF1CA2-D953-46E5-99F4-DA96611E7E6D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E8CF1CA2-D953-46E5-99F4-DA96611E7E6D}"/>
   </bookViews>
   <sheets>
-    <sheet name="goal_data_save" sheetId="6" r:id="rId1"/>
+    <sheet name="goal_data_single_goal" sheetId="7" r:id="rId1"/>
     <sheet name="goal_data" sheetId="4" r:id="rId2"/>
-    <sheet name="goal_data_5" sheetId="5" r:id="rId3"/>
-    <sheet name="utilities" sheetId="2" r:id="rId4"/>
+    <sheet name="goal_data_save" sheetId="6" r:id="rId3"/>
+    <sheet name="goal_data_5" sheetId="5" r:id="rId4"/>
+    <sheet name="utilities" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="32">
   <si>
     <t>minimum_limit</t>
   </si>
@@ -583,11 +584,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C37F228-CE9B-4855-94EE-55EF65F52467}">
-  <dimension ref="A1:K43"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48F546F3-B2EF-4B4F-8BCE-C8A1CCE3A596}">
+  <dimension ref="A1:L42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -647,29 +648,29 @@
       <c r="E2">
         <v>0</v>
       </c>
-      <c r="F2">
-        <f>1/25</f>
-        <v>0.04</v>
+      <c r="F2" s="16">
+        <f>1/15</f>
+        <v>6.6666666666666666E-2</v>
       </c>
       <c r="G2" s="4">
         <f>(25*F2)/B2</f>
-        <v>0.16666666666666666</v>
+        <v>0.27777777777777779</v>
       </c>
       <c r="H2" s="4">
         <f>(5*F2)/(C2-B2)</f>
-        <v>0.1</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="I2" s="4">
         <f>(1*F2)/(D2-C2)</f>
-        <v>0.04</v>
+        <v>6.6666666666666666E-2</v>
       </c>
       <c r="J2" s="9">
         <f>utilities!$E$11</f>
         <v>1E-3</v>
       </c>
       <c r="K2">
-        <f>D2-E2</f>
-        <v>9</v>
+        <f>-(D2-E2)</f>
+        <v>-9</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -686,32 +687,32 @@
         <v>9</v>
       </c>
       <c r="E3" s="16">
-        <f>11*(1+2.5%)^(A3-1)</f>
-        <v>11.274999999999999</v>
-      </c>
-      <c r="F3">
-        <f t="shared" ref="F3:F43" si="0">1/25</f>
-        <v>0.04</v>
+        <f>11</f>
+        <v>11</v>
+      </c>
+      <c r="F3" s="16">
+        <f t="shared" ref="F3:F16" si="0">1/15</f>
+        <v>6.6666666666666666E-2</v>
       </c>
       <c r="G3" s="4">
-        <f t="shared" ref="G3:G27" si="1">(25*F3)/B3</f>
+        <f t="shared" ref="G3:G17" si="1">(25*F3)/B3</f>
+        <v>0.27777777777777779</v>
+      </c>
+      <c r="H3" s="4">
+        <f t="shared" ref="H3:H17" si="2">(5*F3)/(C3-B3)</f>
         <v>0.16666666666666666</v>
       </c>
-      <c r="H3" s="4">
-        <f t="shared" ref="H3:H27" si="2">(5*F3)/(C3-B3)</f>
-        <v>0.1</v>
-      </c>
       <c r="I3" s="4">
-        <f t="shared" ref="I3:I27" si="3">(1*F3)/(D3-C3)</f>
-        <v>0.04</v>
+        <f t="shared" ref="I3:I17" si="3">(1*F3)/(D3-C3)</f>
+        <v>6.6666666666666666E-2</v>
       </c>
       <c r="J3" s="9">
         <f>utilities!$E$11</f>
         <v>1E-3</v>
       </c>
       <c r="K3">
-        <f t="shared" ref="K3:K27" si="4">D3-E3</f>
-        <v>-2.2749999999999986</v>
+        <f t="shared" ref="K3:K16" si="4">D3-E3</f>
+        <v>-2</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -728,24 +729,24 @@
         <v>9</v>
       </c>
       <c r="E4" s="16">
-        <f>11*(1+2.5%)^(A4-1)</f>
-        <v>11.556875</v>
-      </c>
-      <c r="F4">
+        <f>11</f>
+        <v>11</v>
+      </c>
+      <c r="F4" s="16">
         <f t="shared" si="0"/>
-        <v>0.04</v>
+        <v>6.6666666666666666E-2</v>
       </c>
       <c r="G4" s="4">
         <f t="shared" si="1"/>
-        <v>0.16666666666666666</v>
+        <v>0.27777777777777779</v>
       </c>
       <c r="H4" s="4">
         <f t="shared" si="2"/>
-        <v>0.1</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="I4" s="4">
         <f t="shared" si="3"/>
-        <v>0.04</v>
+        <v>6.6666666666666666E-2</v>
       </c>
       <c r="J4" s="9">
         <f>utilities!$E$11</f>
@@ -753,7 +754,7 @@
       </c>
       <c r="K4">
         <f t="shared" si="4"/>
-        <v>-2.5568749999999998</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -770,24 +771,24 @@
         <v>9</v>
       </c>
       <c r="E5" s="16">
-        <f t="shared" ref="E5:E27" si="5">11*(1+2.5%)^(A5-1)</f>
-        <v>11.845796874999998</v>
-      </c>
-      <c r="F5">
+        <f>11</f>
+        <v>11</v>
+      </c>
+      <c r="F5" s="16">
         <f t="shared" si="0"/>
-        <v>0.04</v>
+        <v>6.6666666666666666E-2</v>
       </c>
       <c r="G5" s="4">
         <f t="shared" si="1"/>
-        <v>0.16666666666666666</v>
+        <v>0.27777777777777779</v>
       </c>
       <c r="H5" s="4">
         <f t="shared" si="2"/>
-        <v>0.1</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="I5" s="4">
         <f t="shared" si="3"/>
-        <v>0.04</v>
+        <v>6.6666666666666666E-2</v>
       </c>
       <c r="J5" s="9">
         <f>utilities!$E$11</f>
@@ -795,7 +796,7 @@
       </c>
       <c r="K5">
         <f t="shared" si="4"/>
-        <v>-2.8457968749999978</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -812,24 +813,24 @@
         <v>9</v>
       </c>
       <c r="E6" s="16">
-        <f t="shared" si="5"/>
-        <v>12.141941796874997</v>
-      </c>
-      <c r="F6">
+        <f>11</f>
+        <v>11</v>
+      </c>
+      <c r="F6" s="16">
         <f t="shared" si="0"/>
-        <v>0.04</v>
+        <v>6.6666666666666666E-2</v>
       </c>
       <c r="G6" s="4">
         <f t="shared" si="1"/>
-        <v>0.16666666666666666</v>
+        <v>0.27777777777777779</v>
       </c>
       <c r="H6" s="4">
         <f t="shared" si="2"/>
-        <v>0.1</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="I6" s="4">
         <f t="shared" si="3"/>
-        <v>0.04</v>
+        <v>6.6666666666666666E-2</v>
       </c>
       <c r="J6" s="9">
         <f>utilities!$E$11</f>
@@ -837,7 +838,7 @@
       </c>
       <c r="K6">
         <f t="shared" si="4"/>
-        <v>-3.1419417968749972</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -854,24 +855,24 @@
         <v>9</v>
       </c>
       <c r="E7" s="16">
-        <f t="shared" si="5"/>
-        <v>12.445490341796871</v>
-      </c>
-      <c r="F7">
+        <f>11</f>
+        <v>11</v>
+      </c>
+      <c r="F7" s="16">
         <f t="shared" si="0"/>
-        <v>0.04</v>
+        <v>6.6666666666666666E-2</v>
       </c>
       <c r="G7" s="4">
         <f t="shared" si="1"/>
-        <v>0.16666666666666666</v>
+        <v>0.27777777777777779</v>
       </c>
       <c r="H7" s="4">
         <f t="shared" si="2"/>
-        <v>0.1</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="I7" s="4">
         <f t="shared" si="3"/>
-        <v>0.04</v>
+        <v>6.6666666666666666E-2</v>
       </c>
       <c r="J7" s="9">
         <f>utilities!$E$11</f>
@@ -879,7 +880,7 @@
       </c>
       <c r="K7">
         <f t="shared" si="4"/>
-        <v>-3.4454903417968712</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -896,24 +897,24 @@
         <v>9</v>
       </c>
       <c r="E8" s="16">
-        <f t="shared" si="5"/>
-        <v>12.756627600341792</v>
-      </c>
-      <c r="F8">
+        <f>11</f>
+        <v>11</v>
+      </c>
+      <c r="F8" s="16">
         <f t="shared" si="0"/>
-        <v>0.04</v>
+        <v>6.6666666666666666E-2</v>
       </c>
       <c r="G8" s="4">
         <f t="shared" si="1"/>
-        <v>0.16666666666666666</v>
+        <v>0.27777777777777779</v>
       </c>
       <c r="H8" s="4">
         <f t="shared" si="2"/>
-        <v>0.1</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="I8" s="4">
         <f t="shared" si="3"/>
-        <v>0.04</v>
+        <v>6.6666666666666666E-2</v>
       </c>
       <c r="J8" s="9">
         <f>utilities!$E$11</f>
@@ -921,7 +922,7 @@
       </c>
       <c r="K8">
         <f t="shared" si="4"/>
-        <v>-3.7566276003417922</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -938,24 +939,24 @@
         <v>9</v>
       </c>
       <c r="E9" s="16">
-        <f t="shared" si="5"/>
-        <v>13.075543290350337</v>
-      </c>
-      <c r="F9">
+        <f>11</f>
+        <v>11</v>
+      </c>
+      <c r="F9" s="16">
         <f t="shared" si="0"/>
-        <v>0.04</v>
+        <v>6.6666666666666666E-2</v>
       </c>
       <c r="G9" s="4">
         <f t="shared" si="1"/>
-        <v>0.16666666666666666</v>
+        <v>0.27777777777777779</v>
       </c>
       <c r="H9" s="4">
         <f t="shared" si="2"/>
-        <v>0.1</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="I9" s="4">
         <f t="shared" si="3"/>
-        <v>0.04</v>
+        <v>6.6666666666666666E-2</v>
       </c>
       <c r="J9" s="9">
         <f>utilities!$E$11</f>
@@ -963,7 +964,7 @@
       </c>
       <c r="K9">
         <f t="shared" si="4"/>
-        <v>-4.0755432903503372</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -980,24 +981,24 @@
         <v>9</v>
       </c>
       <c r="E10" s="16">
-        <f t="shared" si="5"/>
-        <v>13.402431872609094</v>
-      </c>
-      <c r="F10">
+        <f>11</f>
+        <v>11</v>
+      </c>
+      <c r="F10" s="16">
         <f t="shared" si="0"/>
-        <v>0.04</v>
+        <v>6.6666666666666666E-2</v>
       </c>
       <c r="G10" s="4">
         <f t="shared" si="1"/>
-        <v>0.16666666666666666</v>
+        <v>0.27777777777777779</v>
       </c>
       <c r="H10" s="4">
         <f t="shared" si="2"/>
-        <v>0.1</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="I10" s="4">
         <f t="shared" si="3"/>
-        <v>0.04</v>
+        <v>6.6666666666666666E-2</v>
       </c>
       <c r="J10" s="9">
         <f>utilities!$E$11</f>
@@ -1005,7 +1006,7 @@
       </c>
       <c r="K10">
         <f t="shared" si="4"/>
-        <v>-4.4024318726090943</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -1013,32 +1014,33 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="C11">
-        <v>98</v>
+        <v>8</v>
       </c>
       <c r="D11">
-        <v>159</v>
+        <v>9</v>
       </c>
       <c r="E11" s="16">
-        <f t="shared" si="5"/>
-        <v>13.73749266942432</v>
-      </c>
-      <c r="F11">
-        <v>1</v>
+        <f>11</f>
+        <v>11</v>
+      </c>
+      <c r="F11" s="16">
+        <f t="shared" si="0"/>
+        <v>6.6666666666666666E-2</v>
       </c>
       <c r="G11" s="4">
         <f t="shared" si="1"/>
-        <v>0.37878787878787878</v>
+        <v>0.27777777777777779</v>
       </c>
       <c r="H11" s="4">
         <f t="shared" si="2"/>
-        <v>0.15625</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="I11" s="4">
         <f t="shared" si="3"/>
-        <v>1.6393442622950821E-2</v>
+        <v>6.6666666666666666E-2</v>
       </c>
       <c r="J11" s="9">
         <f>utilities!$E$11</f>
@@ -1046,7 +1048,7 @@
       </c>
       <c r="K11">
         <f t="shared" si="4"/>
-        <v>145.26250733057569</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -1063,24 +1065,24 @@
         <v>9</v>
       </c>
       <c r="E12" s="16">
-        <f t="shared" si="5"/>
-        <v>14.080929986159928</v>
-      </c>
-      <c r="F12">
+        <f>11</f>
+        <v>11</v>
+      </c>
+      <c r="F12" s="16">
         <f t="shared" si="0"/>
-        <v>0.04</v>
+        <v>6.6666666666666666E-2</v>
       </c>
       <c r="G12" s="4">
         <f t="shared" si="1"/>
-        <v>0.16666666666666666</v>
+        <v>0.27777777777777779</v>
       </c>
       <c r="H12" s="4">
         <f t="shared" si="2"/>
-        <v>0.1</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="I12" s="4">
         <f t="shared" si="3"/>
-        <v>0.04</v>
+        <v>6.6666666666666666E-2</v>
       </c>
       <c r="J12" s="9">
         <f>utilities!$E$11</f>
@@ -1088,7 +1090,7 @@
       </c>
       <c r="K12">
         <f t="shared" si="4"/>
-        <v>-5.0809299861599282</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -1105,24 +1107,24 @@
         <v>9</v>
       </c>
       <c r="E13" s="16">
-        <f t="shared" si="5"/>
-        <v>14.432953235813926</v>
-      </c>
-      <c r="F13">
+        <f>11</f>
+        <v>11</v>
+      </c>
+      <c r="F13" s="16">
         <f t="shared" si="0"/>
-        <v>0.04</v>
+        <v>6.6666666666666666E-2</v>
       </c>
       <c r="G13" s="4">
         <f t="shared" si="1"/>
-        <v>0.16666666666666666</v>
+        <v>0.27777777777777779</v>
       </c>
       <c r="H13" s="4">
         <f t="shared" si="2"/>
-        <v>0.1</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="I13" s="4">
         <f t="shared" si="3"/>
-        <v>0.04</v>
+        <v>6.6666666666666666E-2</v>
       </c>
       <c r="J13" s="9">
         <f>utilities!$E$11</f>
@@ -1130,7 +1132,7 @@
       </c>
       <c r="K13">
         <f t="shared" si="4"/>
-        <v>-5.4329532358139261</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -1147,24 +1149,24 @@
         <v>9</v>
       </c>
       <c r="E14" s="16">
-        <f t="shared" si="5"/>
-        <v>14.793777066709273</v>
-      </c>
-      <c r="F14">
+        <f>11</f>
+        <v>11</v>
+      </c>
+      <c r="F14" s="16">
         <f t="shared" si="0"/>
-        <v>0.04</v>
+        <v>6.6666666666666666E-2</v>
       </c>
       <c r="G14" s="4">
         <f t="shared" si="1"/>
-        <v>0.16666666666666666</v>
+        <v>0.27777777777777779</v>
       </c>
       <c r="H14" s="4">
         <f t="shared" si="2"/>
-        <v>0.1</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="I14" s="4">
         <f t="shared" si="3"/>
-        <v>0.04</v>
+        <v>6.6666666666666666E-2</v>
       </c>
       <c r="J14" s="9">
         <f>utilities!$E$11</f>
@@ -1172,12 +1174,12 @@
       </c>
       <c r="K14">
         <f t="shared" si="4"/>
-        <v>-5.7937770667092732</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B15">
         <v>6</v>
@@ -1189,24 +1191,24 @@
         <v>9</v>
       </c>
       <c r="E15" s="16">
-        <f t="shared" si="5"/>
-        <v>14.793777066709273</v>
-      </c>
-      <c r="F15">
+        <f>11</f>
+        <v>11</v>
+      </c>
+      <c r="F15" s="16">
         <f t="shared" si="0"/>
-        <v>0.04</v>
+        <v>6.6666666666666666E-2</v>
       </c>
       <c r="G15" s="4">
         <f t="shared" si="1"/>
-        <v>0.16666666666666666</v>
+        <v>0.27777777777777779</v>
       </c>
       <c r="H15" s="4">
         <f t="shared" si="2"/>
-        <v>0.1</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="I15" s="4">
         <f t="shared" si="3"/>
-        <v>0.04</v>
+        <v>6.6666666666666666E-2</v>
       </c>
       <c r="J15" s="9">
         <f>utilities!$E$11</f>
@@ -1214,12 +1216,12 @@
       </c>
       <c r="K15">
         <f t="shared" si="4"/>
-        <v>-5.7937770667092732</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B16">
         <v>6</v>
@@ -1231,24 +1233,24 @@
         <v>9</v>
       </c>
       <c r="E16" s="16">
-        <f t="shared" si="5"/>
-        <v>15.163621493377004</v>
-      </c>
-      <c r="F16">
+        <f>11</f>
+        <v>11</v>
+      </c>
+      <c r="F16" s="16">
         <f t="shared" si="0"/>
-        <v>0.04</v>
+        <v>6.6666666666666666E-2</v>
       </c>
       <c r="G16" s="4">
         <f t="shared" si="1"/>
-        <v>0.16666666666666666</v>
+        <v>0.27777777777777779</v>
       </c>
       <c r="H16" s="4">
         <f t="shared" si="2"/>
-        <v>0.1</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="I16" s="4">
         <f t="shared" si="3"/>
-        <v>0.04</v>
+        <v>6.6666666666666666E-2</v>
       </c>
       <c r="J16" s="9">
         <f>utilities!$E$11</f>
@@ -1256,501 +1258,215 @@
       </c>
       <c r="K16">
         <f t="shared" si="4"/>
-        <v>-6.1636214933770042</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B17">
-        <v>6</v>
+        <v>81</v>
       </c>
       <c r="C17">
-        <v>8</v>
+        <v>128</v>
       </c>
       <c r="D17">
-        <v>9</v>
+        <v>159</v>
       </c>
       <c r="E17" s="16">
-        <f t="shared" si="5"/>
-        <v>15.542712030711428</v>
-      </c>
-      <c r="F17">
-        <f t="shared" si="0"/>
-        <v>0.04</v>
+        <f>11</f>
+        <v>11</v>
+      </c>
+      <c r="F17" s="16">
+        <v>1</v>
       </c>
       <c r="G17" s="4">
         <f t="shared" si="1"/>
-        <v>0.16666666666666666</v>
+        <v>0.30864197530864196</v>
       </c>
       <c r="H17" s="4">
         <f t="shared" si="2"/>
-        <v>0.1</v>
+        <v>0.10638297872340426</v>
       </c>
       <c r="I17" s="4">
         <f t="shared" si="3"/>
-        <v>0.04</v>
+        <v>3.2258064516129031E-2</v>
       </c>
       <c r="J17" s="9">
         <f>utilities!$E$11</f>
         <v>1E-3</v>
       </c>
-      <c r="K17">
-        <f t="shared" si="4"/>
-        <v>-6.5427120307114279</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18">
-        <v>16</v>
-      </c>
-      <c r="B18">
-        <v>6</v>
-      </c>
-      <c r="C18">
+      <c r="K17" s="16">
+        <f>D17-E17</f>
+        <v>148</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="E18" s="16"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="K18">
+        <f>SUM(K2:K17)</f>
+        <v>111</v>
+      </c>
+      <c r="L18" s="15">
+        <f>IRR(K2:K17)</f>
+        <v>0.13875755605827766</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="E19" s="16"/>
+      <c r="G19" s="4">
+        <f>SUMPRODUCT(B2:B17,G2:G17)</f>
+        <v>50</v>
+      </c>
+      <c r="H19" s="4">
+        <v>10</v>
+      </c>
+      <c r="I19" s="4">
+        <v>1</v>
+      </c>
+      <c r="J19" s="9">
+        <f>SUM(J2:J17)</f>
+        <v>1.6000000000000007E-2</v>
+      </c>
+      <c r="K19" s="4">
+        <f>SUM(G19:J19)</f>
+        <v>61.015999999999998</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="E20" s="16">
         <v>8</v>
       </c>
-      <c r="D18">
-        <v>9</v>
-      </c>
-      <c r="E18" s="16">
-        <f t="shared" si="5"/>
-        <v>15.931279831479216</v>
-      </c>
-      <c r="F18">
-        <f t="shared" si="0"/>
-        <v>0.04</v>
-      </c>
-      <c r="G18" s="4">
-        <f t="shared" si="1"/>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="H18" s="4">
-        <f t="shared" si="2"/>
-        <v>0.1</v>
-      </c>
-      <c r="I18" s="4">
-        <f t="shared" si="3"/>
-        <v>0.04</v>
-      </c>
-      <c r="J18" s="9">
-        <f>utilities!$E$11</f>
-        <v>1E-3</v>
-      </c>
-      <c r="K18">
-        <f t="shared" si="4"/>
-        <v>-6.9312798314792161</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19">
-        <v>17</v>
-      </c>
-      <c r="B19">
-        <v>6</v>
-      </c>
-      <c r="C19">
-        <v>8</v>
-      </c>
-      <c r="D19">
-        <v>9</v>
-      </c>
-      <c r="E19" s="16">
-        <f t="shared" si="5"/>
-        <v>16.329561827266193</v>
-      </c>
-      <c r="F19">
-        <f t="shared" si="0"/>
-        <v>0.04</v>
-      </c>
-      <c r="G19" s="4">
-        <f t="shared" si="1"/>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="H19" s="4">
-        <f t="shared" si="2"/>
-        <v>0.1</v>
-      </c>
-      <c r="I19" s="4">
-        <f t="shared" si="3"/>
-        <v>0.04</v>
-      </c>
-      <c r="J19" s="9">
-        <f>utilities!$E$11</f>
-        <v>1E-3</v>
-      </c>
-      <c r="K19">
-        <f t="shared" si="4"/>
-        <v>-7.3295618272661933</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A20">
-        <v>18</v>
-      </c>
-      <c r="B20">
-        <v>6</v>
-      </c>
-      <c r="C20">
-        <v>8</v>
-      </c>
-      <c r="D20">
-        <v>9</v>
-      </c>
-      <c r="E20" s="16">
-        <f t="shared" si="5"/>
-        <v>16.737800872947847</v>
-      </c>
-      <c r="F20">
-        <f t="shared" si="0"/>
-        <v>0.04</v>
-      </c>
-      <c r="G20" s="4">
-        <f t="shared" si="1"/>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="H20" s="4">
-        <f t="shared" si="2"/>
-        <v>0.1</v>
-      </c>
-      <c r="I20" s="4">
-        <f t="shared" si="3"/>
-        <v>0.04</v>
-      </c>
-      <c r="J20" s="9">
-        <f>utilities!$E$11</f>
-        <v>1E-3</v>
-      </c>
-      <c r="K20">
-        <f t="shared" si="4"/>
-        <v>-7.7378008729478474</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21">
-        <v>19</v>
-      </c>
-      <c r="B21">
-        <v>6</v>
-      </c>
-      <c r="C21">
-        <v>8</v>
-      </c>
-      <c r="D21">
-        <v>9</v>
-      </c>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E21" s="16">
-        <f t="shared" si="5"/>
-        <v>17.156245894771544</v>
-      </c>
-      <c r="F21">
-        <f t="shared" si="0"/>
-        <v>0.04</v>
+        <f>E20*0.8</f>
+        <v>6.4</v>
       </c>
       <c r="G21" s="4">
-        <f t="shared" si="1"/>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="H21" s="4">
-        <f t="shared" si="2"/>
-        <v>0.1</v>
-      </c>
-      <c r="I21" s="4">
-        <f t="shared" si="3"/>
-        <v>0.04</v>
-      </c>
-      <c r="J21" s="9">
-        <f>utilities!$E$11</f>
-        <v>1E-3</v>
-      </c>
-      <c r="K21">
-        <f t="shared" si="4"/>
-        <v>-8.1562458947715442</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A22">
-        <v>20</v>
-      </c>
-      <c r="B22">
-        <v>6</v>
-      </c>
-      <c r="C22">
-        <v>8</v>
-      </c>
-      <c r="D22">
-        <v>9</v>
-      </c>
+        <f>G17*B17</f>
+        <v>25</v>
+      </c>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E22" s="16">
-        <f t="shared" si="5"/>
-        <v>17.585152042140834</v>
-      </c>
-      <c r="F22">
-        <f t="shared" si="0"/>
-        <v>0.04</v>
+        <f>E20*0.6</f>
+        <v>4.8</v>
       </c>
       <c r="G22" s="4">
-        <f t="shared" si="1"/>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="H22" s="4">
-        <f t="shared" si="2"/>
-        <v>0.1</v>
-      </c>
-      <c r="I22" s="4">
-        <f t="shared" si="3"/>
-        <v>0.04</v>
-      </c>
-      <c r="J22" s="9">
-        <f>utilities!$E$11</f>
-        <v>1E-3</v>
-      </c>
-      <c r="K22">
-        <f t="shared" si="4"/>
-        <v>-8.5851520421408338</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A23">
-        <v>21</v>
-      </c>
-      <c r="B23">
-        <v>6</v>
-      </c>
-      <c r="C23">
-        <v>8</v>
-      </c>
-      <c r="D23">
-        <v>9</v>
-      </c>
-      <c r="E23" s="16">
-        <f t="shared" si="5"/>
-        <v>18.02478084319435</v>
-      </c>
-      <c r="F23">
-        <f t="shared" si="0"/>
-        <v>0.04</v>
-      </c>
+        <f>G16*B16</f>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="E23" s="16"/>
       <c r="G23" s="4">
-        <f t="shared" si="1"/>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="H23" s="4">
-        <f t="shared" si="2"/>
-        <v>0.1</v>
-      </c>
-      <c r="I23" s="4">
-        <f t="shared" si="3"/>
-        <v>0.04</v>
-      </c>
-      <c r="J23" s="9">
-        <f>utilities!$E$11</f>
-        <v>1E-3</v>
-      </c>
-      <c r="K23">
-        <f t="shared" si="4"/>
-        <v>-9.0247808431943497</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A24">
-        <v>22</v>
-      </c>
-      <c r="B24">
-        <v>6</v>
-      </c>
-      <c r="C24">
-        <v>8</v>
-      </c>
-      <c r="D24">
-        <v>9</v>
-      </c>
-      <c r="E24" s="16">
-        <f t="shared" si="5"/>
-        <v>18.475400364274208</v>
-      </c>
-      <c r="F24">
-        <f t="shared" si="0"/>
-        <v>0.04</v>
-      </c>
-      <c r="G24" s="4">
-        <f t="shared" si="1"/>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="H24" s="4">
-        <f t="shared" si="2"/>
-        <v>0.1</v>
-      </c>
-      <c r="I24" s="4">
-        <f t="shared" si="3"/>
-        <v>0.04</v>
-      </c>
-      <c r="J24" s="9">
-        <f>utilities!$E$11</f>
-        <v>1E-3</v>
-      </c>
-      <c r="K24">
-        <f t="shared" si="4"/>
-        <v>-9.4754003642742077</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A25">
-        <v>23</v>
-      </c>
-      <c r="B25">
-        <v>6</v>
-      </c>
-      <c r="C25">
-        <v>8</v>
-      </c>
-      <c r="D25">
-        <v>9</v>
-      </c>
-      <c r="E25" s="16">
-        <f t="shared" si="5"/>
-        <v>18.937285373381062</v>
-      </c>
-      <c r="F25">
-        <f t="shared" si="0"/>
-        <v>0.04</v>
-      </c>
-      <c r="G25" s="4">
-        <f t="shared" si="1"/>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="H25" s="4">
-        <f t="shared" si="2"/>
-        <v>0.1</v>
-      </c>
-      <c r="I25" s="4">
-        <f t="shared" si="3"/>
-        <v>0.04</v>
-      </c>
-      <c r="J25" s="9">
-        <f>utilities!$E$11</f>
-        <v>1E-3</v>
-      </c>
-      <c r="K25">
-        <f t="shared" si="4"/>
-        <v>-9.9372853733810622</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A26">
-        <v>24</v>
-      </c>
-      <c r="B26">
-        <v>6</v>
-      </c>
-      <c r="C26">
-        <v>8</v>
-      </c>
-      <c r="D26">
-        <v>9</v>
-      </c>
-      <c r="E26" s="16">
-        <f t="shared" si="5"/>
-        <v>19.410717507715589</v>
-      </c>
-      <c r="F26">
-        <f t="shared" si="0"/>
-        <v>0.04</v>
-      </c>
-      <c r="G26" s="4">
-        <f t="shared" si="1"/>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="H26" s="4">
-        <f t="shared" si="2"/>
-        <v>0.1</v>
-      </c>
-      <c r="I26" s="4">
-        <f t="shared" si="3"/>
-        <v>0.04</v>
-      </c>
-      <c r="J26" s="9">
-        <f>utilities!$E$11</f>
-        <v>1E-3</v>
-      </c>
-      <c r="K26">
-        <f t="shared" si="4"/>
-        <v>-10.410717507715589</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A27">
+        <f>G22*15</f>
         <v>25</v>
       </c>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="E24" s="16"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="E25" s="16"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="E26" s="16"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>28</v>
+      </c>
       <c r="B27">
-        <v>96</v>
+        <f>SUM(B2:B26)</f>
+        <v>171</v>
       </c>
       <c r="C27">
-        <v>143</v>
+        <f>SUM(C2:C26)</f>
+        <v>248</v>
       </c>
       <c r="D27">
-        <v>259</v>
-      </c>
-      <c r="E27" s="16">
-        <f t="shared" si="5"/>
-        <v>19.895985445408478</v>
-      </c>
-      <c r="F27">
-        <v>1</v>
-      </c>
-      <c r="G27" s="4">
-        <f t="shared" si="1"/>
-        <v>0.26041666666666669</v>
-      </c>
-      <c r="H27" s="4">
-        <f t="shared" si="2"/>
-        <v>0.10638297872340426</v>
-      </c>
-      <c r="I27" s="4">
-        <f t="shared" si="3"/>
-        <v>8.6206896551724137E-3</v>
-      </c>
-      <c r="J27" s="9">
-        <f>utilities!$E$11</f>
-        <v>1E-3</v>
-      </c>
-      <c r="K27">
-        <f t="shared" si="4"/>
-        <v>239.10401455459152</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>28</v>
+        <f>SUM(D2:D26)</f>
+        <v>294</v>
+      </c>
+      <c r="E27">
+        <f>SUM(E2:E26)</f>
+        <v>184.20000000000002</v>
+      </c>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+      <c r="K27" s="15">
+        <f>IRR(K2:K17)</f>
+        <v>0.13875755605827766</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>26</v>
       </c>
       <c r="B28">
-        <f>SUM(B2:B27)</f>
-        <v>306</v>
+        <f>utilities!$H$8</f>
+        <v>0</v>
       </c>
       <c r="C28">
-        <f t="shared" ref="C28:D28" si="6">SUM(C2:C27)</f>
-        <v>433</v>
+        <f>utilities!$I$8</f>
+        <v>0</v>
       </c>
       <c r="D28">
-        <f t="shared" si="6"/>
-        <v>634</v>
+        <f>utilities!$J$8</f>
+        <v>0</v>
       </c>
       <c r="E28">
-        <f>SUM(E2:E27)</f>
-        <v>379.52918032845758</v>
-      </c>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="4"/>
-      <c r="K28" s="15" t="e">
-        <f>IRR(K2:K27)</f>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <f t="shared" ref="F28:F42" si="5">1/25</f>
+        <v>0.04</v>
+      </c>
+      <c r="G28" s="4" t="e">
+        <f>utilities!$H$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H28" s="4" t="e">
+        <f>utilities!$I$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I28" s="4" t="e">
+        <f>utilities!$J$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J28" s="9">
+        <f>utilities!$K$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B29">
         <f>utilities!$H$8</f>
@@ -1768,7 +1484,7 @@
         <v>0</v>
       </c>
       <c r="F29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>0.04</v>
       </c>
       <c r="G29" s="4" t="e">
@@ -1788,9 +1504,9 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B30">
         <f>utilities!$H$8</f>
@@ -1808,7 +1524,7 @@
         <v>0</v>
       </c>
       <c r="F30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>0.04</v>
       </c>
       <c r="G30" s="4" t="e">
@@ -1828,9 +1544,9 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B31">
         <f>utilities!$H$8</f>
@@ -1848,7 +1564,7 @@
         <v>0</v>
       </c>
       <c r="F31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>0.04</v>
       </c>
       <c r="G31" s="4" t="e">
@@ -1868,9 +1584,9 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B32">
         <f>utilities!$H$8</f>
@@ -1888,7 +1604,7 @@
         <v>0</v>
       </c>
       <c r="F32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>0.04</v>
       </c>
       <c r="G32" s="4" t="e">
@@ -1910,7 +1626,7 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B33">
         <f>utilities!$H$8</f>
@@ -1928,7 +1644,7 @@
         <v>0</v>
       </c>
       <c r="F33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>0.04</v>
       </c>
       <c r="G33" s="4" t="e">
@@ -1950,7 +1666,7 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B34">
         <f>utilities!$H$8</f>
@@ -1968,7 +1684,7 @@
         <v>0</v>
       </c>
       <c r="F34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>0.04</v>
       </c>
       <c r="G34" s="4" t="e">
@@ -1990,7 +1706,7 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B35">
         <f>utilities!$H$8</f>
@@ -2008,7 +1724,7 @@
         <v>0</v>
       </c>
       <c r="F35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>0.04</v>
       </c>
       <c r="G35" s="4" t="e">
@@ -2030,7 +1746,7 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B36">
         <f>utilities!$H$8</f>
@@ -2048,7 +1764,7 @@
         <v>0</v>
       </c>
       <c r="F36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>0.04</v>
       </c>
       <c r="G36" s="4" t="e">
@@ -2070,7 +1786,7 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B37">
         <f>utilities!$H$8</f>
@@ -2088,7 +1804,7 @@
         <v>0</v>
       </c>
       <c r="F37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>0.04</v>
       </c>
       <c r="G37" s="4" t="e">
@@ -2110,7 +1826,7 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B38">
         <f>utilities!$H$8</f>
@@ -2128,7 +1844,7 @@
         <v>0</v>
       </c>
       <c r="F38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>0.04</v>
       </c>
       <c r="G38" s="4" t="e">
@@ -2150,7 +1866,7 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B39">
         <f>utilities!$H$8</f>
@@ -2168,7 +1884,7 @@
         <v>0</v>
       </c>
       <c r="F39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>0.04</v>
       </c>
       <c r="G39" s="4" t="e">
@@ -2190,7 +1906,7 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B40">
         <f>utilities!$H$8</f>
@@ -2208,7 +1924,7 @@
         <v>0</v>
       </c>
       <c r="F40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>0.04</v>
       </c>
       <c r="G40" s="4" t="e">
@@ -2230,7 +1946,7 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B41">
         <f>utilities!$H$8</f>
@@ -2248,7 +1964,7 @@
         <v>0</v>
       </c>
       <c r="F41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>0.04</v>
       </c>
       <c r="G41" s="4" t="e">
@@ -2270,7 +1986,7 @@
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B42">
         <f>utilities!$H$8</f>
@@ -2288,7 +2004,7 @@
         <v>0</v>
       </c>
       <c r="F42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>0.04</v>
       </c>
       <c r="G42" s="4" t="e">
@@ -2304,46 +2020,6 @@
         <v>#DIV/0!</v>
       </c>
       <c r="J42" s="9">
-        <f>utilities!$K$11</f>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A43">
-        <v>40</v>
-      </c>
-      <c r="B43">
-        <f>utilities!$H$8</f>
-        <v>0</v>
-      </c>
-      <c r="C43">
-        <f>utilities!$I$8</f>
-        <v>0</v>
-      </c>
-      <c r="D43">
-        <f>utilities!$J$8</f>
-        <v>0</v>
-      </c>
-      <c r="E43">
-        <v>0</v>
-      </c>
-      <c r="F43">
-        <f t="shared" si="0"/>
-        <v>0.04</v>
-      </c>
-      <c r="G43" s="4" t="e">
-        <f>utilities!$H$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H43" s="4" t="e">
-        <f>utilities!$I$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I43" s="4" t="e">
-        <f>utilities!$J$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J43" s="9">
         <f>utilities!$K$11</f>
         <v>1E-3</v>
       </c>
@@ -2357,8 +2033,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67C203FD-C9AE-45F0-8773-EECC728085CE}">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I27"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2457,23 +2133,23 @@
         <v>9</v>
       </c>
       <c r="E3" s="16">
-        <f>11*(1+2.5%)^(A3-1)</f>
+        <f t="shared" ref="E3:E27" si="0">11*(1+2.5%)^(A3-1)</f>
         <v>11.274999999999999</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F43" si="0">1/25</f>
+        <f t="shared" ref="F3:F43" si="1">1/25</f>
         <v>0.04</v>
       </c>
       <c r="G3" s="4">
-        <f t="shared" ref="G3:G27" si="1">25*F3</f>
+        <f t="shared" ref="G3:G27" si="2">25*F3</f>
         <v>1</v>
       </c>
       <c r="H3" s="4">
-        <f t="shared" ref="H3:H27" si="2">5*F3</f>
+        <f t="shared" ref="H3:H27" si="3">5*F3</f>
         <v>0.2</v>
       </c>
       <c r="I3" s="4">
-        <f t="shared" ref="I3:I27" si="3">1*F3</f>
+        <f t="shared" ref="I3:I27" si="4">1*F3</f>
         <v>0.04</v>
       </c>
       <c r="J3" s="9">
@@ -2481,7 +2157,7 @@
         <v>1E-3</v>
       </c>
       <c r="K3">
-        <f t="shared" ref="K3:K27" si="4">D3-E3</f>
+        <f t="shared" ref="K3:K27" si="5">D3-E3</f>
         <v>-2.2749999999999986</v>
       </c>
     </row>
@@ -2499,23 +2175,23 @@
         <v>9</v>
       </c>
       <c r="E4" s="16">
-        <f>11*(1+2.5%)^(A4-1)</f>
+        <f t="shared" si="0"/>
         <v>11.556875</v>
       </c>
       <c r="F4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.04</v>
       </c>
       <c r="G4" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H4" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
       <c r="I4" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.04</v>
       </c>
       <c r="J4" s="9">
@@ -2523,7 +2199,7 @@
         <v>1E-3</v>
       </c>
       <c r="K4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-2.5568749999999998</v>
       </c>
     </row>
@@ -2541,23 +2217,23 @@
         <v>9</v>
       </c>
       <c r="E5" s="16">
-        <f>11*(1+2.5%)^(A5-1)</f>
+        <f t="shared" si="0"/>
         <v>11.845796874999998</v>
       </c>
       <c r="F5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.04</v>
       </c>
       <c r="G5" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H5" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
       <c r="I5" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.04</v>
       </c>
       <c r="J5" s="9">
@@ -2565,7 +2241,7 @@
         <v>1E-3</v>
       </c>
       <c r="K5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-2.8457968749999978</v>
       </c>
     </row>
@@ -2583,23 +2259,23 @@
         <v>9</v>
       </c>
       <c r="E6" s="16">
-        <f>11*(1+2.5%)^(A6-1)</f>
+        <f t="shared" si="0"/>
         <v>12.141941796874997</v>
       </c>
       <c r="F6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.04</v>
       </c>
       <c r="G6" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H6" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
       <c r="I6" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.04</v>
       </c>
       <c r="J6" s="9">
@@ -2607,7 +2283,7 @@
         <v>1E-3</v>
       </c>
       <c r="K6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-3.1419417968749972</v>
       </c>
     </row>
@@ -2625,23 +2301,23 @@
         <v>9</v>
       </c>
       <c r="E7" s="16">
-        <f>11*(1+2.5%)^(A7-1)</f>
+        <f t="shared" si="0"/>
         <v>12.445490341796871</v>
       </c>
       <c r="F7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.04</v>
       </c>
       <c r="G7" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H7" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
       <c r="I7" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.04</v>
       </c>
       <c r="J7" s="9">
@@ -2649,7 +2325,7 @@
         <v>1E-3</v>
       </c>
       <c r="K7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-3.4454903417968712</v>
       </c>
     </row>
@@ -2667,23 +2343,23 @@
         <v>9</v>
       </c>
       <c r="E8" s="16">
-        <f>11*(1+2.5%)^(A8-1)</f>
+        <f t="shared" si="0"/>
         <v>12.756627600341792</v>
       </c>
       <c r="F8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.04</v>
       </c>
       <c r="G8" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H8" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
       <c r="I8" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.04</v>
       </c>
       <c r="J8" s="9">
@@ -2691,7 +2367,7 @@
         <v>1E-3</v>
       </c>
       <c r="K8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-3.7566276003417922</v>
       </c>
     </row>
@@ -2709,23 +2385,23 @@
         <v>9</v>
       </c>
       <c r="E9" s="16">
-        <f>11*(1+2.5%)^(A9-1)</f>
+        <f t="shared" si="0"/>
         <v>13.075543290350337</v>
       </c>
       <c r="F9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.04</v>
       </c>
       <c r="G9" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H9" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
       <c r="I9" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.04</v>
       </c>
       <c r="J9" s="9">
@@ -2733,7 +2409,7 @@
         <v>1E-3</v>
       </c>
       <c r="K9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-4.0755432903503372</v>
       </c>
     </row>
@@ -2751,23 +2427,23 @@
         <v>9</v>
       </c>
       <c r="E10" s="16">
-        <f>11*(1+2.5%)^(A10-1)</f>
+        <f t="shared" si="0"/>
         <v>13.402431872609094</v>
       </c>
       <c r="F10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.04</v>
       </c>
       <c r="G10" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H10" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
       <c r="I10" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.04</v>
       </c>
       <c r="J10" s="9">
@@ -2775,7 +2451,7 @@
         <v>1E-3</v>
       </c>
       <c r="K10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-4.4024318726090943</v>
       </c>
     </row>
@@ -2793,22 +2469,22 @@
         <v>159</v>
       </c>
       <c r="E11" s="16">
-        <f>11*(1+2.5%)^(A11-1)</f>
+        <f t="shared" si="0"/>
         <v>13.73749266942432</v>
       </c>
       <c r="F11">
         <v>1</v>
       </c>
       <c r="G11" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>25</v>
       </c>
       <c r="H11" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="I11" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J11" s="9">
@@ -2816,7 +2492,7 @@
         <v>1E-3</v>
       </c>
       <c r="K11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>145.26250733057569</v>
       </c>
     </row>
@@ -2834,23 +2510,23 @@
         <v>9</v>
       </c>
       <c r="E12" s="16">
-        <f>11*(1+2.5%)^(A12-1)</f>
+        <f t="shared" si="0"/>
         <v>14.080929986159928</v>
       </c>
       <c r="F12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.04</v>
       </c>
       <c r="G12" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H12" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
       <c r="I12" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.04</v>
       </c>
       <c r="J12" s="9">
@@ -2858,7 +2534,7 @@
         <v>1E-3</v>
       </c>
       <c r="K12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-5.0809299861599282</v>
       </c>
     </row>
@@ -2876,23 +2552,23 @@
         <v>9</v>
       </c>
       <c r="E13" s="16">
-        <f>11*(1+2.5%)^(A13-1)</f>
+        <f t="shared" si="0"/>
         <v>14.432953235813926</v>
       </c>
       <c r="F13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.04</v>
       </c>
       <c r="G13" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H13" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
       <c r="I13" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.04</v>
       </c>
       <c r="J13" s="9">
@@ -2900,7 +2576,7 @@
         <v>1E-3</v>
       </c>
       <c r="K13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-5.4329532358139261</v>
       </c>
     </row>
@@ -2918,23 +2594,23 @@
         <v>9</v>
       </c>
       <c r="E14" s="16">
-        <f>11*(1+2.5%)^(A14-1)</f>
+        <f t="shared" si="0"/>
         <v>14.793777066709273</v>
       </c>
       <c r="F14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.04</v>
       </c>
       <c r="G14" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H14" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
       <c r="I14" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.04</v>
       </c>
       <c r="J14" s="9">
@@ -2942,7 +2618,7 @@
         <v>1E-3</v>
       </c>
       <c r="K14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-5.7937770667092732</v>
       </c>
     </row>
@@ -2960,23 +2636,23 @@
         <v>9</v>
       </c>
       <c r="E15" s="16">
-        <f>11*(1+2.5%)^(A15-1)</f>
+        <f t="shared" si="0"/>
         <v>14.793777066709273</v>
       </c>
       <c r="F15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.04</v>
       </c>
       <c r="G15" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H15" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
       <c r="I15" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.04</v>
       </c>
       <c r="J15" s="9">
@@ -2984,7 +2660,7 @@
         <v>1E-3</v>
       </c>
       <c r="K15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-5.7937770667092732</v>
       </c>
     </row>
@@ -3002,23 +2678,23 @@
         <v>9</v>
       </c>
       <c r="E16" s="16">
-        <f>11*(1+2.5%)^(A16-1)</f>
+        <f t="shared" si="0"/>
         <v>15.163621493377004</v>
       </c>
       <c r="F16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.04</v>
       </c>
       <c r="G16" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H16" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
       <c r="I16" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.04</v>
       </c>
       <c r="J16" s="9">
@@ -3026,7 +2702,7 @@
         <v>1E-3</v>
       </c>
       <c r="K16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-6.1636214933770042</v>
       </c>
     </row>
@@ -3044,23 +2720,23 @@
         <v>9</v>
       </c>
       <c r="E17" s="16">
-        <f>11*(1+2.5%)^(A17-1)</f>
+        <f t="shared" si="0"/>
         <v>15.542712030711428</v>
       </c>
       <c r="F17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.04</v>
       </c>
       <c r="G17" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H17" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
       <c r="I17" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.04</v>
       </c>
       <c r="J17" s="9">
@@ -3068,7 +2744,7 @@
         <v>1E-3</v>
       </c>
       <c r="K17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-6.5427120307114279</v>
       </c>
     </row>
@@ -3086,23 +2762,23 @@
         <v>9</v>
       </c>
       <c r="E18" s="16">
-        <f>11*(1+2.5%)^(A18-1)</f>
+        <f t="shared" si="0"/>
         <v>15.931279831479216</v>
       </c>
       <c r="F18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.04</v>
       </c>
       <c r="G18" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H18" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
       <c r="I18" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.04</v>
       </c>
       <c r="J18" s="9">
@@ -3110,7 +2786,7 @@
         <v>1E-3</v>
       </c>
       <c r="K18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-6.9312798314792161</v>
       </c>
     </row>
@@ -3128,23 +2804,23 @@
         <v>9</v>
       </c>
       <c r="E19" s="16">
-        <f>11*(1+2.5%)^(A19-1)</f>
+        <f t="shared" si="0"/>
         <v>16.329561827266193</v>
       </c>
       <c r="F19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.04</v>
       </c>
       <c r="G19" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H19" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
       <c r="I19" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.04</v>
       </c>
       <c r="J19" s="9">
@@ -3152,7 +2828,7 @@
         <v>1E-3</v>
       </c>
       <c r="K19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-7.3295618272661933</v>
       </c>
     </row>
@@ -3170,23 +2846,23 @@
         <v>9</v>
       </c>
       <c r="E20" s="16">
-        <f>11*(1+2.5%)^(A20-1)</f>
+        <f t="shared" si="0"/>
         <v>16.737800872947847</v>
       </c>
       <c r="F20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.04</v>
       </c>
       <c r="G20" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H20" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
       <c r="I20" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.04</v>
       </c>
       <c r="J20" s="9">
@@ -3194,7 +2870,7 @@
         <v>1E-3</v>
       </c>
       <c r="K20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-7.7378008729478474</v>
       </c>
     </row>
@@ -3212,23 +2888,23 @@
         <v>9</v>
       </c>
       <c r="E21" s="16">
-        <f>11*(1+2.5%)^(A21-1)</f>
+        <f t="shared" si="0"/>
         <v>17.156245894771544</v>
       </c>
       <c r="F21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.04</v>
       </c>
       <c r="G21" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H21" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
       <c r="I21" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.04</v>
       </c>
       <c r="J21" s="9">
@@ -3236,7 +2912,7 @@
         <v>1E-3</v>
       </c>
       <c r="K21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-8.1562458947715442</v>
       </c>
     </row>
@@ -3254,23 +2930,23 @@
         <v>9</v>
       </c>
       <c r="E22" s="16">
-        <f>11*(1+2.5%)^(A22-1)</f>
+        <f t="shared" si="0"/>
         <v>17.585152042140834</v>
       </c>
       <c r="F22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.04</v>
       </c>
       <c r="G22" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H22" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
       <c r="I22" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.04</v>
       </c>
       <c r="J22" s="9">
@@ -3278,7 +2954,7 @@
         <v>1E-3</v>
       </c>
       <c r="K22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-8.5851520421408338</v>
       </c>
     </row>
@@ -3296,23 +2972,23 @@
         <v>9</v>
       </c>
       <c r="E23" s="16">
-        <f>11*(1+2.5%)^(A23-1)</f>
+        <f t="shared" si="0"/>
         <v>18.02478084319435</v>
       </c>
       <c r="F23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.04</v>
       </c>
       <c r="G23" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H23" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
       <c r="I23" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.04</v>
       </c>
       <c r="J23" s="9">
@@ -3320,7 +2996,7 @@
         <v>1E-3</v>
       </c>
       <c r="K23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-9.0247808431943497</v>
       </c>
     </row>
@@ -3338,23 +3014,23 @@
         <v>9</v>
       </c>
       <c r="E24" s="16">
-        <f>11*(1+2.5%)^(A24-1)</f>
+        <f t="shared" si="0"/>
         <v>18.475400364274208</v>
       </c>
       <c r="F24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.04</v>
       </c>
       <c r="G24" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H24" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
       <c r="I24" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.04</v>
       </c>
       <c r="J24" s="9">
@@ -3362,7 +3038,7 @@
         <v>1E-3</v>
       </c>
       <c r="K24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-9.4754003642742077</v>
       </c>
     </row>
@@ -3380,23 +3056,23 @@
         <v>9</v>
       </c>
       <c r="E25" s="16">
-        <f>11*(1+2.5%)^(A25-1)</f>
+        <f t="shared" si="0"/>
         <v>18.937285373381062</v>
       </c>
       <c r="F25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.04</v>
       </c>
       <c r="G25" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H25" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
       <c r="I25" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.04</v>
       </c>
       <c r="J25" s="9">
@@ -3404,7 +3080,7 @@
         <v>1E-3</v>
       </c>
       <c r="K25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-9.9372853733810622</v>
       </c>
     </row>
@@ -3422,23 +3098,23 @@
         <v>9</v>
       </c>
       <c r="E26" s="16">
-        <f>11*(1+2.5%)^(A26-1)</f>
+        <f t="shared" si="0"/>
         <v>19.410717507715589</v>
       </c>
       <c r="F26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.04</v>
       </c>
       <c r="G26" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H26" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
       <c r="I26" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.04</v>
       </c>
       <c r="J26" s="9">
@@ -3446,7 +3122,7 @@
         <v>1E-3</v>
       </c>
       <c r="K26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-10.410717507715589</v>
       </c>
     </row>
@@ -3464,22 +3140,22 @@
         <v>259</v>
       </c>
       <c r="E27" s="16">
-        <f>11*(1+2.5%)^(A27-1)</f>
+        <f t="shared" si="0"/>
         <v>19.895985445408478</v>
       </c>
       <c r="F27">
         <v>1</v>
       </c>
       <c r="G27" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>25</v>
       </c>
       <c r="H27" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="I27" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J27" s="9">
@@ -3487,7 +3163,7 @@
         <v>1E-3</v>
       </c>
       <c r="K27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>239.10401455459152</v>
       </c>
     </row>
@@ -3500,11 +3176,11 @@
         <v>306</v>
       </c>
       <c r="C28">
-        <f t="shared" ref="C28:D28" si="5">SUM(C2:C27)</f>
+        <f t="shared" ref="C28:D28" si="6">SUM(C2:C27)</f>
         <v>433</v>
       </c>
       <c r="D28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>634</v>
       </c>
       <c r="E28">
@@ -3539,7 +3215,7 @@
         <v>0</v>
       </c>
       <c r="F29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.04</v>
       </c>
       <c r="G29" s="4" t="e">
@@ -3579,7 +3255,7 @@
         <v>0</v>
       </c>
       <c r="F30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.04</v>
       </c>
       <c r="G30" s="4" t="e">
@@ -3619,7 +3295,7 @@
         <v>0</v>
       </c>
       <c r="F31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.04</v>
       </c>
       <c r="G31" s="4" t="e">
@@ -3659,7 +3335,7 @@
         <v>0</v>
       </c>
       <c r="F32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.04</v>
       </c>
       <c r="G32" s="4" t="e">
@@ -3699,7 +3375,7 @@
         <v>0</v>
       </c>
       <c r="F33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.04</v>
       </c>
       <c r="G33" s="4" t="e">
@@ -3739,7 +3415,7 @@
         <v>0</v>
       </c>
       <c r="F34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.04</v>
       </c>
       <c r="G34" s="4" t="e">
@@ -3779,7 +3455,7 @@
         <v>0</v>
       </c>
       <c r="F35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.04</v>
       </c>
       <c r="G35" s="4" t="e">
@@ -3819,7 +3495,7 @@
         <v>0</v>
       </c>
       <c r="F36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.04</v>
       </c>
       <c r="G36" s="4" t="e">
@@ -3859,7 +3535,7 @@
         <v>0</v>
       </c>
       <c r="F37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.04</v>
       </c>
       <c r="G37" s="4" t="e">
@@ -3899,7 +3575,7 @@
         <v>0</v>
       </c>
       <c r="F38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.04</v>
       </c>
       <c r="G38" s="4" t="e">
@@ -3939,7 +3615,7 @@
         <v>0</v>
       </c>
       <c r="F39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.04</v>
       </c>
       <c r="G39" s="4" t="e">
@@ -3979,7 +3655,7 @@
         <v>0</v>
       </c>
       <c r="F40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.04</v>
       </c>
       <c r="G40" s="4" t="e">
@@ -4019,7 +3695,7 @@
         <v>0</v>
       </c>
       <c r="F41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.04</v>
       </c>
       <c r="G41" s="4" t="e">
@@ -4059,7 +3735,7 @@
         <v>0</v>
       </c>
       <c r="F42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.04</v>
       </c>
       <c r="G42" s="4" t="e">
@@ -4099,7 +3775,7 @@
         <v>0</v>
       </c>
       <c r="F43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.04</v>
       </c>
       <c r="G43" s="4" t="e">
@@ -4125,6 +3801,1777 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C37F228-CE9B-4855-94EE-55EF65F52467}">
+  <dimension ref="A1:K43"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="7" max="7" width="16.6640625" customWidth="1"/>
+    <col min="10" max="10" width="8.88671875" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>6</v>
+      </c>
+      <c r="C2">
+        <v>8</v>
+      </c>
+      <c r="D2">
+        <v>9</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <f>1/25</f>
+        <v>0.04</v>
+      </c>
+      <c r="G2" s="4">
+        <f>(25*F2)/B2</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="H2" s="4">
+        <f>(5*F2)/(C2-B2)</f>
+        <v>0.1</v>
+      </c>
+      <c r="I2" s="4">
+        <f>(1*F2)/(D2-C2)</f>
+        <v>0.04</v>
+      </c>
+      <c r="J2" s="9">
+        <f>utilities!$E$11</f>
+        <v>1E-3</v>
+      </c>
+      <c r="K2">
+        <f>D2-E2</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>6</v>
+      </c>
+      <c r="C3">
+        <v>8</v>
+      </c>
+      <c r="D3">
+        <v>9</v>
+      </c>
+      <c r="E3" s="16">
+        <f>11*(1+2.5%)^(A3-1)</f>
+        <v>11.274999999999999</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F43" si="0">1/25</f>
+        <v>0.04</v>
+      </c>
+      <c r="G3" s="4">
+        <f t="shared" ref="G3:G27" si="1">(25*F3)/B3</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="H3" s="4">
+        <f t="shared" ref="H3:H27" si="2">(5*F3)/(C3-B3)</f>
+        <v>0.1</v>
+      </c>
+      <c r="I3" s="4">
+        <f t="shared" ref="I3:I27" si="3">(1*F3)/(D3-C3)</f>
+        <v>0.04</v>
+      </c>
+      <c r="J3" s="9">
+        <f>utilities!$E$11</f>
+        <v>1E-3</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K27" si="4">D3-E3</f>
+        <v>-2.2749999999999986</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <v>8</v>
+      </c>
+      <c r="D4">
+        <v>9</v>
+      </c>
+      <c r="E4" s="16">
+        <f>11*(1+2.5%)^(A4-1)</f>
+        <v>11.556875</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="G4" s="4">
+        <f t="shared" si="1"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="H4" s="4">
+        <f t="shared" si="2"/>
+        <v>0.1</v>
+      </c>
+      <c r="I4" s="4">
+        <f t="shared" si="3"/>
+        <v>0.04</v>
+      </c>
+      <c r="J4" s="9">
+        <f>utilities!$E$11</f>
+        <v>1E-3</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="4"/>
+        <v>-2.5568749999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>8</v>
+      </c>
+      <c r="D5">
+        <v>9</v>
+      </c>
+      <c r="E5" s="16">
+        <f t="shared" ref="E5:E27" si="5">11*(1+2.5%)^(A5-1)</f>
+        <v>11.845796874999998</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="G5" s="4">
+        <f t="shared" si="1"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="H5" s="4">
+        <f t="shared" si="2"/>
+        <v>0.1</v>
+      </c>
+      <c r="I5" s="4">
+        <f t="shared" si="3"/>
+        <v>0.04</v>
+      </c>
+      <c r="J5" s="9">
+        <f>utilities!$E$11</f>
+        <v>1E-3</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="4"/>
+        <v>-2.8457968749999978</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>6</v>
+      </c>
+      <c r="C6">
+        <v>8</v>
+      </c>
+      <c r="D6">
+        <v>9</v>
+      </c>
+      <c r="E6" s="16">
+        <f t="shared" si="5"/>
+        <v>12.141941796874997</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="G6" s="4">
+        <f t="shared" si="1"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="H6" s="4">
+        <f t="shared" si="2"/>
+        <v>0.1</v>
+      </c>
+      <c r="I6" s="4">
+        <f t="shared" si="3"/>
+        <v>0.04</v>
+      </c>
+      <c r="J6" s="9">
+        <f>utilities!$E$11</f>
+        <v>1E-3</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="4"/>
+        <v>-3.1419417968749972</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>8</v>
+      </c>
+      <c r="D7">
+        <v>9</v>
+      </c>
+      <c r="E7" s="16">
+        <f t="shared" si="5"/>
+        <v>12.445490341796871</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="G7" s="4">
+        <f t="shared" si="1"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="H7" s="4">
+        <f t="shared" si="2"/>
+        <v>0.1</v>
+      </c>
+      <c r="I7" s="4">
+        <f t="shared" si="3"/>
+        <v>0.04</v>
+      </c>
+      <c r="J7" s="9">
+        <f>utilities!$E$11</f>
+        <v>1E-3</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="4"/>
+        <v>-3.4454903417968712</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <v>8</v>
+      </c>
+      <c r="D8">
+        <v>9</v>
+      </c>
+      <c r="E8" s="16">
+        <f t="shared" si="5"/>
+        <v>12.756627600341792</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="G8" s="4">
+        <f t="shared" si="1"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="H8" s="4">
+        <f t="shared" si="2"/>
+        <v>0.1</v>
+      </c>
+      <c r="I8" s="4">
+        <f t="shared" si="3"/>
+        <v>0.04</v>
+      </c>
+      <c r="J8" s="9">
+        <f>utilities!$E$11</f>
+        <v>1E-3</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="4"/>
+        <v>-3.7566276003417922</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>6</v>
+      </c>
+      <c r="C9">
+        <v>8</v>
+      </c>
+      <c r="D9">
+        <v>9</v>
+      </c>
+      <c r="E9" s="16">
+        <f t="shared" si="5"/>
+        <v>13.075543290350337</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="G9" s="4">
+        <f t="shared" si="1"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="H9" s="4">
+        <f t="shared" si="2"/>
+        <v>0.1</v>
+      </c>
+      <c r="I9" s="4">
+        <f t="shared" si="3"/>
+        <v>0.04</v>
+      </c>
+      <c r="J9" s="9">
+        <f>utilities!$E$11</f>
+        <v>1E-3</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="4"/>
+        <v>-4.0755432903503372</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>6</v>
+      </c>
+      <c r="C10">
+        <v>8</v>
+      </c>
+      <c r="D10">
+        <v>9</v>
+      </c>
+      <c r="E10" s="16">
+        <f t="shared" si="5"/>
+        <v>13.402431872609094</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="G10" s="4">
+        <f t="shared" si="1"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="H10" s="4">
+        <f t="shared" si="2"/>
+        <v>0.1</v>
+      </c>
+      <c r="I10" s="4">
+        <f t="shared" si="3"/>
+        <v>0.04</v>
+      </c>
+      <c r="J10" s="9">
+        <f>utilities!$E$11</f>
+        <v>1E-3</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="4"/>
+        <v>-4.4024318726090943</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>66</v>
+      </c>
+      <c r="C11">
+        <v>98</v>
+      </c>
+      <c r="D11">
+        <v>159</v>
+      </c>
+      <c r="E11" s="16">
+        <f t="shared" si="5"/>
+        <v>13.73749266942432</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11" s="4">
+        <f t="shared" si="1"/>
+        <v>0.37878787878787878</v>
+      </c>
+      <c r="H11" s="4">
+        <f t="shared" si="2"/>
+        <v>0.15625</v>
+      </c>
+      <c r="I11" s="4">
+        <f t="shared" si="3"/>
+        <v>1.6393442622950821E-2</v>
+      </c>
+      <c r="J11" s="9">
+        <f>utilities!$E$11</f>
+        <v>1E-3</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="4"/>
+        <v>145.26250733057569</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>6</v>
+      </c>
+      <c r="C12">
+        <v>8</v>
+      </c>
+      <c r="D12">
+        <v>9</v>
+      </c>
+      <c r="E12" s="16">
+        <f t="shared" si="5"/>
+        <v>14.080929986159928</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="G12" s="4">
+        <f t="shared" si="1"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="H12" s="4">
+        <f t="shared" si="2"/>
+        <v>0.1</v>
+      </c>
+      <c r="I12" s="4">
+        <f t="shared" si="3"/>
+        <v>0.04</v>
+      </c>
+      <c r="J12" s="9">
+        <f>utilities!$E$11</f>
+        <v>1E-3</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="4"/>
+        <v>-5.0809299861599282</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>6</v>
+      </c>
+      <c r="C13">
+        <v>8</v>
+      </c>
+      <c r="D13">
+        <v>9</v>
+      </c>
+      <c r="E13" s="16">
+        <f t="shared" si="5"/>
+        <v>14.432953235813926</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="G13" s="4">
+        <f t="shared" si="1"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="H13" s="4">
+        <f t="shared" si="2"/>
+        <v>0.1</v>
+      </c>
+      <c r="I13" s="4">
+        <f t="shared" si="3"/>
+        <v>0.04</v>
+      </c>
+      <c r="J13" s="9">
+        <f>utilities!$E$11</f>
+        <v>1E-3</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="4"/>
+        <v>-5.4329532358139261</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>6</v>
+      </c>
+      <c r="C14">
+        <v>8</v>
+      </c>
+      <c r="D14">
+        <v>9</v>
+      </c>
+      <c r="E14" s="16">
+        <f t="shared" si="5"/>
+        <v>14.793777066709273</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="G14" s="4">
+        <f t="shared" si="1"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="H14" s="4">
+        <f t="shared" si="2"/>
+        <v>0.1</v>
+      </c>
+      <c r="I14" s="4">
+        <f t="shared" si="3"/>
+        <v>0.04</v>
+      </c>
+      <c r="J14" s="9">
+        <f>utilities!$E$11</f>
+        <v>1E-3</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="4"/>
+        <v>-5.7937770667092732</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>6</v>
+      </c>
+      <c r="C15">
+        <v>8</v>
+      </c>
+      <c r="D15">
+        <v>9</v>
+      </c>
+      <c r="E15" s="16">
+        <f t="shared" si="5"/>
+        <v>14.793777066709273</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="G15" s="4">
+        <f t="shared" si="1"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="H15" s="4">
+        <f t="shared" si="2"/>
+        <v>0.1</v>
+      </c>
+      <c r="I15" s="4">
+        <f t="shared" si="3"/>
+        <v>0.04</v>
+      </c>
+      <c r="J15" s="9">
+        <f>utilities!$E$11</f>
+        <v>1E-3</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="4"/>
+        <v>-5.7937770667092732</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>6</v>
+      </c>
+      <c r="C16">
+        <v>8</v>
+      </c>
+      <c r="D16">
+        <v>9</v>
+      </c>
+      <c r="E16" s="16">
+        <f t="shared" si="5"/>
+        <v>15.163621493377004</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="G16" s="4">
+        <f t="shared" si="1"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="H16" s="4">
+        <f t="shared" si="2"/>
+        <v>0.1</v>
+      </c>
+      <c r="I16" s="4">
+        <f t="shared" si="3"/>
+        <v>0.04</v>
+      </c>
+      <c r="J16" s="9">
+        <f>utilities!$E$11</f>
+        <v>1E-3</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="4"/>
+        <v>-6.1636214933770042</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>6</v>
+      </c>
+      <c r="C17">
+        <v>8</v>
+      </c>
+      <c r="D17">
+        <v>9</v>
+      </c>
+      <c r="E17" s="16">
+        <f t="shared" si="5"/>
+        <v>15.542712030711428</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="G17" s="4">
+        <f t="shared" si="1"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="H17" s="4">
+        <f t="shared" si="2"/>
+        <v>0.1</v>
+      </c>
+      <c r="I17" s="4">
+        <f t="shared" si="3"/>
+        <v>0.04</v>
+      </c>
+      <c r="J17" s="9">
+        <f>utilities!$E$11</f>
+        <v>1E-3</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="4"/>
+        <v>-6.5427120307114279</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <v>6</v>
+      </c>
+      <c r="C18">
+        <v>8</v>
+      </c>
+      <c r="D18">
+        <v>9</v>
+      </c>
+      <c r="E18" s="16">
+        <f t="shared" si="5"/>
+        <v>15.931279831479216</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="G18" s="4">
+        <f t="shared" si="1"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="H18" s="4">
+        <f t="shared" si="2"/>
+        <v>0.1</v>
+      </c>
+      <c r="I18" s="4">
+        <f t="shared" si="3"/>
+        <v>0.04</v>
+      </c>
+      <c r="J18" s="9">
+        <f>utilities!$E$11</f>
+        <v>1E-3</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="4"/>
+        <v>-6.9312798314792161</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <v>6</v>
+      </c>
+      <c r="C19">
+        <v>8</v>
+      </c>
+      <c r="D19">
+        <v>9</v>
+      </c>
+      <c r="E19" s="16">
+        <f t="shared" si="5"/>
+        <v>16.329561827266193</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="G19" s="4">
+        <f t="shared" si="1"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="H19" s="4">
+        <f t="shared" si="2"/>
+        <v>0.1</v>
+      </c>
+      <c r="I19" s="4">
+        <f t="shared" si="3"/>
+        <v>0.04</v>
+      </c>
+      <c r="J19" s="9">
+        <f>utilities!$E$11</f>
+        <v>1E-3</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="4"/>
+        <v>-7.3295618272661933</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <v>6</v>
+      </c>
+      <c r="C20">
+        <v>8</v>
+      </c>
+      <c r="D20">
+        <v>9</v>
+      </c>
+      <c r="E20" s="16">
+        <f t="shared" si="5"/>
+        <v>16.737800872947847</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="G20" s="4">
+        <f t="shared" si="1"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="H20" s="4">
+        <f t="shared" si="2"/>
+        <v>0.1</v>
+      </c>
+      <c r="I20" s="4">
+        <f t="shared" si="3"/>
+        <v>0.04</v>
+      </c>
+      <c r="J20" s="9">
+        <f>utilities!$E$11</f>
+        <v>1E-3</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="4"/>
+        <v>-7.7378008729478474</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>6</v>
+      </c>
+      <c r="C21">
+        <v>8</v>
+      </c>
+      <c r="D21">
+        <v>9</v>
+      </c>
+      <c r="E21" s="16">
+        <f t="shared" si="5"/>
+        <v>17.156245894771544</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="G21" s="4">
+        <f t="shared" si="1"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="H21" s="4">
+        <f t="shared" si="2"/>
+        <v>0.1</v>
+      </c>
+      <c r="I21" s="4">
+        <f t="shared" si="3"/>
+        <v>0.04</v>
+      </c>
+      <c r="J21" s="9">
+        <f>utilities!$E$11</f>
+        <v>1E-3</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="4"/>
+        <v>-8.1562458947715442</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22">
+        <v>6</v>
+      </c>
+      <c r="C22">
+        <v>8</v>
+      </c>
+      <c r="D22">
+        <v>9</v>
+      </c>
+      <c r="E22" s="16">
+        <f t="shared" si="5"/>
+        <v>17.585152042140834</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="G22" s="4">
+        <f t="shared" si="1"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="H22" s="4">
+        <f t="shared" si="2"/>
+        <v>0.1</v>
+      </c>
+      <c r="I22" s="4">
+        <f t="shared" si="3"/>
+        <v>0.04</v>
+      </c>
+      <c r="J22" s="9">
+        <f>utilities!$E$11</f>
+        <v>1E-3</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="4"/>
+        <v>-8.5851520421408338</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23">
+        <v>6</v>
+      </c>
+      <c r="C23">
+        <v>8</v>
+      </c>
+      <c r="D23">
+        <v>9</v>
+      </c>
+      <c r="E23" s="16">
+        <f t="shared" si="5"/>
+        <v>18.02478084319435</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="G23" s="4">
+        <f t="shared" si="1"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="H23" s="4">
+        <f t="shared" si="2"/>
+        <v>0.1</v>
+      </c>
+      <c r="I23" s="4">
+        <f t="shared" si="3"/>
+        <v>0.04</v>
+      </c>
+      <c r="J23" s="9">
+        <f>utilities!$E$11</f>
+        <v>1E-3</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="4"/>
+        <v>-9.0247808431943497</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24">
+        <v>6</v>
+      </c>
+      <c r="C24">
+        <v>8</v>
+      </c>
+      <c r="D24">
+        <v>9</v>
+      </c>
+      <c r="E24" s="16">
+        <f t="shared" si="5"/>
+        <v>18.475400364274208</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="G24" s="4">
+        <f t="shared" si="1"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="H24" s="4">
+        <f t="shared" si="2"/>
+        <v>0.1</v>
+      </c>
+      <c r="I24" s="4">
+        <f t="shared" si="3"/>
+        <v>0.04</v>
+      </c>
+      <c r="J24" s="9">
+        <f>utilities!$E$11</f>
+        <v>1E-3</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="4"/>
+        <v>-9.4754003642742077</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25">
+        <v>6</v>
+      </c>
+      <c r="C25">
+        <v>8</v>
+      </c>
+      <c r="D25">
+        <v>9</v>
+      </c>
+      <c r="E25" s="16">
+        <f t="shared" si="5"/>
+        <v>18.937285373381062</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="G25" s="4">
+        <f t="shared" si="1"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="H25" s="4">
+        <f t="shared" si="2"/>
+        <v>0.1</v>
+      </c>
+      <c r="I25" s="4">
+        <f t="shared" si="3"/>
+        <v>0.04</v>
+      </c>
+      <c r="J25" s="9">
+        <f>utilities!$E$11</f>
+        <v>1E-3</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="4"/>
+        <v>-9.9372853733810622</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26">
+        <v>6</v>
+      </c>
+      <c r="C26">
+        <v>8</v>
+      </c>
+      <c r="D26">
+        <v>9</v>
+      </c>
+      <c r="E26" s="16">
+        <f t="shared" si="5"/>
+        <v>19.410717507715589</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="G26" s="4">
+        <f t="shared" si="1"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="H26" s="4">
+        <f t="shared" si="2"/>
+        <v>0.1</v>
+      </c>
+      <c r="I26" s="4">
+        <f t="shared" si="3"/>
+        <v>0.04</v>
+      </c>
+      <c r="J26" s="9">
+        <f>utilities!$E$11</f>
+        <v>1E-3</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="4"/>
+        <v>-10.410717507715589</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27">
+        <v>96</v>
+      </c>
+      <c r="C27">
+        <v>143</v>
+      </c>
+      <c r="D27">
+        <v>259</v>
+      </c>
+      <c r="E27" s="16">
+        <f t="shared" si="5"/>
+        <v>19.895985445408478</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+      <c r="G27" s="4">
+        <f t="shared" si="1"/>
+        <v>0.26041666666666669</v>
+      </c>
+      <c r="H27" s="4">
+        <f t="shared" si="2"/>
+        <v>0.10638297872340426</v>
+      </c>
+      <c r="I27" s="4">
+        <f t="shared" si="3"/>
+        <v>8.6206896551724137E-3</v>
+      </c>
+      <c r="J27" s="9">
+        <f>utilities!$E$11</f>
+        <v>1E-3</v>
+      </c>
+      <c r="K27">
+        <f t="shared" si="4"/>
+        <v>239.10401455459152</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28">
+        <f>SUM(B2:B27)</f>
+        <v>306</v>
+      </c>
+      <c r="C28">
+        <f t="shared" ref="C28:D28" si="6">SUM(C2:C27)</f>
+        <v>433</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="6"/>
+        <v>634</v>
+      </c>
+      <c r="E28">
+        <f>SUM(E2:E27)</f>
+        <v>379.52918032845758</v>
+      </c>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+      <c r="K28" s="15" t="e">
+        <f>IRR(K2:K27)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>26</v>
+      </c>
+      <c r="B29">
+        <f>utilities!$H$8</f>
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <f>utilities!$I$8</f>
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <f>utilities!$J$8</f>
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="G29" s="4" t="e">
+        <f>utilities!$H$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H29" s="4" t="e">
+        <f>utilities!$I$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I29" s="4" t="e">
+        <f>utilities!$J$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J29" s="9">
+        <f>utilities!$K$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>27</v>
+      </c>
+      <c r="B30">
+        <f>utilities!$H$8</f>
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <f>utilities!$I$8</f>
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <f>utilities!$J$8</f>
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="G30" s="4" t="e">
+        <f>utilities!$H$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H30" s="4" t="e">
+        <f>utilities!$I$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I30" s="4" t="e">
+        <f>utilities!$J$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J30" s="9">
+        <f>utilities!$K$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>28</v>
+      </c>
+      <c r="B31">
+        <f>utilities!$H$8</f>
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <f>utilities!$I$8</f>
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <f>utilities!$J$8</f>
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="G31" s="4" t="e">
+        <f>utilities!$H$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H31" s="4" t="e">
+        <f>utilities!$I$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I31" s="4" t="e">
+        <f>utilities!$J$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J31" s="9">
+        <f>utilities!$K$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>29</v>
+      </c>
+      <c r="B32">
+        <f>utilities!$H$8</f>
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <f>utilities!$I$8</f>
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <f>utilities!$J$8</f>
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="G32" s="4" t="e">
+        <f>utilities!$H$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H32" s="4" t="e">
+        <f>utilities!$I$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I32" s="4" t="e">
+        <f>utilities!$J$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J32" s="9">
+        <f>utilities!$K$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>30</v>
+      </c>
+      <c r="B33">
+        <f>utilities!$H$8</f>
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <f>utilities!$I$8</f>
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <f>utilities!$J$8</f>
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="G33" s="4" t="e">
+        <f>utilities!$H$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H33" s="4" t="e">
+        <f>utilities!$I$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I33" s="4" t="e">
+        <f>utilities!$J$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J33" s="9">
+        <f>utilities!$K$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>31</v>
+      </c>
+      <c r="B34">
+        <f>utilities!$H$8</f>
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <f>utilities!$I$8</f>
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <f>utilities!$J$8</f>
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="G34" s="4" t="e">
+        <f>utilities!$H$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H34" s="4" t="e">
+        <f>utilities!$I$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I34" s="4" t="e">
+        <f>utilities!$J$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J34" s="9">
+        <f>utilities!$K$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>32</v>
+      </c>
+      <c r="B35">
+        <f>utilities!$H$8</f>
+        <v>0</v>
+      </c>
+      <c r="C35">
+        <f>utilities!$I$8</f>
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <f>utilities!$J$8</f>
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="G35" s="4" t="e">
+        <f>utilities!$H$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H35" s="4" t="e">
+        <f>utilities!$I$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I35" s="4" t="e">
+        <f>utilities!$J$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J35" s="9">
+        <f>utilities!$K$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>33</v>
+      </c>
+      <c r="B36">
+        <f>utilities!$H$8</f>
+        <v>0</v>
+      </c>
+      <c r="C36">
+        <f>utilities!$I$8</f>
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <f>utilities!$J$8</f>
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="G36" s="4" t="e">
+        <f>utilities!$H$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H36" s="4" t="e">
+        <f>utilities!$I$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I36" s="4" t="e">
+        <f>utilities!$J$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J36" s="9">
+        <f>utilities!$K$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>34</v>
+      </c>
+      <c r="B37">
+        <f>utilities!$H$8</f>
+        <v>0</v>
+      </c>
+      <c r="C37">
+        <f>utilities!$I$8</f>
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <f>utilities!$J$8</f>
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="G37" s="4" t="e">
+        <f>utilities!$H$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H37" s="4" t="e">
+        <f>utilities!$I$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I37" s="4" t="e">
+        <f>utilities!$J$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J37" s="9">
+        <f>utilities!$K$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>35</v>
+      </c>
+      <c r="B38">
+        <f>utilities!$H$8</f>
+        <v>0</v>
+      </c>
+      <c r="C38">
+        <f>utilities!$I$8</f>
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <f>utilities!$J$8</f>
+        <v>0</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="G38" s="4" t="e">
+        <f>utilities!$H$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H38" s="4" t="e">
+        <f>utilities!$I$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I38" s="4" t="e">
+        <f>utilities!$J$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J38" s="9">
+        <f>utilities!$K$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>36</v>
+      </c>
+      <c r="B39">
+        <f>utilities!$H$8</f>
+        <v>0</v>
+      </c>
+      <c r="C39">
+        <f>utilities!$I$8</f>
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <f>utilities!$J$8</f>
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="G39" s="4" t="e">
+        <f>utilities!$H$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H39" s="4" t="e">
+        <f>utilities!$I$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I39" s="4" t="e">
+        <f>utilities!$J$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J39" s="9">
+        <f>utilities!$K$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>37</v>
+      </c>
+      <c r="B40">
+        <f>utilities!$H$8</f>
+        <v>0</v>
+      </c>
+      <c r="C40">
+        <f>utilities!$I$8</f>
+        <v>0</v>
+      </c>
+      <c r="D40">
+        <f>utilities!$J$8</f>
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="G40" s="4" t="e">
+        <f>utilities!$H$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H40" s="4" t="e">
+        <f>utilities!$I$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I40" s="4" t="e">
+        <f>utilities!$J$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J40" s="9">
+        <f>utilities!$K$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>38</v>
+      </c>
+      <c r="B41">
+        <f>utilities!$H$8</f>
+        <v>0</v>
+      </c>
+      <c r="C41">
+        <f>utilities!$I$8</f>
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <f>utilities!$J$8</f>
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="G41" s="4" t="e">
+        <f>utilities!$H$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H41" s="4" t="e">
+        <f>utilities!$I$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I41" s="4" t="e">
+        <f>utilities!$J$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J41" s="9">
+        <f>utilities!$K$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>39</v>
+      </c>
+      <c r="B42">
+        <f>utilities!$H$8</f>
+        <v>0</v>
+      </c>
+      <c r="C42">
+        <f>utilities!$I$8</f>
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <f>utilities!$J$8</f>
+        <v>0</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="F42">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="G42" s="4" t="e">
+        <f>utilities!$H$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H42" s="4" t="e">
+        <f>utilities!$I$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I42" s="4" t="e">
+        <f>utilities!$J$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J42" s="9">
+        <f>utilities!$K$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>40</v>
+      </c>
+      <c r="B43">
+        <f>utilities!$H$8</f>
+        <v>0</v>
+      </c>
+      <c r="C43">
+        <f>utilities!$I$8</f>
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <f>utilities!$J$8</f>
+        <v>0</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+      <c r="F43">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="G43" s="4" t="e">
+        <f>utilities!$H$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H43" s="4" t="e">
+        <f>utilities!$I$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I43" s="4" t="e">
+        <f>utilities!$J$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J43" s="9">
+        <f>utilities!$K$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F977CF0C-F948-4BB4-989B-6B75181A9A01}">
   <dimension ref="A1:L43"/>
   <sheetViews>
@@ -5607,12 +7054,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{117A8B26-635D-4B40-A90B-7735D1F1002F}">
   <dimension ref="A1:W33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5640,6 +7087,9 @@
       <c r="C2" t="s">
         <v>13</v>
       </c>
+      <c r="N2">
+        <v>150</v>
+      </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3">
@@ -5653,6 +7103,10 @@
       </c>
       <c r="D3">
         <v>1E-3</v>
+      </c>
+      <c r="N3">
+        <f>N2*0.8</f>
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.3">
@@ -5660,6 +7114,10 @@
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
       <c r="D4" s="5"/>
+      <c r="N4">
+        <f>N2*0.5</f>
+        <v>75</v>
+      </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">

</xml_diff>

<commit_message>
generate bond returns based on scenarios yelds
</commit_message>
<xml_diff>
--- a/julia_msp/goal_data.xlsx
+++ b/julia_msp/goal_data.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matsz\programowanie\Optymalizacja_portfela\julia_msp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D461FBA-EBA0-4AB1-A1E5-95AD43F59EAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A3E4D3D-F9DF-4D20-94E8-C7E7CFF8460A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E8CF1CA2-D953-46E5-99F4-DA96611E7E6D}"/>
   </bookViews>
   <sheets>
-    <sheet name="goal_data_single_goal" sheetId="7" r:id="rId1"/>
-    <sheet name="goal_data" sheetId="4" r:id="rId2"/>
-    <sheet name="goal_data_save" sheetId="6" r:id="rId3"/>
-    <sheet name="goal_data_5" sheetId="5" r:id="rId4"/>
-    <sheet name="utilities" sheetId="2" r:id="rId5"/>
+    <sheet name="goal_data_single_g_3y" sheetId="8" r:id="rId1"/>
+    <sheet name="goal_data_single_goal" sheetId="7" r:id="rId2"/>
+    <sheet name="goal_data" sheetId="4" r:id="rId3"/>
+    <sheet name="goal_data_save" sheetId="6" r:id="rId4"/>
+    <sheet name="goal_data_5" sheetId="5" r:id="rId5"/>
+    <sheet name="utilities" sheetId="2" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="32">
   <si>
     <t>minimum_limit</t>
   </si>
@@ -584,11 +585,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48F546F3-B2EF-4B4F-8BCE-C8A1CCE3A596}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F3B9D2B-0182-4CF6-B908-72130F84FCD0}">
   <dimension ref="A1:L42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -637,6 +638,1170 @@
         <v>1</v>
       </c>
       <c r="B2">
+        <f>6+9</f>
+        <v>15</v>
+      </c>
+      <c r="C2">
+        <f>8+12</f>
+        <v>20</v>
+      </c>
+      <c r="D2">
+        <f>9+14</f>
+        <v>23</v>
+      </c>
+      <c r="E2">
+        <v>16</v>
+      </c>
+      <c r="F2" s="16">
+        <f>1/5</f>
+        <v>0.2</v>
+      </c>
+      <c r="G2" s="4">
+        <f>(25*F2)/B2</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H2" s="4">
+        <f>(5*F2)/(C2-B2)</f>
+        <v>0.2</v>
+      </c>
+      <c r="I2" s="4">
+        <f>(1*F2)/(D2-C2)</f>
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="J2" s="9">
+        <f>utilities!$E$11*3</f>
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="K2">
+        <f>-(D2-E2+35)</f>
+        <v>-42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>18</v>
+      </c>
+      <c r="C3">
+        <v>24</v>
+      </c>
+      <c r="D3">
+        <v>27</v>
+      </c>
+      <c r="E3" s="16">
+        <v>34</v>
+      </c>
+      <c r="F3" s="16">
+        <f t="shared" ref="F3:F7" si="0">1/5</f>
+        <v>0.2</v>
+      </c>
+      <c r="G3" s="4">
+        <f t="shared" ref="G3:G17" si="1">(25*F3)/B3</f>
+        <v>0.27777777777777779</v>
+      </c>
+      <c r="H3" s="4">
+        <f t="shared" ref="H3:H17" si="2">(5*F3)/(C3-B3)</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="I3" s="4">
+        <f t="shared" ref="I3:I17" si="3">(1*F3)/(D3-C3)</f>
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="J3" s="9">
+        <f>utilities!$E$11*3</f>
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K16" si="4">D3-E3</f>
+        <v>-7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>18</v>
+      </c>
+      <c r="C4">
+        <v>24</v>
+      </c>
+      <c r="D4">
+        <v>27</v>
+      </c>
+      <c r="E4" s="16">
+        <v>33</v>
+      </c>
+      <c r="F4" s="16">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="G4" s="4">
+        <f t="shared" si="1"/>
+        <v>0.27777777777777779</v>
+      </c>
+      <c r="H4" s="4">
+        <f t="shared" si="2"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="I4" s="4">
+        <f t="shared" si="3"/>
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="J4" s="9">
+        <f>utilities!$E$11*3</f>
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="4"/>
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>18</v>
+      </c>
+      <c r="C5">
+        <v>24</v>
+      </c>
+      <c r="D5">
+        <v>27</v>
+      </c>
+      <c r="E5" s="16">
+        <v>33</v>
+      </c>
+      <c r="F5" s="16">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="G5" s="4">
+        <f t="shared" si="1"/>
+        <v>0.27777777777777779</v>
+      </c>
+      <c r="H5" s="4">
+        <f t="shared" si="2"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="I5" s="4">
+        <f t="shared" si="3"/>
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="J5" s="9">
+        <f>utilities!$E$11*3</f>
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="4"/>
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>18</v>
+      </c>
+      <c r="C6">
+        <v>24</v>
+      </c>
+      <c r="D6">
+        <v>27</v>
+      </c>
+      <c r="E6" s="16">
+        <v>33</v>
+      </c>
+      <c r="F6" s="16">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="G6" s="4">
+        <f t="shared" si="1"/>
+        <v>0.27777777777777779</v>
+      </c>
+      <c r="H6" s="4">
+        <f t="shared" si="2"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="I6" s="4">
+        <f t="shared" si="3"/>
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="J6" s="9">
+        <f>utilities!$E$11*3</f>
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="K6" s="16">
+        <f>D6-E6</f>
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>84</v>
+      </c>
+      <c r="C7">
+        <f>120+12</f>
+        <v>132</v>
+      </c>
+      <c r="D7">
+        <f>150+13</f>
+        <v>163</v>
+      </c>
+      <c r="E7" s="16">
+        <v>16</v>
+      </c>
+      <c r="F7" s="16">
+        <v>1</v>
+      </c>
+      <c r="G7" s="4">
+        <f t="shared" si="1"/>
+        <v>0.29761904761904762</v>
+      </c>
+      <c r="H7" s="4">
+        <f t="shared" si="2"/>
+        <v>0.10416666666666667</v>
+      </c>
+      <c r="I7" s="4">
+        <f t="shared" si="3"/>
+        <v>3.2258064516129031E-2</v>
+      </c>
+      <c r="J7" s="9">
+        <f>utilities!$E$11*3</f>
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="4"/>
+        <v>147</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16">
+        <v>1</v>
+      </c>
+      <c r="G17" s="4" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H17" s="4" t="e">
+        <f>(5*F17)/(C17-B17)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I17" s="4" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J17" s="9">
+        <f>utilities!$E$11</f>
+        <v>1E-3</v>
+      </c>
+      <c r="K17" s="16">
+        <f>D17-E17</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B18" s="16">
+        <f t="shared" ref="B18:D18" si="5">SUM(B2:B17)</f>
+        <v>171</v>
+      </c>
+      <c r="C18" s="16">
+        <f t="shared" si="5"/>
+        <v>248</v>
+      </c>
+      <c r="D18" s="16">
+        <f t="shared" si="5"/>
+        <v>294</v>
+      </c>
+      <c r="E18" s="16">
+        <f>SUM(E2:E17)</f>
+        <v>165</v>
+      </c>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="K18">
+        <f>SUM(K2:K17)</f>
+        <v>80</v>
+      </c>
+      <c r="L18" s="15">
+        <f>IRR(K2:K7)</f>
+        <v>0.20331670399466484</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="E19" s="16"/>
+      <c r="G19" s="4">
+        <f>SUMPRODUCT(B2:B7,G2:G7)</f>
+        <v>50</v>
+      </c>
+      <c r="H19" s="4">
+        <v>10</v>
+      </c>
+      <c r="I19" s="4">
+        <v>1</v>
+      </c>
+      <c r="J19" s="9">
+        <f>SUM(J2:J17)</f>
+        <v>1.9E-2</v>
+      </c>
+      <c r="K19" s="4">
+        <f>SUM(G19:J19)</f>
+        <v>61.018999999999998</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="E20" s="16">
+        <v>8</v>
+      </c>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="E21" s="16">
+        <f>E20*0.8</f>
+        <v>6.4</v>
+      </c>
+      <c r="G21" s="4" t="e">
+        <f>G17*B17</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="E22" s="16">
+        <f>E20*0.6</f>
+        <v>4.8</v>
+      </c>
+      <c r="G22" s="4">
+        <f>G16*B16</f>
+        <v>0</v>
+      </c>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="9">
+        <f>1*I16</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="E23" s="16"/>
+      <c r="G23" s="4">
+        <f>G22*15</f>
+        <v>0</v>
+      </c>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="E24" s="16"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="E25" s="16"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="E26" s="16"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27">
+        <f>SUM(B2:B26)</f>
+        <v>342</v>
+      </c>
+      <c r="C27">
+        <f>SUM(C2:C26)</f>
+        <v>496</v>
+      </c>
+      <c r="D27">
+        <f>SUM(D2:D26)</f>
+        <v>588</v>
+      </c>
+      <c r="E27">
+        <f>SUM(E2:E26)</f>
+        <v>349.2</v>
+      </c>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+      <c r="K27" s="15">
+        <f>IRR(K2:K17)</f>
+        <v>0.20331670399466484</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="B28">
+        <f>utilities!$H$8</f>
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <f>utilities!$I$8</f>
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <f>utilities!$J$8</f>
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <f t="shared" ref="F28:F42" si="6">1/25</f>
+        <v>0.04</v>
+      </c>
+      <c r="G28" s="4" t="e">
+        <f>utilities!$H$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H28" s="4" t="e">
+        <f>utilities!$I$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I28" s="4" t="e">
+        <f>utilities!$J$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J28" s="9">
+        <f>utilities!$K$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="B29">
+        <f>utilities!$H$8</f>
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <f>utilities!$I$8</f>
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <f>utilities!$J$8</f>
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="6"/>
+        <v>0.04</v>
+      </c>
+      <c r="G29" s="4" t="e">
+        <f>utilities!$H$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H29" s="4" t="e">
+        <f>utilities!$I$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I29" s="4" t="e">
+        <f>utilities!$J$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J29" s="9">
+        <f>utilities!$K$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>28</v>
+      </c>
+      <c r="B30">
+        <f>utilities!$H$8</f>
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <f>utilities!$I$8</f>
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <f>utilities!$J$8</f>
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="6"/>
+        <v>0.04</v>
+      </c>
+      <c r="G30" s="4" t="e">
+        <f>utilities!$H$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H30" s="4" t="e">
+        <f>utilities!$I$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I30" s="4" t="e">
+        <f>utilities!$J$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J30" s="9">
+        <f>utilities!$K$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="B31">
+        <f>utilities!$H$8</f>
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <f>utilities!$I$8</f>
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <f>utilities!$J$8</f>
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="6"/>
+        <v>0.04</v>
+      </c>
+      <c r="G31" s="4" t="e">
+        <f>utilities!$H$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H31" s="4" t="e">
+        <f>utilities!$I$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I31" s="4" t="e">
+        <f>utilities!$J$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J31" s="9">
+        <f>utilities!$K$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>30</v>
+      </c>
+      <c r="B32">
+        <f>utilities!$H$8</f>
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <f>utilities!$I$8</f>
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <f>utilities!$J$8</f>
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="6"/>
+        <v>0.04</v>
+      </c>
+      <c r="G32" s="4" t="e">
+        <f>utilities!$H$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H32" s="4" t="e">
+        <f>utilities!$I$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I32" s="4" t="e">
+        <f>utilities!$J$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J32" s="9">
+        <f>utilities!$K$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>31</v>
+      </c>
+      <c r="B33">
+        <f>utilities!$H$8</f>
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <f>utilities!$I$8</f>
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <f>utilities!$J$8</f>
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="6"/>
+        <v>0.04</v>
+      </c>
+      <c r="G33" s="4" t="e">
+        <f>utilities!$H$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H33" s="4" t="e">
+        <f>utilities!$I$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I33" s="4" t="e">
+        <f>utilities!$J$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J33" s="9">
+        <f>utilities!$K$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>32</v>
+      </c>
+      <c r="B34">
+        <f>utilities!$H$8</f>
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <f>utilities!$I$8</f>
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <f>utilities!$J$8</f>
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="6"/>
+        <v>0.04</v>
+      </c>
+      <c r="G34" s="4" t="e">
+        <f>utilities!$H$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H34" s="4" t="e">
+        <f>utilities!$I$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I34" s="4" t="e">
+        <f>utilities!$J$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J34" s="9">
+        <f>utilities!$K$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>33</v>
+      </c>
+      <c r="B35">
+        <f>utilities!$H$8</f>
+        <v>0</v>
+      </c>
+      <c r="C35">
+        <f>utilities!$I$8</f>
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <f>utilities!$J$8</f>
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="6"/>
+        <v>0.04</v>
+      </c>
+      <c r="G35" s="4" t="e">
+        <f>utilities!$H$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H35" s="4" t="e">
+        <f>utilities!$I$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I35" s="4" t="e">
+        <f>utilities!$J$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J35" s="9">
+        <f>utilities!$K$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>34</v>
+      </c>
+      <c r="B36">
+        <f>utilities!$H$8</f>
+        <v>0</v>
+      </c>
+      <c r="C36">
+        <f>utilities!$I$8</f>
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <f>utilities!$J$8</f>
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="6"/>
+        <v>0.04</v>
+      </c>
+      <c r="G36" s="4" t="e">
+        <f>utilities!$H$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H36" s="4" t="e">
+        <f>utilities!$I$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I36" s="4" t="e">
+        <f>utilities!$J$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J36" s="9">
+        <f>utilities!$K$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>35</v>
+      </c>
+      <c r="B37">
+        <f>utilities!$H$8</f>
+        <v>0</v>
+      </c>
+      <c r="C37">
+        <f>utilities!$I$8</f>
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <f>utilities!$J$8</f>
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="6"/>
+        <v>0.04</v>
+      </c>
+      <c r="G37" s="4" t="e">
+        <f>utilities!$H$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H37" s="4" t="e">
+        <f>utilities!$I$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I37" s="4" t="e">
+        <f>utilities!$J$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J37" s="9">
+        <f>utilities!$K$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>36</v>
+      </c>
+      <c r="B38">
+        <f>utilities!$H$8</f>
+        <v>0</v>
+      </c>
+      <c r="C38">
+        <f>utilities!$I$8</f>
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <f>utilities!$J$8</f>
+        <v>0</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="6"/>
+        <v>0.04</v>
+      </c>
+      <c r="G38" s="4" t="e">
+        <f>utilities!$H$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H38" s="4" t="e">
+        <f>utilities!$I$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I38" s="4" t="e">
+        <f>utilities!$J$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J38" s="9">
+        <f>utilities!$K$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>37</v>
+      </c>
+      <c r="B39">
+        <f>utilities!$H$8</f>
+        <v>0</v>
+      </c>
+      <c r="C39">
+        <f>utilities!$I$8</f>
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <f>utilities!$J$8</f>
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="6"/>
+        <v>0.04</v>
+      </c>
+      <c r="G39" s="4" t="e">
+        <f>utilities!$H$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H39" s="4" t="e">
+        <f>utilities!$I$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I39" s="4" t="e">
+        <f>utilities!$J$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J39" s="9">
+        <f>utilities!$K$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>38</v>
+      </c>
+      <c r="B40">
+        <f>utilities!$H$8</f>
+        <v>0</v>
+      </c>
+      <c r="C40">
+        <f>utilities!$I$8</f>
+        <v>0</v>
+      </c>
+      <c r="D40">
+        <f>utilities!$J$8</f>
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40">
+        <f t="shared" si="6"/>
+        <v>0.04</v>
+      </c>
+      <c r="G40" s="4" t="e">
+        <f>utilities!$H$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H40" s="4" t="e">
+        <f>utilities!$I$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I40" s="4" t="e">
+        <f>utilities!$J$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J40" s="9">
+        <f>utilities!$K$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>39</v>
+      </c>
+      <c r="B41">
+        <f>utilities!$H$8</f>
+        <v>0</v>
+      </c>
+      <c r="C41">
+        <f>utilities!$I$8</f>
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <f>utilities!$J$8</f>
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41">
+        <f t="shared" si="6"/>
+        <v>0.04</v>
+      </c>
+      <c r="G41" s="4" t="e">
+        <f>utilities!$H$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H41" s="4" t="e">
+        <f>utilities!$I$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I41" s="4" t="e">
+        <f>utilities!$J$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J41" s="9">
+        <f>utilities!$K$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>40</v>
+      </c>
+      <c r="B42">
+        <f>utilities!$H$8</f>
+        <v>0</v>
+      </c>
+      <c r="C42">
+        <f>utilities!$I$8</f>
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <f>utilities!$J$8</f>
+        <v>0</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="F42">
+        <f t="shared" si="6"/>
+        <v>0.04</v>
+      </c>
+      <c r="G42" s="4" t="e">
+        <f>utilities!$H$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H42" s="4" t="e">
+        <f>utilities!$I$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I42" s="4" t="e">
+        <f>utilities!$J$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J42" s="9">
+        <f>utilities!$K$11</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48F546F3-B2EF-4B4F-8BCE-C8A1CCE3A596}">
+  <dimension ref="A1:L42"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="7" max="7" width="16.6640625" customWidth="1"/>
+    <col min="10" max="10" width="8.88671875" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
         <v>6</v>
       </c>
       <c r="C2">
@@ -1303,7 +2468,22 @@
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="E18" s="16"/>
+      <c r="B18" s="16">
+        <f t="shared" ref="B18:D18" si="5">SUM(B2:B17)</f>
+        <v>171</v>
+      </c>
+      <c r="C18" s="16">
+        <f t="shared" si="5"/>
+        <v>248</v>
+      </c>
+      <c r="D18" s="16">
+        <f t="shared" si="5"/>
+        <v>294</v>
+      </c>
+      <c r="E18" s="16">
+        <f>SUM(E2:E17)</f>
+        <v>165</v>
+      </c>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
@@ -1368,6 +2548,10 @@
       </c>
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
+      <c r="J22" s="9">
+        <f>1*I16</f>
+        <v>6.6666666666666666E-2</v>
+      </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E23" s="16"/>
@@ -1402,19 +2586,19 @@
       </c>
       <c r="B27">
         <f>SUM(B2:B26)</f>
-        <v>171</v>
+        <v>342</v>
       </c>
       <c r="C27">
         <f>SUM(C2:C26)</f>
-        <v>248</v>
+        <v>496</v>
       </c>
       <c r="D27">
         <f>SUM(D2:D26)</f>
-        <v>294</v>
+        <v>588</v>
       </c>
       <c r="E27">
         <f>SUM(E2:E26)</f>
-        <v>184.20000000000002</v>
+        <v>349.2</v>
       </c>
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
@@ -1444,7 +2628,7 @@
         <v>0</v>
       </c>
       <c r="F28">
-        <f t="shared" ref="F28:F42" si="5">1/25</f>
+        <f t="shared" ref="F28:F42" si="6">1/25</f>
         <v>0.04</v>
       </c>
       <c r="G28" s="4" t="e">
@@ -1484,7 +2668,7 @@
         <v>0</v>
       </c>
       <c r="F29">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.04</v>
       </c>
       <c r="G29" s="4" t="e">
@@ -1524,7 +2708,7 @@
         <v>0</v>
       </c>
       <c r="F30">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.04</v>
       </c>
       <c r="G30" s="4" t="e">
@@ -1564,7 +2748,7 @@
         <v>0</v>
       </c>
       <c r="F31">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.04</v>
       </c>
       <c r="G31" s="4" t="e">
@@ -1604,7 +2788,7 @@
         <v>0</v>
       </c>
       <c r="F32">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.04</v>
       </c>
       <c r="G32" s="4" t="e">
@@ -1644,7 +2828,7 @@
         <v>0</v>
       </c>
       <c r="F33">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.04</v>
       </c>
       <c r="G33" s="4" t="e">
@@ -1684,7 +2868,7 @@
         <v>0</v>
       </c>
       <c r="F34">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.04</v>
       </c>
       <c r="G34" s="4" t="e">
@@ -1724,7 +2908,7 @@
         <v>0</v>
       </c>
       <c r="F35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.04</v>
       </c>
       <c r="G35" s="4" t="e">
@@ -1764,7 +2948,7 @@
         <v>0</v>
       </c>
       <c r="F36">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.04</v>
       </c>
       <c r="G36" s="4" t="e">
@@ -1804,7 +2988,7 @@
         <v>0</v>
       </c>
       <c r="F37">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.04</v>
       </c>
       <c r="G37" s="4" t="e">
@@ -1844,7 +3028,7 @@
         <v>0</v>
       </c>
       <c r="F38">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.04</v>
       </c>
       <c r="G38" s="4" t="e">
@@ -1884,7 +3068,7 @@
         <v>0</v>
       </c>
       <c r="F39">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.04</v>
       </c>
       <c r="G39" s="4" t="e">
@@ -1924,7 +3108,7 @@
         <v>0</v>
       </c>
       <c r="F40">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.04</v>
       </c>
       <c r="G40" s="4" t="e">
@@ -1964,7 +3148,7 @@
         <v>0</v>
       </c>
       <c r="F41">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.04</v>
       </c>
       <c r="G41" s="4" t="e">
@@ -2004,7 +3188,7 @@
         <v>0</v>
       </c>
       <c r="F42">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.04</v>
       </c>
       <c r="G42" s="4" t="e">
@@ -2029,7 +3213,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67C203FD-C9AE-45F0-8773-EECC728085CE}">
   <dimension ref="A1:K43"/>
   <sheetViews>
@@ -3800,7 +4984,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C37F228-CE9B-4855-94EE-55EF65F52467}">
   <dimension ref="A1:K43"/>
   <sheetViews>
@@ -5571,7 +6755,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F977CF0C-F948-4BB4-989B-6B75181A9A01}">
   <dimension ref="A1:L43"/>
   <sheetViews>
@@ -7054,7 +8238,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{117A8B26-635D-4B40-A90B-7735D1F1002F}">
   <dimension ref="A1:W33"/>
   <sheetViews>

</xml_diff>